<commit_message>
Added daily tracker tab + update trades
New Tracker tab and minor additions to Trade tab. Updated trades for 9/21/2022
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE018856-5F3F-4EEF-B7A3-10E520314E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726259B0-8AE0-4213-B49E-DE15B6C65508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30360" yWindow="3615" windowWidth="20280" windowHeight="15420" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <t>SPX Open</t>
   </si>
@@ -163,12 +163,6 @@
     <t>Spread</t>
   </si>
   <si>
-    <t>STO BullPut</t>
-  </si>
-  <si>
-    <t>STO BearCall</t>
-  </si>
-  <si>
     <t>Time (EST)</t>
   </si>
   <si>
@@ -178,12 +172,6 @@
     <t>Qty</t>
   </si>
   <si>
-    <t>Sep20 3830/3805 @ -4.30</t>
-  </si>
-  <si>
-    <t>Sep20 3895/3925 @ -3.00</t>
-  </si>
-  <si>
     <t>P/L ea.</t>
   </si>
   <si>
@@ -208,7 +196,40 @@
     <t>Linked Data</t>
   </si>
   <si>
-    <t>4:03pm</t>
+    <t>Max. P/L</t>
+  </si>
+  <si>
+    <t>STO</t>
+  </si>
+  <si>
+    <t>Sep20 3830/3805 @ -4.30 BullPut</t>
+  </si>
+  <si>
+    <t>Sep20 3895/3925 @ -3.00 BearCall</t>
+  </si>
+  <si>
+    <t>Capture %</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>High volitility expected, betting that market goes up overall</t>
+  </si>
+  <si>
+    <t>Sep21 3815/3790 @ -5.20 BullPut</t>
+  </si>
+  <si>
+    <t>Stop Loss Value</t>
+  </si>
+  <si>
+    <t>Profit Taker %</t>
+  </si>
+  <si>
+    <t>Stop Loss %</t>
+  </si>
+  <si>
+    <t>Profit Taker Value</t>
   </si>
 </sst>
 </file>
@@ -378,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -479,35 +500,60 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,7 +871,7 @@
   <dimension ref="B1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,16 +887,14 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>50</v>
-      </c>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="20">
-        <v>44824</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>57</v>
+        <v>44825</v>
+      </c>
+      <c r="C2" s="55">
+        <v>0.40972222222222227</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -879,14 +923,14 @@
         <v>3</v>
       </c>
       <c r="C5" s="12">
-        <v>3849.91</v>
+        <v>3876.23</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="27">
         <f>(C9-C18)/(C17-C18)</f>
-        <v>0.30966785750188597</v>
+        <v>0.67418322291861388</v>
       </c>
       <c r="G5" s="25">
         <v>0.4</v>
@@ -898,14 +942,14 @@
         <v>4</v>
       </c>
       <c r="C6" s="13">
-        <v>3899.89</v>
+        <v>3855.93</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="27">
         <f>(C9-C23)/(C22-C23)</f>
-        <v>0.44075371198480678</v>
+        <v>0.49471068299340765</v>
       </c>
       <c r="G6" s="25">
         <v>0.33</v>
@@ -917,14 +961,14 @@
         <v>13</v>
       </c>
       <c r="C7" s="13">
-        <v>3886.61</v>
+        <v>3877.91</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="28">
         <f>(C9-C28)/(C27-C28)</f>
-        <v>0.37811331435020734</v>
+        <v>0.43338859247351447</v>
       </c>
       <c r="G7" s="26">
         <v>0.27</v>
@@ -936,14 +980,14 @@
         <v>11</v>
       </c>
       <c r="C8" s="13">
-        <v>3910.65</v>
+        <v>3895.3</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="29">
         <f>F5*G5+F6*G6+F7*G7</f>
-        <v>0.37140646283029666</v>
+        <v>0.54994273452311893</v>
       </c>
       <c r="G8" s="24" t="s">
         <v>34</v>
@@ -955,7 +999,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="12">
-        <v>3876.23</v>
+        <v>3877</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -964,9 +1008,7 @@
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13">
-        <v>3856.04</v>
-      </c>
+      <c r="C10" s="13"/>
       <c r="E10" s="10" t="s">
         <v>33</v>
       </c>
@@ -982,9 +1024,7 @@
       <c r="B11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="13">
-        <v>3877.96</v>
-      </c>
+      <c r="C11" s="13"/>
       <c r="E11" s="15" t="s">
         <v>10</v>
       </c>
@@ -999,9 +1039,7 @@
       <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="13">
-        <v>3895.32</v>
-      </c>
+      <c r="C12" s="13"/>
       <c r="E12" s="16" t="s">
         <v>25</v>
       </c>
@@ -1017,7 +1055,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="14">
-        <v>0.253</v>
+        <v>0.249</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>26</v>
@@ -1061,7 +1099,7 @@
       </c>
       <c r="C16" s="4">
         <f>C6*C$13*252^-0.5</f>
-        <v>62.154504461153429</v>
+        <v>60.482288842034471</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>37</v>
@@ -1079,7 +1117,7 @@
       </c>
       <c r="C17" s="4">
         <f>C6+C16</f>
-        <v>3962.0445044611533</v>
+        <v>3916.4122888420343</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>27</v>
@@ -1097,7 +1135,7 @@
       </c>
       <c r="C18" s="6">
         <f>C6-C16</f>
-        <v>3837.7354955388464</v>
+        <v>3795.4477111579654</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>28</v>
@@ -1132,7 +1170,7 @@
       </c>
       <c r="C21" s="4">
         <f>C7*C$13*(2/252)^0.5</f>
-        <v>87.600424834533229</v>
+        <v>86.022448537842592</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -1141,7 +1179,7 @@
       </c>
       <c r="C22" s="4">
         <f>C7+C21</f>
-        <v>3974.2104248345336</v>
+        <v>3963.9324485378424</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1150,7 +1188,7 @@
       </c>
       <c r="C23" s="6">
         <f>C7-C21</f>
-        <v>3799.0095751654667</v>
+        <v>3791.8875514621573</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1166,7 +1204,7 @@
       </c>
       <c r="C26" s="4">
         <f>C17*C$13*(5/252)^0.5</f>
-        <v>141.1967181505629</v>
+        <v>137.36385913121455</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1175,7 +1213,7 @@
       </c>
       <c r="C27" s="4">
         <f>C8+C26</f>
-        <v>4051.846718150563</v>
+        <v>4032.6638591312148</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1184,7 +1222,7 @@
       </c>
       <c r="C28" s="6">
         <f>C8-C26</f>
-        <v>3769.4532818494372</v>
+        <v>3757.9361408687855</v>
       </c>
     </row>
   </sheetData>
@@ -1195,148 +1233,158 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C82D01-CC02-4066-B9D6-9DFF5A0A89C9}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="43" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.140625" style="50"/>
-    <col min="6" max="6" width="9.140625" style="49"/>
-    <col min="7" max="7" width="10.42578125" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="17"/>
+    <col min="2" max="5" width="9.140625" style="46"/>
+    <col min="6" max="6" width="9.140625" style="45"/>
+    <col min="7" max="7" width="10.42578125" style="45" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="17"/>
+    <col min="10" max="10" width="10" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="46"/>
-    </row>
-    <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="44"/>
+    </row>
+    <row r="2" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43">
         <f>Indicator!B2</f>
+        <v>44825</v>
+      </c>
+      <c r="B2" s="47">
+        <f>Indicator!$C$9</f>
+        <v>3877</v>
+      </c>
+      <c r="C2" s="47">
+        <f>Indicator!$C$10</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="47">
+        <f>Indicator!$C$11</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="47">
+        <f>Indicator!$C$12</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="48">
+        <f>Indicator!$C$13</f>
+        <v>0.249</v>
+      </c>
+      <c r="G2" s="48">
+        <f>Indicator!$F$8</f>
+        <v>0.54994273452311893</v>
+      </c>
+      <c r="H2" s="49">
+        <f>SUMIF(Trades!A:A,Tracker!A2,Trades!H:H)</f>
+        <v>5.17</v>
+      </c>
+      <c r="I2" s="50">
+        <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A2,  Trades!C:C, "STO")</f>
+        <v>5.17</v>
+      </c>
+      <c r="J2" s="21">
+        <f>H2/I2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="43"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="44"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="43">
         <v>44824</v>
       </c>
-      <c r="B2" s="50">
-        <f>Indicator!$C$9</f>
+      <c r="B5" s="46">
         <v>3876.23</v>
       </c>
-      <c r="C2" s="50">
-        <f>Indicator!$C$10</f>
+      <c r="C5" s="46">
         <v>3856.04</v>
       </c>
-      <c r="D2" s="50">
-        <f>Indicator!$C$11</f>
+      <c r="D5" s="46">
         <v>3877.96</v>
       </c>
-      <c r="E2" s="50">
-        <f>Indicator!$C$12</f>
+      <c r="E5" s="46">
         <v>3895.32</v>
       </c>
-      <c r="F2" s="49">
-        <f>Indicator!$C$13</f>
-        <v>0.253</v>
-      </c>
-      <c r="G2" s="49">
-        <f>Indicator!$F$8</f>
-        <v>0.37140646283029666</v>
-      </c>
-      <c r="H2" s="46">
-        <f>SUMIF(Trades!A:A,Tracker!A2,Trades!H:H)</f>
+      <c r="F5" s="45">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="G5" s="45">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="H5" s="17">
         <v>7.2899999999999991</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="46"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="53" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="43">
-        <v>44823</v>
-      </c>
-      <c r="B5" s="50">
-        <v>3849.91</v>
-      </c>
-      <c r="C5" s="50">
-        <v>3899.89</v>
-      </c>
-      <c r="D5" s="50">
-        <v>3886.61</v>
-      </c>
-      <c r="E5" s="50">
-        <v>3910.65</v>
-      </c>
-      <c r="F5" s="49">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="H5" s="48"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="43">
-        <v>44824</v>
-      </c>
-      <c r="B6" s="50">
-        <v>3876.23</v>
-      </c>
-      <c r="C6" s="50">
-        <v>3856.04</v>
-      </c>
-      <c r="D6" s="50">
-        <v>3877.96</v>
-      </c>
-      <c r="E6" s="50">
-        <v>3895.32</v>
-      </c>
-      <c r="F6" s="49">
-        <v>0.253</v>
-      </c>
-      <c r="G6" s="49">
-        <v>0.37140646283029666</v>
-      </c>
-      <c r="H6" s="17">
+      <c r="I5">
         <v>7.2899999999999991</v>
+      </c>
+      <c r="J5" s="21">
+        <f>H5/I5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="17" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1347,101 +1395,173 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="44" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.5703125" style="46" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="62" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="63" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="64" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="65" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="66" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="66" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="45" t="s">
+      <c r="G1" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="62">
+        <v>44824</v>
+      </c>
+      <c r="B2" s="63">
+        <v>949</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="43">
-        <v>44824</v>
-      </c>
-      <c r="B2" s="44">
-        <v>949</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2">
+      <c r="E2" s="31">
         <v>-0.15</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="31">
         <v>1</v>
       </c>
-      <c r="G2" s="46">
+      <c r="G2" s="64">
         <v>4.2699999999999996</v>
       </c>
-      <c r="H2" s="46">
+      <c r="H2" s="65">
         <f>G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="43">
+      <c r="I2" s="66">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <f>-I2*G2</f>
+        <v>-12.809999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="62">
         <v>44824</v>
       </c>
-      <c r="B3" s="44">
+      <c r="B3" s="63">
         <v>950</v>
       </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3">
+      <c r="C3" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="31">
         <v>0.09</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="31">
         <v>1</v>
       </c>
-      <c r="G3" s="46">
+      <c r="G3" s="64">
         <v>3.02</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="65">
         <f>G3*F3</f>
         <v>3.02</v>
+      </c>
+      <c r="I3" s="66">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <f>-I3*G3</f>
+        <v>-9.06</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="62">
+        <v>44825</v>
+      </c>
+      <c r="B4" s="63">
+        <v>944</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="31">
+        <v>-0.15</v>
+      </c>
+      <c r="F4" s="31">
+        <v>1</v>
+      </c>
+      <c r="G4" s="64">
+        <v>5.17</v>
+      </c>
+      <c r="H4" s="65">
+        <f>G4*F4</f>
+        <v>5.17</v>
+      </c>
+      <c r="I4" s="66">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <f>-I4*G4</f>
+        <v>-15.51</v>
+      </c>
+      <c r="K4" s="66">
+        <v>0.75</v>
+      </c>
+      <c r="L4">
+        <f>-G4+K4*G4</f>
+        <v>-1.2925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added statistical proof for 0DTE strategy
New statistical proof for 0DTE strategy
Updated for market close
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B980CFE5-9A86-46E4-93E9-A88D792B02BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE7F219-D0A4-4CE6-9C0A-8D2D48EDFF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27525" yWindow="5010" windowWidth="23580" windowHeight="14010" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
+    <workbookView xWindow="27525" yWindow="5010" windowWidth="23580" windowHeight="14010" activeTab="3" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator" sheetId="1" r:id="rId1"/>
     <sheet name="Dashboard" sheetId="4" r:id="rId2"/>
     <sheet name="Tracker" sheetId="3" r:id="rId3"/>
     <sheet name="Trades" sheetId="2" r:id="rId4"/>
+    <sheet name="Statistical Proof" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="114">
   <si>
     <t>SPX Open</t>
   </si>
@@ -312,16 +313,84 @@
   </si>
   <si>
     <t>Sep22 3745/3720 @ -5.00 Bull Put</t>
+  </si>
+  <si>
+    <t>Assuming 1std = $50 distance from SPX</t>
+  </si>
+  <si>
+    <t>Assuming max win = $500</t>
+  </si>
+  <si>
+    <t>Assuming max loss = ($250)</t>
+  </si>
+  <si>
+    <t>1-Side Max Loss</t>
+  </si>
+  <si>
+    <t>Break Even Low</t>
+  </si>
+  <si>
+    <t>Max Win Low</t>
+  </si>
+  <si>
+    <t>Max Win High</t>
+  </si>
+  <si>
+    <t>Break Even High</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>SPX Distance</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>Quick Calc Worst Case</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Max Win</t>
+  </si>
+  <si>
+    <t>Max Loss</t>
+  </si>
+  <si>
+    <t>Even - Win</t>
+  </si>
+  <si>
+    <t>Loss - Even</t>
+  </si>
+  <si>
+    <t>Expected Returns</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Profit / Loss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -483,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -597,24 +666,6 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -690,6 +741,36 @@
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="5" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,10 +856,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -799,6 +877,9 @@
                 <c:pt idx="1">
                   <c:v>44825</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>44826</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -813,6 +894,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1113</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2084</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -888,6 +972,9 @@
                       <c:pt idx="1">
                         <c:v>44825</c:v>
                       </c:pt>
+                      <c:pt idx="2">
+                        <c:v>44826</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -908,6 +995,9 @@
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>3.84</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>9.7100000000000009</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -971,6 +1061,9 @@
                       <c:pt idx="1">
                         <c:v>44825</c:v>
                       </c:pt>
+                      <c:pt idx="2">
+                        <c:v>44826</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -991,6 +1084,9 @@
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>5.17</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>9.7100000000000009</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1054,6 +1150,9 @@
                       <c:pt idx="1">
                         <c:v>44825</c:v>
                       </c:pt>
+                      <c:pt idx="2">
+                        <c:v>44826</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1074,6 +1173,9 @@
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>0.74274661508704065</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1332,7 +1434,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent4"/>
             </a:solidFill>
             <a:ln w="25400">
               <a:noFill/>
@@ -1352,6 +1454,9 @@
                 <c:pt idx="1">
                   <c:v>44825</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>44826</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1367,6 +1472,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.7100000000000009</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -1441,6 +1549,9 @@
                       <c:pt idx="1">
                         <c:v>44825</c:v>
                       </c:pt>
+                      <c:pt idx="2">
+                        <c:v>44826</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1461,6 +1572,9 @@
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>0.74274661508704065</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1521,6 +1635,9 @@
                       <c:pt idx="1">
                         <c:v>44825</c:v>
                       </c:pt>
+                      <c:pt idx="2">
+                        <c:v>44826</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1541,6 +1658,9 @@
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>1113</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2084</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1567,7 +1687,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent5"/>
             </a:solidFill>
             <a:ln w="25400">
               <a:noFill/>
@@ -1587,6 +1707,9 @@
                 <c:pt idx="1">
                   <c:v>44825</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>44826</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1602,6 +1725,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.7100000000000009</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -1943,10 +2069,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1966,6 +2089,9 @@
                 <c:pt idx="1">
                   <c:v>44825</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>44826</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1981,6 +2107,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.74274661508704065</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2041,6 +2170,9 @@
                       <c:pt idx="1">
                         <c:v>44825</c:v>
                       </c:pt>
+                      <c:pt idx="2">
+                        <c:v>44826</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2061,6 +2193,9 @@
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>5.17</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>9.7100000000000009</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2121,6 +2256,9 @@
                       <c:pt idx="1">
                         <c:v>44825</c:v>
                       </c:pt>
+                      <c:pt idx="2">
+                        <c:v>44826</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2141,6 +2279,9 @@
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>1113</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2084</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2208,6 +2349,9 @@
                       <c:pt idx="1">
                         <c:v>44825</c:v>
                       </c:pt>
+                      <c:pt idx="2">
+                        <c:v>44826</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2228,6 +2372,9 @@
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>3.84</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>9.7100000000000009</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4519,8 +4666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{044E485C-BC7E-40C9-B7A6-38794294458B}">
   <dimension ref="B1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4533,7 +4680,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="64" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="19" t="s">
@@ -4544,8 +4691,8 @@
       <c r="B2" s="20">
         <v>44826</v>
       </c>
-      <c r="C2" s="71">
-        <v>0.4284722222222222</v>
+      <c r="C2" s="65">
+        <v>0.69236111111111109</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4581,7 +4728,7 @@
       </c>
       <c r="F5" s="27">
         <f>(C9-C18)/(C17-C18)</f>
-        <v>0.44283124481493741</v>
+        <v>0.43878819282165138</v>
       </c>
       <c r="G5" s="25">
         <v>0.4</v>
@@ -4600,7 +4747,7 @@
       </c>
       <c r="F6" s="27">
         <f>(C9-C23)/(C22-C23)</f>
-        <v>0.27286790363856178</v>
+        <v>0.27003371226894063</v>
       </c>
       <c r="G6" s="25">
         <v>0.33</v>
@@ -4619,7 +4766,7 @@
       </c>
       <c r="F7" s="28">
         <f>(C9-C28)/(C27-C28)</f>
-        <v>0.21097045559782512</v>
+        <v>0.20919137431995871</v>
       </c>
       <c r="G7" s="26">
         <v>0.27</v>
@@ -4638,7 +4785,7 @@
       </c>
       <c r="F8" s="29">
         <f>F5*G5+F6*G6+F7*G7</f>
-        <v>0.32414092913811315</v>
+        <v>0.32110807324379981</v>
       </c>
       <c r="G8" s="24" t="s">
         <v>28</v>
@@ -4650,7 +4797,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="12">
-        <v>3782.86</v>
+        <v>3782.36</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -4659,7 +4806,9 @@
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="13">
+        <v>3757.99</v>
+      </c>
       <c r="E10" s="10" t="s">
         <v>27</v>
       </c>
@@ -4675,7 +4824,9 @@
       <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="13"/>
+      <c r="C11" s="13">
+        <v>3773.96</v>
+      </c>
       <c r="E11" s="15" t="s">
         <v>58</v>
       </c>
@@ -4690,7 +4841,9 @@
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="13">
+        <v>3835.41</v>
+      </c>
       <c r="E12" s="16" t="s">
         <v>60</v>
       </c>
@@ -4868,7 +5021,7 @@
   <dimension ref="B1:N27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4878,8 +5031,8 @@
     <col min="3" max="3" width="11.28515625" style="17" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="17"/>
     <col min="5" max="5" width="23" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" style="74" customWidth="1"/>
-    <col min="7" max="7" width="7" style="74" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" style="68" customWidth="1"/>
+    <col min="7" max="7" width="7" style="68" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="17"/>
     <col min="10" max="10" width="26.28515625" style="17" bestFit="1" customWidth="1"/>
@@ -4888,7 +5041,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C1" s="81"/>
+      <c r="C1" s="75"/>
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
     </row>
@@ -4899,21 +5052,21 @@
       <c r="C2" s="17">
         <v>2022</v>
       </c>
-      <c r="F2" s="90" t="s">
+      <c r="F2" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="G2" s="90" t="s">
+      <c r="G2" s="84" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="77" t="s">
+      <c r="H2" s="71" t="s">
         <v>85</v>
       </c>
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
-      <c r="K2" s="76" t="s">
+      <c r="K2" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="L2" s="77" t="s">
+      <c r="L2" s="71" t="s">
         <v>6</v>
       </c>
       <c r="M2" s="22"/>
@@ -4923,66 +5076,66 @@
       <c r="B3" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="81">
+      <c r="C3" s="75">
         <v>44824</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="84">
+      <c r="F3" s="78">
         <f>COUNTA(Tracker!K:K)-1</f>
-        <v>2</v>
-      </c>
-      <c r="G3" s="86" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="78">
+      <c r="H3" s="72">
         <f>C7/F3</f>
-        <v>556.5</v>
+        <v>694.66666666666663</v>
       </c>
       <c r="J3" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="74">
+      <c r="K3" s="68">
         <f>2*1.25%</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="L3" s="78">
+      <c r="L3" s="72">
         <f>K3*C5</f>
         <v>592.0412500000001</v>
       </c>
-      <c r="M3" s="83"/>
+      <c r="M3" s="77"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="78">
+      <c r="C4" s="72">
         <v>23681.65</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="F4" s="84">
+      <c r="F4" s="78">
         <f>COUNTIF(Tracker!J:J, "&gt;0")</f>
-        <v>2</v>
-      </c>
-      <c r="G4" s="87">
+        <v>3</v>
+      </c>
+      <c r="G4" s="81">
         <f>F4/F3</f>
         <v>1</v>
       </c>
-      <c r="H4" s="78">
+      <c r="H4" s="72">
         <f>(SUMIF(Tracker!H:H, "&gt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&gt;0", Tracker!H2))/F4*100</f>
-        <v>556.5</v>
+        <v>694.66666666666663</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="K4" s="74">
+      <c r="K4" s="68">
         <f>-3.75%</f>
         <v>-3.7499999999999999E-2</v>
       </c>
-      <c r="L4" s="78">
+      <c r="L4" s="72">
         <f>K4*C5</f>
         <v>-888.06187499999999</v>
       </c>
@@ -4991,36 +5144,36 @@
       <c r="B5" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="78">
+      <c r="C5" s="72">
         <v>23681.65</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="84">
+      <c r="F5" s="78">
         <f>COUNTIF(Tracker!J:J, "&lt;0")</f>
         <v>0</v>
       </c>
-      <c r="G5" s="87">
+      <c r="G5" s="81">
         <f>F5/F3</f>
         <v>0</v>
       </c>
-      <c r="H5" s="78" t="e">
-        <f>(SUMIF(Tracker!H:H, "&lt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&lt;0", Tracker!H2))/F5*100</f>
-        <v>#DIV/0!</v>
+      <c r="H5" s="72">
+        <f>IFERROR((SUMIF(Tracker!H:H, "&lt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&lt;0", Tracker!H2))/F5*100, 0)</f>
+        <v>0</v>
       </c>
       <c r="J5" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="K5" s="74">
+      <c r="K5" s="68">
         <f>+K3+K4</f>
         <v>-1.2499999999999997E-2</v>
       </c>
-      <c r="L5" s="78">
+      <c r="L5" s="72">
         <f>+L3+L4</f>
         <v>-296.02062499999988</v>
       </c>
-      <c r="M5" s="83"/>
+      <c r="M5" s="77"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="22"/>
@@ -5030,25 +5183,25 @@
       <c r="B7" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="78">
+      <c r="C7" s="72">
         <f>INDEX(Tracker!K:K, COUNTA(Tracker!K:K)+3,1)</f>
-        <v>1113</v>
+        <v>2084</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="82">
+      <c r="F7" s="76">
         <f>C7/C4</f>
-        <v>4.699841438413286E-2</v>
-      </c>
-      <c r="G7" s="82"/>
+        <v>8.8000624956453624E-2</v>
+      </c>
+      <c r="G7" s="76"/>
       <c r="J7" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="88">
+      <c r="K7" s="82">
         <v>20</v>
       </c>
-      <c r="L7" s="88">
+      <c r="L7" s="82">
         <v>25</v>
       </c>
     </row>
@@ -5056,26 +5209,26 @@
       <c r="B8" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="78">
+      <c r="C8" s="72">
         <f>INDEX(Tracker!L:L, COUNTA(Tracker!L:L)+3,1)</f>
-        <v>1246</v>
+        <v>2217</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="82">
+      <c r="F8" s="76">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>266.15681009798004</v>
-      </c>
-      <c r="G8" s="82"/>
+        <v>28610.850928801134</v>
+      </c>
+      <c r="G8" s="76"/>
       <c r="J8" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="K8" s="88">
+      <c r="K8" s="82">
         <f>FLOOR(MROUND(C4/1000, 5)/20, 1)</f>
         <v>1</v>
       </c>
-      <c r="L8" s="85">
+      <c r="L8" s="79">
         <f>FLOOR(MROUND(C4/1000, 5)/25, 1)</f>
         <v>1</v>
       </c>
@@ -5084,45 +5237,45 @@
       <c r="B9" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="82">
+      <c r="C9" s="76">
         <f>C7/C8</f>
-        <v>0.8932584269662921</v>
+        <v>0.94000902119981955</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="82">
+      <c r="F9" s="76">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>3.8396448137552506</v>
-      </c>
-      <c r="G9" s="82"/>
+        <v>17.096752173544029</v>
+      </c>
+      <c r="G9" s="76"/>
       <c r="J9" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="K9" s="89">
+      <c r="K9" s="83">
         <f>K7*K8*100*2</f>
         <v>4000</v>
       </c>
-      <c r="L9" s="89">
+      <c r="L9" s="83">
         <f>L7*L8*100*2</f>
         <v>5000</v>
       </c>
     </row>
     <row r="24" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K24" s="75"/>
-      <c r="L24" s="75"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
     </row>
     <row r="25" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K25" s="75"/>
-      <c r="L25" s="75"/>
+      <c r="K25" s="69"/>
+      <c r="L25" s="69"/>
     </row>
     <row r="26" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K26" s="75"/>
-      <c r="L26" s="75"/>
+      <c r="K26" s="69"/>
+      <c r="L26" s="69"/>
     </row>
     <row r="27" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K27" s="75"/>
-      <c r="L27" s="75"/>
+      <c r="K27" s="69"/>
+      <c r="L27" s="69"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5136,58 +5289,58 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="58" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="9.140625" style="42"/>
     <col min="6" max="6" width="9.140625" style="41"/>
     <col min="7" max="7" width="10.42578125" style="41" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="17"/>
-    <col min="9" max="9" width="9.140625" style="67"/>
+    <col min="9" max="9" width="9.140625" style="61"/>
     <col min="10" max="10" width="10" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="72" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="66" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="55.140625" style="17" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="63"/>
-      <c r="K1" s="72"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="57"/>
+      <c r="K1" s="66"/>
     </row>
     <row r="2" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64">
+      <c r="A2" s="58">
         <f>Indicator!B2</f>
         <v>44826</v>
       </c>
       <c r="B2" s="43">
         <f>Indicator!$C$9</f>
-        <v>3782.86</v>
+        <v>3782.36</v>
       </c>
       <c r="C2" s="43">
         <f>Indicator!$C$10</f>
-        <v>0</v>
+        <v>3757.99</v>
       </c>
       <c r="D2" s="43">
         <f>Indicator!$C$11</f>
-        <v>0</v>
+        <v>3773.96</v>
       </c>
       <c r="E2" s="43">
         <f>Indicator!$C$12</f>
-        <v>0</v>
+        <v>3835.41</v>
       </c>
       <c r="F2" s="44">
         <f>Indicator!$C$13</f>
@@ -5195,33 +5348,33 @@
       </c>
       <c r="G2" s="44">
         <f>Indicator!$F$8</f>
-        <v>0.32414092913811315</v>
-      </c>
-      <c r="H2" s="65">
+        <v>0.32110807324379981</v>
+      </c>
+      <c r="H2" s="59">
         <f>SUMIF(Trades!A:A,Tracker!A2,Trades!H:H)</f>
         <v>9.7100000000000009</v>
       </c>
-      <c r="I2" s="66">
+      <c r="I2" s="60">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A2,  Trades!C:C, "STO")</f>
         <v>9.7100000000000009</v>
       </c>
       <c r="J2" s="21"/>
-      <c r="K2" s="72"/>
+      <c r="K2" s="66"/>
     </row>
     <row r="3" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="64"/>
+      <c r="A3" s="58"/>
       <c r="B3" s="42"/>
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
       <c r="E3" s="42"/>
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="67"/>
-      <c r="K3" s="72"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="61"/>
+      <c r="K3" s="66"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="62" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="45" t="s">
@@ -5245,24 +5398,24 @@
       <c r="H4" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="69" t="s">
+      <c r="I4" s="63" t="s">
         <v>64</v>
       </c>
       <c r="J4" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="K4" s="73" t="s">
+      <c r="K4" s="67" t="s">
         <v>65</v>
       </c>
       <c r="L4" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="M4" s="80" t="s">
+      <c r="M4" s="74" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="64">
+      <c r="A5" s="58">
         <v>44824</v>
       </c>
       <c r="B5" s="42">
@@ -5286,14 +5439,14 @@
       <c r="H5" s="17">
         <v>7.2899999999999991</v>
       </c>
-      <c r="I5" s="67">
+      <c r="I5" s="61">
         <v>7.2899999999999991</v>
       </c>
       <c r="J5" s="21">
         <f>H5/I5</f>
         <v>1</v>
       </c>
-      <c r="K5" s="72">
+      <c r="K5" s="66">
         <f>H5*100</f>
         <v>728.99999999999989</v>
       </c>
@@ -5303,7 +5456,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="64">
+      <c r="A6" s="58">
         <v>44825</v>
       </c>
       <c r="B6" s="42">
@@ -5327,14 +5480,14 @@
       <c r="H6" s="17">
         <v>3.84</v>
       </c>
-      <c r="I6" s="67">
+      <c r="I6" s="61">
         <v>5.17</v>
       </c>
       <c r="J6" s="21">
         <f>H6/I6</f>
         <v>0.74274661508704065</v>
       </c>
-      <c r="K6" s="72">
+      <c r="K6" s="66">
         <f>K5+H6*100</f>
         <v>1113</v>
       </c>
@@ -5347,7 +5500,45 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J7" s="21"/>
+      <c r="A7" s="58">
+        <v>44826</v>
+      </c>
+      <c r="B7" s="42">
+        <v>3782.36</v>
+      </c>
+      <c r="C7" s="42">
+        <v>3757.99</v>
+      </c>
+      <c r="D7" s="42">
+        <v>3773.96</v>
+      </c>
+      <c r="E7" s="42">
+        <v>3835.41</v>
+      </c>
+      <c r="F7" s="41">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="G7" s="41">
+        <v>0.32110807324379981</v>
+      </c>
+      <c r="H7" s="17">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="I7" s="61">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="J7" s="21">
+        <f>H7/I7</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="66">
+        <f>K6+H7*100</f>
+        <v>2084</v>
+      </c>
+      <c r="L7">
+        <f>I7*100+L6</f>
+        <v>2217</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5359,69 +5550,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="54" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="55" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="49" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" style="31" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="56" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="57" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" style="79" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" style="79" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="50" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="51" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" style="73" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:12" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="I1" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="79" t="s">
+      <c r="J1" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="58" t="s">
+      <c r="K1" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="79" t="s">
+      <c r="L1" s="91" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="54">
+      <c r="A2" s="48">
         <v>44824</v>
       </c>
-      <c r="B2" s="55">
+      <c r="B2" s="49">
         <v>949</v>
       </c>
       <c r="C2" s="31" t="s">
@@ -5436,26 +5627,26 @@
       <c r="F2" s="31">
         <v>1</v>
       </c>
-      <c r="G2" s="56">
+      <c r="G2" s="50">
         <v>4.2699999999999996</v>
       </c>
-      <c r="H2" s="57">
-        <f>G2*F2</f>
+      <c r="H2" s="51">
+        <f t="shared" ref="H2:H7" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
-      <c r="I2" s="58">
+      <c r="I2" s="52">
         <v>3</v>
       </c>
-      <c r="J2" s="79">
-        <f>-I2*G2</f>
+      <c r="J2" s="73">
+        <f t="shared" ref="J2:J4" si="1">-I2*H2</f>
         <v>-12.809999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="54">
+      <c r="A3" s="48">
         <v>44824</v>
       </c>
-      <c r="B3" s="55">
+      <c r="B3" s="49">
         <v>950</v>
       </c>
       <c r="C3" s="31" t="s">
@@ -5470,26 +5661,26 @@
       <c r="F3" s="31">
         <v>1</v>
       </c>
-      <c r="G3" s="56">
+      <c r="G3" s="50">
         <v>3.02</v>
       </c>
-      <c r="H3" s="57">
-        <f>G3*F3</f>
+      <c r="H3" s="51">
+        <f t="shared" si="0"/>
         <v>3.02</v>
       </c>
-      <c r="I3" s="58">
+      <c r="I3" s="52">
         <v>3</v>
       </c>
-      <c r="J3" s="79">
-        <f>-I3*G3</f>
+      <c r="J3" s="73">
+        <f t="shared" si="1"/>
         <v>-9.06</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="54">
+      <c r="A4" s="48">
         <v>44825</v>
       </c>
-      <c r="B4" s="55">
+      <c r="B4" s="49">
         <v>944</v>
       </c>
       <c r="C4" s="31" t="s">
@@ -5504,33 +5695,33 @@
       <c r="F4" s="31">
         <v>1</v>
       </c>
-      <c r="G4" s="56">
+      <c r="G4" s="50">
         <v>5.17</v>
       </c>
-      <c r="H4" s="57">
-        <f>G4*F4</f>
+      <c r="H4" s="51">
+        <f t="shared" si="0"/>
         <v>5.17</v>
       </c>
-      <c r="I4" s="58">
+      <c r="I4" s="52">
         <v>2.5</v>
       </c>
-      <c r="J4" s="79">
-        <f>-I4*G4</f>
+      <c r="J4" s="73">
+        <f t="shared" si="1"/>
         <v>-12.925000000000001</v>
       </c>
-      <c r="K4" s="58">
+      <c r="K4" s="52">
         <v>0.75</v>
       </c>
-      <c r="L4" s="79">
+      <c r="L4" s="73">
         <f>-G4+K4*G4</f>
         <v>-1.2925</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="54">
+      <c r="A5" s="48">
         <v>44825</v>
       </c>
-      <c r="B5" s="55">
+      <c r="B5" s="49">
         <v>243</v>
       </c>
       <c r="C5" s="31" t="s">
@@ -5542,25 +5733,25 @@
       <c r="F5" s="31">
         <v>1</v>
       </c>
-      <c r="G5" s="56">
+      <c r="G5" s="50">
         <v>-1.33</v>
       </c>
-      <c r="H5" s="57">
-        <f>G5*F5</f>
+      <c r="H5" s="51">
+        <f t="shared" si="0"/>
         <v>-1.33</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="54">
+      <c r="A6" s="48">
         <v>44826</v>
       </c>
-      <c r="B6" s="55">
+      <c r="B6" s="49">
         <v>937</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="69" t="s">
         <v>91</v>
       </c>
       <c r="E6" s="31">
@@ -5569,28 +5760,32 @@
       <c r="F6" s="31">
         <v>1</v>
       </c>
-      <c r="G6" s="56">
+      <c r="G6" s="50">
         <v>4.97</v>
       </c>
-      <c r="H6" s="57">
-        <f>G6*F6</f>
+      <c r="H6" s="51">
+        <f t="shared" si="0"/>
         <v>4.97</v>
       </c>
-      <c r="I6" s="58">
+      <c r="I6" s="52">
         <v>3</v>
       </c>
+      <c r="J6" s="73">
+        <f>-I6*H6</f>
+        <v>-14.91</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="54">
+      <c r="A7" s="48">
         <v>44826</v>
       </c>
-      <c r="B7" s="55">
+      <c r="B7" s="49">
         <v>946</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="75" t="s">
+      <c r="D7" s="69" t="s">
         <v>90</v>
       </c>
       <c r="E7" s="31">
@@ -5599,19 +5794,327 @@
       <c r="F7" s="31">
         <v>2</v>
       </c>
-      <c r="G7" s="56">
+      <c r="G7" s="50">
         <v>2.37</v>
       </c>
-      <c r="H7" s="57">
-        <f>G7*F7</f>
+      <c r="H7" s="51">
+        <f t="shared" si="0"/>
         <v>4.74</v>
       </c>
-      <c r="I7" s="58">
+      <c r="I7" s="52">
         <v>3</v>
+      </c>
+      <c r="J7" s="73">
+        <f>-I7*H7</f>
+        <v>-14.22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F65F32E-FB9F-420E-8864-907EF6C913D5}">
+  <dimension ref="B2:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="8" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="92"/>
+      <c r="C6" s="92" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="92" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="92" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="92" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="92" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="92" t="s">
+        <v>95</v>
+      </c>
+      <c r="I6" s="92"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="92" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="93">
+        <v>-1.5</v>
+      </c>
+      <c r="D7" s="93">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="E7" s="93">
+        <v>-1</v>
+      </c>
+      <c r="F7" s="93">
+        <v>1</v>
+      </c>
+      <c r="G7" s="93">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H7" s="93">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="92" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8">
+        <v>-75</v>
+      </c>
+      <c r="D8">
+        <v>-55</v>
+      </c>
+      <c r="E8">
+        <v>-50</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+      <c r="G8">
+        <v>55</v>
+      </c>
+      <c r="H8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="92" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="94">
+        <v>-0.43319999999999997</v>
+      </c>
+      <c r="D9" s="94">
+        <v>-0.36430000000000001</v>
+      </c>
+      <c r="E9" s="94">
+        <v>-0.34129999999999999</v>
+      </c>
+      <c r="F9" s="94">
+        <v>0.34129999999999999</v>
+      </c>
+      <c r="G9" s="94">
+        <v>0.36430000000000001</v>
+      </c>
+      <c r="H9" s="94">
+        <v>0.43319999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="92" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="95">
+        <v>-250</v>
+      </c>
+      <c r="D10" s="95">
+        <v>0</v>
+      </c>
+      <c r="E10" s="95">
+        <v>500</v>
+      </c>
+      <c r="F10" s="95">
+        <v>500</v>
+      </c>
+      <c r="G10" s="95">
+        <v>0</v>
+      </c>
+      <c r="H10" s="95">
+        <v>-250</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="92" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="99" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="99" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="99" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="99"/>
+      <c r="G13" s="92"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="96">
+        <f>E10</f>
+        <v>500</v>
+      </c>
+      <c r="D14" s="94">
+        <f>F9-E9</f>
+        <v>0.68259999999999998</v>
+      </c>
+      <c r="E14" s="96">
+        <f>C14*D14</f>
+        <v>341.3</v>
+      </c>
+      <c r="F14" s="94"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="96">
+        <f>C10</f>
+        <v>-250</v>
+      </c>
+      <c r="D15" s="94">
+        <f>100%+C9-H9</f>
+        <v>0.1336</v>
+      </c>
+      <c r="E15" s="96">
+        <f>D15*C15</f>
+        <v>-33.4</v>
+      </c>
+      <c r="F15" s="94"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="96">
+        <v>0</v>
+      </c>
+      <c r="D16" s="94">
+        <f>G9-D9-D14</f>
+        <v>4.6000000000000041E-2</v>
+      </c>
+      <c r="E16" s="96">
+        <f t="shared" ref="E16:E17" si="0">D16*C16</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="94"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="96">
+        <v>-250</v>
+      </c>
+      <c r="D17" s="94">
+        <f>(H9-G9)*2</f>
+        <v>0.13779999999999992</v>
+      </c>
+      <c r="E17" s="96">
+        <f t="shared" si="0"/>
+        <v>-34.449999999999982</v>
+      </c>
+      <c r="F17" s="94"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="95"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="95"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="92" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="100" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="100" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="100" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="96">
+        <f>SUM(E14:E17)</f>
+        <v>273.45000000000005</v>
+      </c>
+      <c r="D21" s="97">
+        <f>C21*21</f>
+        <v>5742.4500000000007</v>
+      </c>
+      <c r="E21" s="96">
+        <f>C21*252</f>
+        <v>68909.400000000009</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="92" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="96">
+        <f>E10</f>
+        <v>500</v>
+      </c>
+      <c r="D22" s="97">
+        <f>C22*21</f>
+        <v>10500</v>
+      </c>
+      <c r="E22" s="96">
+        <f>C22*252</f>
+        <v>126000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="92" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="98">
+        <f>C21/C22</f>
+        <v>0.54690000000000005</v>
+      </c>
+      <c r="D23" s="98">
+        <f>D21/D22</f>
+        <v>0.54690000000000005</v>
+      </c>
+      <c r="E23" s="98">
+        <f>E21/E22</f>
+        <v>0.54690000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Market Open Sep23/2022 - Update 0DTE Experiment.xlsx
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE7F219-D0A4-4CE6-9C0A-8D2D48EDFF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276166EE-00A8-489B-9E7B-8C82D65FE323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27525" yWindow="5010" windowWidth="23580" windowHeight="14010" activeTab="3" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
+    <workbookView xWindow="27990" yWindow="5325" windowWidth="23580" windowHeight="14010" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="117">
   <si>
     <t>SPX Open</t>
   </si>
@@ -379,6 +379,15 @@
   </si>
   <si>
     <t>Profit / Loss</t>
+  </si>
+  <si>
+    <t>Sep23 3685/3660 @ -6.50 Bull Put</t>
+  </si>
+  <si>
+    <t>Discovered IBKR-Web does not live update Delta</t>
+  </si>
+  <si>
+    <t>Sep23 3665/3640 @ -4.00 Bull Put</t>
   </si>
 </sst>
 </file>
@@ -552,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -770,6 +779,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="5" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -4666,8 +4681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{044E485C-BC7E-40C9-B7A6-38794294458B}">
   <dimension ref="B1:K28"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4689,10 +4704,10 @@
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="20">
-        <v>44826</v>
+        <v>44827</v>
       </c>
       <c r="C2" s="65">
-        <v>0.69236111111111109</v>
+        <v>0.40972222222222227</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4721,14 +4736,14 @@
         <v>3</v>
       </c>
       <c r="C5" s="12">
-        <v>3871.4</v>
+        <v>3782.36</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="27">
         <f>(C9-C18)/(C17-C18)</f>
-        <v>0.43878819282165138</v>
+        <v>6.8059372151140718E-2</v>
       </c>
       <c r="G5" s="25">
         <v>0.4</v>
@@ -4740,14 +4755,14 @@
         <v>4</v>
       </c>
       <c r="C6" s="13">
-        <v>3789.93</v>
+        <v>3757.99</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="27">
         <f>(C9-C23)/(C22-C23)</f>
-        <v>0.27003371226894063</v>
+        <v>0.1059023383282697</v>
       </c>
       <c r="G6" s="25">
         <v>0.33</v>
@@ -4759,14 +4774,14 @@
         <v>12</v>
       </c>
       <c r="C7" s="13">
-        <v>3822.93</v>
+        <v>3773.96</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="28">
         <f>(C9-C28)/(C27-C28)</f>
-        <v>0.20919137431995871</v>
+        <v>3.7522048178788195E-2</v>
       </c>
       <c r="G7" s="26">
         <v>0.27</v>
@@ -4778,14 +4793,14 @@
         <v>10</v>
       </c>
       <c r="C8" s="13">
-        <v>3864.09</v>
+        <v>3835.41</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="29">
         <f>F5*G5+F6*G6+F7*G7</f>
-        <v>0.32110807324379981</v>
+        <v>7.2302473517058111E-2</v>
       </c>
       <c r="G8" s="24" t="s">
         <v>28</v>
@@ -4797,7 +4812,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="12">
-        <v>3782.36</v>
+        <v>3704</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -4806,9 +4821,7 @@
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13">
-        <v>3757.99</v>
-      </c>
+      <c r="C10" s="13"/>
       <c r="E10" s="10" t="s">
         <v>27</v>
       </c>
@@ -4824,9 +4837,7 @@
       <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="13">
-        <v>3773.96</v>
-      </c>
+      <c r="C11" s="13"/>
       <c r="E11" s="15" t="s">
         <v>58</v>
       </c>
@@ -4841,9 +4852,7 @@
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13">
-        <v>3835.41</v>
-      </c>
+      <c r="C12" s="13"/>
       <c r="E12" s="16" t="s">
         <v>60</v>
       </c>
@@ -4859,7 +4868,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="14">
-        <v>0.25900000000000001</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>61</v>
@@ -4903,7 +4912,7 @@
       </c>
       <c r="C16" s="4">
         <f>C6*C$13*252^-0.5</f>
-        <v>61.834475642448638</v>
+        <v>62.49701523665361</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>63</v>
@@ -4921,7 +4930,7 @@
       </c>
       <c r="C17" s="4">
         <f>C6+C16</f>
-        <v>3851.7644756424484</v>
+        <v>3820.4870152366534</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>59</v>
@@ -4939,7 +4948,7 @@
       </c>
       <c r="C18" s="6">
         <f>C6-C16</f>
-        <v>3728.0955243575513</v>
+        <v>3695.4929847633462</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4955,7 +4964,7 @@
       </c>
       <c r="C21" s="4">
         <f>C7*C$13*(2/252)^0.5</f>
-        <v>88.208581353988166</v>
+        <v>88.759724814447566</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -4964,7 +4973,7 @@
       </c>
       <c r="C22" s="4">
         <f>C7+C21</f>
-        <v>3911.1385813539882</v>
+        <v>3862.7197248144475</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4973,7 +4982,7 @@
       </c>
       <c r="C23" s="6">
         <f>C7-C21</f>
-        <v>3734.7214186460114</v>
+        <v>3685.2002751855525</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4989,7 +4998,7 @@
       </c>
       <c r="C26" s="4">
         <f>C17*C$13*(5/252)^0.5</f>
-        <v>140.5219666522591</v>
+        <v>142.07163766674157</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -4998,7 +5007,7 @@
       </c>
       <c r="C27" s="4">
         <f>C8+C26</f>
-        <v>4004.6119666522591</v>
+        <v>3977.4816376667413</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5007,7 +5016,7 @@
       </c>
       <c r="C28" s="6">
         <f>C8-C26</f>
-        <v>3723.5680333477412</v>
+        <v>3693.3383623332584</v>
       </c>
     </row>
   </sheetData>
@@ -5126,7 +5135,7 @@
       </c>
       <c r="H4" s="72">
         <f>(SUMIF(Tracker!H:H, "&gt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&gt;0", Tracker!H2))/F4*100</f>
-        <v>694.66666666666663</v>
+        <v>694.66666666666652</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>88</v>
@@ -5218,7 +5227,7 @@
       </c>
       <c r="F8" s="76">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>28610.850928801134</v>
+        <v>2198.9330550062496</v>
       </c>
       <c r="G8" s="76"/>
       <c r="J8" s="22" t="s">
@@ -5246,7 +5255,7 @@
       </c>
       <c r="F9" s="76">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>17.096752173544029</v>
+        <v>7.7740575614878065</v>
       </c>
       <c r="G9" s="76"/>
       <c r="J9" s="22" t="s">
@@ -5286,10 +5295,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C82D01-CC02-4066-B9D6-9DFF5A0A89C9}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5324,39 +5333,39 @@
     <row r="2" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="58">
         <f>Indicator!B2</f>
-        <v>44826</v>
+        <v>44827</v>
       </c>
       <c r="B2" s="43">
         <f>Indicator!$C$9</f>
-        <v>3782.36</v>
+        <v>3704</v>
       </c>
       <c r="C2" s="43">
         <f>Indicator!$C$10</f>
-        <v>3757.99</v>
+        <v>0</v>
       </c>
       <c r="D2" s="43">
         <f>Indicator!$C$11</f>
-        <v>3773.96</v>
+        <v>0</v>
       </c>
       <c r="E2" s="43">
         <f>Indicator!$C$12</f>
-        <v>3835.41</v>
+        <v>0</v>
       </c>
       <c r="F2" s="44">
         <f>Indicator!$C$13</f>
-        <v>0.25900000000000001</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="G2" s="44">
         <f>Indicator!$F$8</f>
-        <v>0.32110807324379981</v>
+        <v>7.2302473517058111E-2</v>
       </c>
       <c r="H2" s="59">
         <f>SUMIF(Trades!A:A,Tracker!A2,Trades!H:H)</f>
-        <v>9.7100000000000009</v>
+        <v>10.44</v>
       </c>
       <c r="I2" s="60">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A2,  Trades!C:C, "STO")</f>
-        <v>9.7100000000000009</v>
+        <v>10.44</v>
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="66"/>
@@ -5540,6 +5549,11 @@
         <v>2217</v>
       </c>
     </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="17" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5548,10 +5562,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5560,7 +5574,7 @@
     <col min="2" max="2" width="9.7109375" style="49" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="102" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.140625" style="50" customWidth="1"/>
     <col min="8" max="8" width="7.140625" style="51" customWidth="1"/>
@@ -5583,7 +5597,7 @@
       <c r="D1" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="101" t="s">
         <v>35</v>
       </c>
       <c r="F1" s="34" t="s">
@@ -5621,7 +5635,7 @@
       <c r="D2" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="31">
+      <c r="E2" s="102">
         <v>-0.15</v>
       </c>
       <c r="F2" s="31">
@@ -5631,7 +5645,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="51">
-        <f t="shared" ref="H2:H7" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H9" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="52">
@@ -5655,7 +5669,7 @@
       <c r="D3" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="102">
         <v>0.09</v>
       </c>
       <c r="F3" s="31">
@@ -5689,7 +5703,7 @@
       <c r="D4" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="102">
         <v>-0.15</v>
       </c>
       <c r="F4" s="31">
@@ -5754,7 +5768,7 @@
       <c r="D6" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="102">
         <v>-0.16</v>
       </c>
       <c r="F6" s="31">
@@ -5788,7 +5802,7 @@
       <c r="D7" s="69" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="102">
         <v>0.13</v>
       </c>
       <c r="F7" s="31">
@@ -5807,6 +5821,74 @@
       <c r="J7" s="73">
         <f>-I7*H7</f>
         <v>-14.22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="48">
+        <v>44827</v>
+      </c>
+      <c r="B8" s="49">
+        <v>936</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="69" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="102">
+        <v>-0.3</v>
+      </c>
+      <c r="F8" s="31">
+        <v>1</v>
+      </c>
+      <c r="G8" s="50">
+        <v>6.47</v>
+      </c>
+      <c r="H8" s="51">
+        <f t="shared" si="0"/>
+        <v>6.47</v>
+      </c>
+      <c r="I8" s="52">
+        <v>3</v>
+      </c>
+      <c r="J8" s="73">
+        <f>-I8*H8</f>
+        <v>-19.41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="48">
+        <v>44827</v>
+      </c>
+      <c r="B9" s="49">
+        <v>949</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="102">
+        <v>-0.19</v>
+      </c>
+      <c r="F9" s="31">
+        <v>1</v>
+      </c>
+      <c r="G9" s="50">
+        <v>3.97</v>
+      </c>
+      <c r="H9" s="51">
+        <f t="shared" si="0"/>
+        <v>3.97</v>
+      </c>
+      <c r="I9" s="52">
+        <v>3</v>
+      </c>
+      <c r="J9" s="73">
+        <f>-I9*H9</f>
+        <v>-11.91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Market Close Sep23/2022 - Update 0DTE Experiment.xlsx
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276166EE-00A8-489B-9E7B-8C82D65FE323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637D1496-A300-4E4C-AF90-554E4052DE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27990" yWindow="5325" windowWidth="23580" windowHeight="14010" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
+    <workbookView xWindow="3120" yWindow="5685" windowWidth="23580" windowHeight="14010" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="120">
   <si>
     <t>SPX Open</t>
   </si>
@@ -384,10 +384,19 @@
     <t>Sep23 3685/3660 @ -6.50 Bull Put</t>
   </si>
   <si>
-    <t>Discovered IBKR-Web does not live update Delta</t>
-  </si>
-  <si>
     <t>Sep23 3665/3640 @ -4.00 Bull Put</t>
+  </si>
+  <si>
+    <t>BTC SL</t>
+  </si>
+  <si>
+    <t>Sep23 3665/3640 @ -12.40 Bull Put</t>
+  </si>
+  <si>
+    <t>Sep23 3655/3640 @ -2.25 Bull Put</t>
+  </si>
+  <si>
+    <t>Discovered IBKR-Web does not live update Delta; deviated from strategy; high volitility triggered SL</t>
   </si>
 </sst>
 </file>
@@ -895,6 +904,9 @@
                 <c:pt idx="2">
                   <c:v>44826</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44827</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -912,6 +924,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2084</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.999999999999545</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -990,6 +1005,9 @@
                       <c:pt idx="2">
                         <c:v>44826</c:v>
                       </c:pt>
+                      <c:pt idx="3">
+                        <c:v>44827</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1013,6 +1031,9 @@
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>9.7100000000000009</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-19.870000000000005</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1079,6 +1100,9 @@
                       <c:pt idx="2">
                         <c:v>44826</c:v>
                       </c:pt>
+                      <c:pt idx="3">
+                        <c:v>44827</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1102,6 +1126,9 @@
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>9.7100000000000009</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>12.66</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1168,6 +1195,9 @@
                       <c:pt idx="2">
                         <c:v>44826</c:v>
                       </c:pt>
+                      <c:pt idx="3">
+                        <c:v>44827</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1191,6 +1221,9 @@
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-1.5695102685624016</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1472,6 +1505,9 @@
                 <c:pt idx="2">
                   <c:v>44826</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44827</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1490,6 +1526,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9.7100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.66</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -1567,6 +1606,9 @@
                       <c:pt idx="2">
                         <c:v>44826</c:v>
                       </c:pt>
+                      <c:pt idx="3">
+                        <c:v>44827</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1590,6 +1632,9 @@
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-1.5695102685624016</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1653,6 +1698,9 @@
                       <c:pt idx="2">
                         <c:v>44826</c:v>
                       </c:pt>
+                      <c:pt idx="3">
+                        <c:v>44827</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1676,6 +1724,9 @@
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>2084</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>96.999999999999545</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1725,6 +1776,9 @@
                 <c:pt idx="2">
                   <c:v>44826</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44827</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1743,6 +1797,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9.7100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-19.870000000000005</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -1777,7 +1834,7 @@
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2107,6 +2164,9 @@
                 <c:pt idx="2">
                   <c:v>44826</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44827</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -2125,6 +2185,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.5695102685624016</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2188,6 +2251,9 @@
                       <c:pt idx="2">
                         <c:v>44826</c:v>
                       </c:pt>
+                      <c:pt idx="3">
+                        <c:v>44827</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2211,6 +2277,9 @@
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>9.7100000000000009</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>12.66</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2274,6 +2343,9 @@
                       <c:pt idx="2">
                         <c:v>44826</c:v>
                       </c:pt>
+                      <c:pt idx="3">
+                        <c:v>44827</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2297,6 +2369,9 @@
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>2084</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>96.999999999999545</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2367,6 +2442,9 @@
                       <c:pt idx="2">
                         <c:v>44826</c:v>
                       </c:pt>
+                      <c:pt idx="3">
+                        <c:v>44827</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2390,6 +2468,9 @@
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>9.7100000000000009</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-19.870000000000005</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4682,7 +4763,7 @@
   <dimension ref="B1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4707,7 +4788,7 @@
         <v>44827</v>
       </c>
       <c r="C2" s="65">
-        <v>0.40972222222222227</v>
+        <v>0.19305555555555554</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4743,7 +4824,7 @@
       </c>
       <c r="F5" s="27">
         <f>(C9-C18)/(C17-C18)</f>
-        <v>6.8059372151140718E-2</v>
+        <v>0.26561758376169692</v>
       </c>
       <c r="G5" s="25">
         <v>0.4</v>
@@ -4762,7 +4843,7 @@
       </c>
       <c r="F6" s="27">
         <f>(C9-C23)/(C22-C23)</f>
-        <v>0.1059023383282697</v>
+        <v>0.2495364121152378</v>
       </c>
       <c r="G6" s="25">
         <v>0.33</v>
@@ -4781,7 +4862,7 @@
       </c>
       <c r="F7" s="28">
         <f>(C9-C28)/(C27-C28)</f>
-        <v>3.7522048178788195E-2</v>
+        <v>0.13846254004577735</v>
       </c>
       <c r="G7" s="26">
         <v>0.27</v>
@@ -4800,7 +4881,7 @@
       </c>
       <c r="F8" s="29">
         <f>F5*G5+F6*G6+F7*G7</f>
-        <v>7.2302473517058111E-2</v>
+        <v>0.22597893531506713</v>
       </c>
       <c r="G8" s="24" t="s">
         <v>28</v>
@@ -4812,7 +4893,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="12">
-        <v>3704</v>
+        <v>3727.14</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -4821,7 +4902,9 @@
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="13">
+        <v>3693.49</v>
+      </c>
       <c r="E10" s="10" t="s">
         <v>27</v>
       </c>
@@ -4837,7 +4920,9 @@
       <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="13"/>
+      <c r="C11" s="13">
+        <v>3725.74</v>
+      </c>
       <c r="E11" s="15" t="s">
         <v>58</v>
       </c>
@@ -4852,7 +4937,9 @@
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="13">
+        <v>3799.45</v>
+      </c>
       <c r="E12" s="16" t="s">
         <v>60</v>
       </c>
@@ -4868,7 +4955,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="14">
-        <v>0.26400000000000001</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>61</v>
@@ -4912,7 +4999,7 @@
       </c>
       <c r="C16" s="4">
         <f>C6*C$13*252^-0.5</f>
-        <v>62.49701523665361</v>
+        <v>65.811250893142827</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>63</v>
@@ -4930,7 +5017,7 @@
       </c>
       <c r="C17" s="4">
         <f>C6+C16</f>
-        <v>3820.4870152366534</v>
+        <v>3823.8012508931424</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>59</v>
@@ -4948,7 +5035,7 @@
       </c>
       <c r="C18" s="6">
         <f>C6-C16</f>
-        <v>3695.4929847633462</v>
+        <v>3692.1787491068571</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4964,7 +5051,7 @@
       </c>
       <c r="C21" s="4">
         <f>C7*C$13*(2/252)^0.5</f>
-        <v>88.759724814447566</v>
+        <v>93.466679918244026</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -4973,7 +5060,7 @@
       </c>
       <c r="C22" s="4">
         <f>C7+C21</f>
-        <v>3862.7197248144475</v>
+        <v>3867.4266799182442</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4982,7 +5069,7 @@
       </c>
       <c r="C23" s="6">
         <f>C7-C21</f>
-        <v>3685.2002751855525</v>
+        <v>3680.4933200817559</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4998,7 +5085,7 @@
       </c>
       <c r="C26" s="4">
         <f>C17*C$13*(5/252)^0.5</f>
-        <v>142.07163766674157</v>
+        <v>149.7355212011901</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -5007,7 +5094,7 @@
       </c>
       <c r="C27" s="4">
         <f>C8+C26</f>
-        <v>3977.4816376667413</v>
+        <v>3985.1455212011901</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5016,7 +5103,7 @@
       </c>
       <c r="C28" s="6">
         <f>C8-C26</f>
-        <v>3693.3383623332584</v>
+        <v>3685.6744787988096</v>
       </c>
     </row>
   </sheetData>
@@ -5030,7 +5117,7 @@
   <dimension ref="B1:N27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5093,14 +5180,14 @@
       </c>
       <c r="F3" s="78">
         <f>COUNTA(Tracker!K:K)-1</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3" s="80" t="s">
         <v>28</v>
       </c>
       <c r="H3" s="72">
         <f>C7/F3</f>
-        <v>694.66666666666663</v>
+        <v>24.249999999999886</v>
       </c>
       <c r="J3" s="22" t="s">
         <v>87</v>
@@ -5131,11 +5218,11 @@
       </c>
       <c r="G4" s="81">
         <f>F4/F3</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H4" s="72">
         <f>(SUMIF(Tracker!H:H, "&gt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&gt;0", Tracker!H2))/F4*100</f>
-        <v>694.66666666666652</v>
+        <v>694.66666666666663</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>88</v>
@@ -5161,15 +5248,15 @@
       </c>
       <c r="F5" s="78">
         <f>COUNTIF(Tracker!J:J, "&lt;0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="81">
         <f>F5/F3</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H5" s="72">
         <f>IFERROR((SUMIF(Tracker!H:H, "&lt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&lt;0", Tracker!H2))/F5*100, 0)</f>
-        <v>0</v>
+        <v>-1987.0000000000005</v>
       </c>
       <c r="J5" s="22" t="s">
         <v>89</v>
@@ -5194,14 +5281,14 @@
       </c>
       <c r="C7" s="72">
         <f>INDEX(Tracker!K:K, COUNTA(Tracker!K:K)+3,1)</f>
-        <v>2084</v>
+        <v>96.999999999999545</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>72</v>
       </c>
       <c r="F7" s="76">
         <f>C7/C4</f>
-        <v>8.8000624956453624E-2</v>
+        <v>4.0959983784913442E-3</v>
       </c>
       <c r="G7" s="76"/>
       <c r="J7" s="22" t="s">
@@ -5220,14 +5307,14 @@
       </c>
       <c r="C8" s="72">
         <f>INDEX(Tracker!L:L, COUNTA(Tracker!L:L)+3,1)</f>
-        <v>2217</v>
+        <v>3483</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>77</v>
       </c>
       <c r="F8" s="76">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>2198.9330550062496</v>
+        <v>0.45207922266486622</v>
       </c>
       <c r="G8" s="76"/>
       <c r="J8" s="22" t="s">
@@ -5248,14 +5335,14 @@
       </c>
       <c r="C9" s="76">
         <f>C7/C8</f>
-        <v>0.94000902119981955</v>
+        <v>2.7849554981337798E-2</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>78</v>
       </c>
       <c r="F9" s="76">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>7.7740575614878065</v>
+        <v>0.1109955883822813</v>
       </c>
       <c r="G9" s="76"/>
       <c r="J9" s="22" t="s">
@@ -5298,7 +5385,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5337,35 +5424,35 @@
       </c>
       <c r="B2" s="43">
         <f>Indicator!$C$9</f>
-        <v>3704</v>
+        <v>3727.14</v>
       </c>
       <c r="C2" s="43">
         <f>Indicator!$C$10</f>
-        <v>0</v>
+        <v>3693.49</v>
       </c>
       <c r="D2" s="43">
         <f>Indicator!$C$11</f>
-        <v>0</v>
+        <v>3725.74</v>
       </c>
       <c r="E2" s="43">
         <f>Indicator!$C$12</f>
-        <v>0</v>
+        <v>3799.45</v>
       </c>
       <c r="F2" s="44">
         <f>Indicator!$C$13</f>
-        <v>0.26400000000000001</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="G2" s="44">
         <f>Indicator!$F$8</f>
-        <v>7.2302473517058111E-2</v>
+        <v>0.22597893531506713</v>
       </c>
       <c r="H2" s="59">
         <f>SUMIF(Trades!A:A,Tracker!A2,Trades!H:H)</f>
-        <v>10.44</v>
+        <v>-19.870000000000005</v>
       </c>
       <c r="I2" s="60">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A2,  Trades!C:C, "STO")</f>
-        <v>10.44</v>
+        <v>12.66</v>
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="66"/>
@@ -5550,8 +5637,47 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="58">
+        <v>44827</v>
+      </c>
+      <c r="B8" s="42">
+        <v>3727.14</v>
+      </c>
+      <c r="C8" s="42">
+        <v>3693.49</v>
+      </c>
+      <c r="D8" s="42">
+        <v>3725.74</v>
+      </c>
+      <c r="E8" s="42">
+        <v>3799.45</v>
+      </c>
+      <c r="F8" s="41">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="G8" s="41">
+        <v>0.22597893531506713</v>
+      </c>
+      <c r="H8" s="17">
+        <v>-19.870000000000005</v>
+      </c>
+      <c r="I8" s="61">
+        <v>12.66</v>
+      </c>
+      <c r="J8" s="21">
+        <f>H8/I8</f>
+        <v>-1.5695102685624016</v>
+      </c>
+      <c r="K8" s="66">
+        <f>K7+H8*100</f>
+        <v>96.999999999999545</v>
+      </c>
+      <c r="L8">
+        <f>I8*100+L7</f>
+        <v>3483</v>
+      </c>
       <c r="M8" s="17" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -5562,10 +5688,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:H9"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5868,7 +5994,7 @@
         <v>45</v>
       </c>
       <c r="D9" s="69" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E9" s="102">
         <v>-0.19</v>
@@ -5889,6 +6015,88 @@
       <c r="J9" s="73">
         <f>-I9*H9</f>
         <v>-11.91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="48">
+        <v>44827</v>
+      </c>
+      <c r="B10" s="49">
+        <v>240</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="69" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="31">
+        <v>1</v>
+      </c>
+      <c r="G10" s="50">
+        <v>-12.43</v>
+      </c>
+      <c r="H10" s="51">
+        <f t="shared" ref="H10:H12" si="2">G10*F10</f>
+        <v>-12.43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="48">
+        <v>44827</v>
+      </c>
+      <c r="B11" s="49">
+        <v>255</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="69" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" s="31">
+        <v>1</v>
+      </c>
+      <c r="G11" s="50">
+        <v>-20.100000000000001</v>
+      </c>
+      <c r="H11" s="51">
+        <f t="shared" si="2"/>
+        <v>-20.100000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="48">
+        <v>44827</v>
+      </c>
+      <c r="B12" s="49">
+        <v>311</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="69" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="102">
+        <v>-0.19</v>
+      </c>
+      <c r="F12" s="31">
+        <v>1</v>
+      </c>
+      <c r="G12" s="50">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="H12" s="51">
+        <f t="shared" si="2"/>
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="I12" s="52">
+        <v>3</v>
+      </c>
+      <c r="J12" s="73">
+        <f>-I12*H12</f>
+        <v>-6.66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Market Open Sep26/2022 - Update 0DTE Experiment.xlsx
New tracking twin strategies
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637D1496-A300-4E4C-AF90-554E4052DE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E307DE-0505-4D3D-A401-76581C7A1822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="5685" windowWidth="23580" windowHeight="14010" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
+    <workbookView xWindow="12855" yWindow="5925" windowWidth="23580" windowHeight="14010" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator" sheetId="1" r:id="rId1"/>
     <sheet name="Dashboard" sheetId="4" r:id="rId2"/>
     <sheet name="Tracker" sheetId="3" r:id="rId3"/>
     <sheet name="Trades" sheetId="2" r:id="rId4"/>
-    <sheet name="Statistical Proof" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="Delta15" sheetId="6" r:id="rId5"/>
+    <sheet name="DeltaInd" sheetId="7" r:id="rId6"/>
+    <sheet name="Statistical Proof" sheetId="5" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="123">
   <si>
     <t>SPX Open</t>
   </si>
@@ -397,6 +399,15 @@
   </si>
   <si>
     <t>Discovered IBKR-Web does not live update Delta; deviated from strategy; high volitility triggered SL</t>
+  </si>
+  <si>
+    <t>Sep26 3740/3765 Bear Call @ -3.30</t>
+  </si>
+  <si>
+    <t>Sep26 3650/3625 Bull Put @-4.30</t>
+  </si>
+  <si>
+    <t>Sep26 3760/3785 Bear Call @ -1.50</t>
   </si>
 </sst>
 </file>
@@ -4785,10 +4796,10 @@
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="20">
-        <v>44827</v>
+        <v>44830</v>
       </c>
       <c r="C2" s="65">
-        <v>0.19305555555555554</v>
+        <v>0.45624999999999999</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4817,14 +4828,14 @@
         <v>3</v>
       </c>
       <c r="C5" s="12">
-        <v>3782.36</v>
+        <v>3727.14</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="27">
         <f>(C9-C18)/(C17-C18)</f>
-        <v>0.26561758376169692</v>
+        <v>0.41674616372904594</v>
       </c>
       <c r="G5" s="25">
         <v>0.4</v>
@@ -4836,14 +4847,14 @@
         <v>4</v>
       </c>
       <c r="C6" s="13">
-        <v>3757.99</v>
+        <v>3693.49</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="27">
         <f>(C9-C23)/(C22-C23)</f>
-        <v>0.2495364121152378</v>
+        <v>0.26688600747623897</v>
       </c>
       <c r="G6" s="25">
         <v>0.33</v>
@@ -4855,14 +4866,14 @@
         <v>12</v>
       </c>
       <c r="C7" s="13">
-        <v>3773.96</v>
+        <v>3725.74</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="28">
         <f>(C9-C28)/(C27-C28)</f>
-        <v>0.13846254004577735</v>
+        <v>0.1034058134695641</v>
       </c>
       <c r="G7" s="26">
         <v>0.27</v>
@@ -4874,14 +4885,14 @@
         <v>10</v>
       </c>
       <c r="C8" s="13">
-        <v>3835.41</v>
+        <v>3799.45</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="29">
         <f>F5*G5+F6*G6+F7*G7</f>
-        <v>0.22597893531506713</v>
+        <v>0.28269041759555957</v>
       </c>
       <c r="G8" s="24" t="s">
         <v>28</v>
@@ -4893,7 +4904,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="12">
-        <v>3727.14</v>
+        <v>3682.72</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -4902,9 +4913,7 @@
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13">
-        <v>3693.49</v>
-      </c>
+      <c r="C10" s="13"/>
       <c r="E10" s="10" t="s">
         <v>27</v>
       </c>
@@ -4920,9 +4929,7 @@
       <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="13">
-        <v>3725.74</v>
-      </c>
+      <c r="C11" s="13"/>
       <c r="E11" s="15" t="s">
         <v>58</v>
       </c>
@@ -4937,9 +4944,7 @@
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13">
-        <v>3799.45</v>
-      </c>
+      <c r="C12" s="13"/>
       <c r="E12" s="16" t="s">
         <v>60</v>
       </c>
@@ -4999,7 +5004,7 @@
       </c>
       <c r="C16" s="4">
         <f>C6*C$13*252^-0.5</f>
-        <v>65.811250893142827</v>
+        <v>64.68170406555474</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>63</v>
@@ -5017,7 +5022,7 @@
       </c>
       <c r="C17" s="4">
         <f>C6+C16</f>
-        <v>3823.8012508931424</v>
+        <v>3758.1717040655544</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>59</v>
@@ -5035,7 +5040,7 @@
       </c>
       <c r="C18" s="6">
         <f>C6-C16</f>
-        <v>3692.1787491068571</v>
+        <v>3628.8082959344451</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5051,7 +5056,7 @@
       </c>
       <c r="C21" s="4">
         <f>C7*C$13*(2/252)^0.5</f>
-        <v>93.466679918244026</v>
+        <v>92.272453348365772</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -5060,7 +5065,7 @@
       </c>
       <c r="C22" s="4">
         <f>C7+C21</f>
-        <v>3867.4266799182442</v>
+        <v>3818.0124533483654</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5069,7 +5074,7 @@
       </c>
       <c r="C23" s="6">
         <f>C7-C21</f>
-        <v>3680.4933200817559</v>
+        <v>3633.4675466516342</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5085,7 +5090,7 @@
       </c>
       <c r="C26" s="4">
         <f>C17*C$13*(5/252)^0.5</f>
-        <v>149.7355212011901</v>
+        <v>147.1655459970313</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -5094,7 +5099,7 @@
       </c>
       <c r="C27" s="4">
         <f>C8+C26</f>
-        <v>3985.1455212011901</v>
+        <v>3946.6155459970309</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5103,7 +5108,7 @@
       </c>
       <c r="C28" s="6">
         <f>C8-C26</f>
-        <v>3685.6744787988096</v>
+        <v>3652.2844540029687</v>
       </c>
     </row>
   </sheetData>
@@ -5222,7 +5227,7 @@
       </c>
       <c r="H4" s="72">
         <f>(SUMIF(Tracker!H:H, "&gt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&gt;0", Tracker!H2))/F4*100</f>
-        <v>694.66666666666663</v>
+        <v>694.66666666666652</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>88</v>
@@ -5314,7 +5319,7 @@
       </c>
       <c r="F8" s="76">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>0.45207922266486622</v>
+        <v>0.23755894099839581</v>
       </c>
       <c r="G8" s="76"/>
       <c r="J8" s="22" t="s">
@@ -5342,7 +5347,7 @@
       </c>
       <c r="F9" s="76">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>0.1109955883822813</v>
+        <v>6.1992217001927807E-2</v>
       </c>
       <c r="G9" s="76"/>
       <c r="J9" s="22" t="s">
@@ -5420,23 +5425,23 @@
     <row r="2" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="58">
         <f>Indicator!B2</f>
-        <v>44827</v>
+        <v>44830</v>
       </c>
       <c r="B2" s="43">
         <f>Indicator!$C$9</f>
-        <v>3727.14</v>
+        <v>3682.72</v>
       </c>
       <c r="C2" s="43">
         <f>Indicator!$C$10</f>
-        <v>3693.49</v>
+        <v>0</v>
       </c>
       <c r="D2" s="43">
         <f>Indicator!$C$11</f>
-        <v>3725.74</v>
+        <v>0</v>
       </c>
       <c r="E2" s="43">
         <f>Indicator!$C$12</f>
-        <v>3799.45</v>
+        <v>0</v>
       </c>
       <c r="F2" s="44">
         <f>Indicator!$C$13</f>
@@ -5444,15 +5449,15 @@
       </c>
       <c r="G2" s="44">
         <f>Indicator!$F$8</f>
-        <v>0.22597893531506713</v>
+        <v>0.28269041759555957</v>
       </c>
       <c r="H2" s="59">
         <f>SUMIF(Trades!A:A,Tracker!A2,Trades!H:H)</f>
-        <v>-19.870000000000005</v>
+        <v>9.01</v>
       </c>
       <c r="I2" s="60">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A2,  Trades!C:C, "STO")</f>
-        <v>12.66</v>
+        <v>9.01</v>
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="66"/>
@@ -5688,10 +5693,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="H13" sqref="H13:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5700,7 +5705,7 @@
     <col min="2" max="2" width="9.7109375" style="49" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" style="102" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" style="102" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.140625" style="50" customWidth="1"/>
     <col min="8" max="8" width="7.140625" style="51" customWidth="1"/>
@@ -6037,7 +6042,7 @@
         <v>-12.43</v>
       </c>
       <c r="H10" s="51">
-        <f t="shared" ref="H10:H12" si="2">G10*F10</f>
+        <f t="shared" ref="H10:H15" si="2">G10*F10</f>
         <v>-12.43</v>
       </c>
     </row>
@@ -6097,6 +6102,108 @@
       <c r="J12" s="73">
         <f>-I12*H12</f>
         <v>-6.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="48">
+        <v>44830</v>
+      </c>
+      <c r="B13" s="49">
+        <v>742</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="69" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="102">
+        <v>-0.15</v>
+      </c>
+      <c r="F13" s="31">
+        <v>1</v>
+      </c>
+      <c r="G13" s="50">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="H13" s="51">
+        <f t="shared" si="2"/>
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="I13" s="52">
+        <v>3</v>
+      </c>
+      <c r="J13" s="73">
+        <f t="shared" ref="J13:J14" si="3">-I13*H13</f>
+        <v>-12.809999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="48">
+        <v>44830</v>
+      </c>
+      <c r="B14" s="49">
+        <v>742</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="102">
+        <v>0.15</v>
+      </c>
+      <c r="F14" s="31">
+        <v>1</v>
+      </c>
+      <c r="G14" s="50">
+        <v>3.27</v>
+      </c>
+      <c r="H14" s="51">
+        <f t="shared" si="2"/>
+        <v>3.27</v>
+      </c>
+      <c r="I14" s="52">
+        <v>3</v>
+      </c>
+      <c r="J14" s="73">
+        <f t="shared" si="3"/>
+        <v>-9.81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="48">
+        <v>44830</v>
+      </c>
+      <c r="B15" s="49">
+        <v>815</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15" s="102">
+        <v>0.1</v>
+      </c>
+      <c r="F15" s="31">
+        <v>1</v>
+      </c>
+      <c r="G15" s="50">
+        <v>1.47</v>
+      </c>
+      <c r="H15" s="51">
+        <f t="shared" si="2"/>
+        <v>1.47</v>
+      </c>
+      <c r="I15" s="52">
+        <v>3</v>
+      </c>
+      <c r="J15" s="73">
+        <f t="shared" ref="J15" si="4">-I15*H15</f>
+        <v>-4.41</v>
       </c>
     </row>
   </sheetData>
@@ -6106,6 +6213,290 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE4BC4F-EB6D-4F7C-A4AB-32C246F0D899}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="49" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" style="102" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="50" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="51" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" style="73" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="101" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="88" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="89" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="90" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="90" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="91" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="99" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="48">
+        <v>44830</v>
+      </c>
+      <c r="B2" s="49">
+        <v>742</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="69" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="102">
+        <v>-0.15</v>
+      </c>
+      <c r="F2" s="31">
+        <v>1</v>
+      </c>
+      <c r="G2" s="50">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="H2" s="51">
+        <f t="shared" ref="H2:H3" si="0">G2*F2</f>
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="I2" s="52">
+        <v>3</v>
+      </c>
+      <c r="J2" s="73">
+        <f t="shared" ref="J2:J3" si="1">-I2*H2</f>
+        <v>-12.809999999999999</v>
+      </c>
+      <c r="N2" s="73">
+        <f>SUM(H:H)</f>
+        <v>7.5399999999999991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="48">
+        <v>44830</v>
+      </c>
+      <c r="B3" s="49">
+        <v>742</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="102">
+        <v>0.15</v>
+      </c>
+      <c r="F3" s="31">
+        <v>1</v>
+      </c>
+      <c r="G3" s="50">
+        <v>3.27</v>
+      </c>
+      <c r="H3" s="51">
+        <f t="shared" si="0"/>
+        <v>3.27</v>
+      </c>
+      <c r="I3" s="52">
+        <v>3</v>
+      </c>
+      <c r="J3" s="73">
+        <f t="shared" si="1"/>
+        <v>-9.81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5E4B5F-C3CE-4821-8081-9385439A4F7E}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="49" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" style="102" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="50" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="51" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" style="73" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="101" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="88" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="89" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="90" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="90" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="91" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="99" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="48">
+        <v>44830</v>
+      </c>
+      <c r="B2" s="49">
+        <v>742</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="69" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="102">
+        <v>-0.15</v>
+      </c>
+      <c r="F2" s="31">
+        <v>1</v>
+      </c>
+      <c r="G2" s="50">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="H2" s="51">
+        <f t="shared" ref="H2:H3" si="0">G2*F2</f>
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="I2" s="52">
+        <v>3</v>
+      </c>
+      <c r="J2" s="73">
+        <f t="shared" ref="J2" si="1">-I2*H2</f>
+        <v>-12.809999999999999</v>
+      </c>
+      <c r="N2" s="73">
+        <f>SUM(H:H)</f>
+        <v>5.7399999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="48">
+        <v>44830</v>
+      </c>
+      <c r="B3" s="49">
+        <v>815</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="102">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="31">
+        <v>1</v>
+      </c>
+      <c r="G3" s="50">
+        <v>1.47</v>
+      </c>
+      <c r="H3" s="51">
+        <f t="shared" si="0"/>
+        <v>1.47</v>
+      </c>
+      <c r="I3" s="52">
+        <v>3</v>
+      </c>
+      <c r="J3" s="73">
+        <f t="shared" ref="J3" si="2">-I3*H3</f>
+        <v>-4.41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F65F32E-FB9F-420E-8864-907EF6C913D5}">
   <dimension ref="B2:I23"/>
   <sheetViews>

</xml_diff>

<commit_message>
Market Close Sep26/2022 - Update 0DTE Experiment.xlsx
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E307DE-0505-4D3D-A401-76581C7A1822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BBA2AC-BB1C-4CE4-B9FC-CB07196DC7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12855" yWindow="5925" windowWidth="23580" windowHeight="14010" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
+    <workbookView xWindow="27270" yWindow="5520" windowWidth="23580" windowHeight="14010" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Tracker" sheetId="3" r:id="rId3"/>
     <sheet name="Trades" sheetId="2" r:id="rId4"/>
     <sheet name="Delta15" sheetId="6" r:id="rId5"/>
-    <sheet name="DeltaInd" sheetId="7" r:id="rId6"/>
+    <sheet name="DeltaMR" sheetId="7" r:id="rId6"/>
     <sheet name="Statistical Proof" sheetId="5" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="124">
   <si>
     <t>SPX Open</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>Sep26 3760/3785 Bear Call @ -1.50</t>
+  </si>
+  <si>
+    <t>Sep26 3650/3625 Bull Put @ -4.30</t>
   </si>
 </sst>
 </file>
@@ -918,6 +921,9 @@
                 <c:pt idx="3">
                   <c:v>44827</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>44830</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -938,6 +944,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>96.999999999999545</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1424.9999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1019,6 +1028,9 @@
                       <c:pt idx="3">
                         <c:v>44827</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>44830</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1045,6 +1057,9 @@
                       </c:pt>
                       <c:pt idx="3">
                         <c:v>-19.870000000000005</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>13.28</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1114,6 +1129,9 @@
                       <c:pt idx="3">
                         <c:v>44827</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>44830</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1140,6 +1158,9 @@
                       </c:pt>
                       <c:pt idx="3">
                         <c:v>12.66</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>13.28</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1209,6 +1230,9 @@
                       <c:pt idx="3">
                         <c:v>44827</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>44830</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1235,6 +1259,9 @@
                       </c:pt>
                       <c:pt idx="3">
                         <c:v>-1.5695102685624016</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1519,6 +1546,9 @@
                 <c:pt idx="3">
                   <c:v>44827</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>44830</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1540,6 +1570,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>12.66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.28</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -1620,6 +1653,9 @@
                       <c:pt idx="3">
                         <c:v>44827</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>44830</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1646,6 +1682,9 @@
                       </c:pt>
                       <c:pt idx="3">
                         <c:v>-1.5695102685624016</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1712,6 +1751,9 @@
                       <c:pt idx="3">
                         <c:v>44827</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>44830</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1738,6 +1780,9 @@
                       </c:pt>
                       <c:pt idx="3">
                         <c:v>96.999999999999545</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1424.9999999999995</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1790,6 +1835,9 @@
                 <c:pt idx="3">
                   <c:v>44827</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>44830</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1811,6 +1859,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>-19.870000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.28</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2178,6 +2229,9 @@
                 <c:pt idx="3">
                   <c:v>44827</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>44830</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -2199,6 +2253,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>-1.5695102685624016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2265,6 +2322,9 @@
                       <c:pt idx="3">
                         <c:v>44827</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>44830</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2291,6 +2351,9 @@
                       </c:pt>
                       <c:pt idx="3">
                         <c:v>12.66</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>13.28</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2357,6 +2420,9 @@
                       <c:pt idx="3">
                         <c:v>44827</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>44830</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2383,6 +2449,9 @@
                       </c:pt>
                       <c:pt idx="3">
                         <c:v>96.999999999999545</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1424.9999999999995</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2456,6 +2525,9 @@
                       <c:pt idx="3">
                         <c:v>44827</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>44830</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2482,6 +2554,9 @@
                       </c:pt>
                       <c:pt idx="3">
                         <c:v>-19.870000000000005</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>13.28</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4774,7 +4849,7 @@
   <dimension ref="B1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4799,7 +4874,7 @@
         <v>44830</v>
       </c>
       <c r="C2" s="65">
-        <v>0.45624999999999999</v>
+        <v>0.68055555555555547</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4913,7 +4988,9 @@
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="13">
+        <v>3655.52</v>
+      </c>
       <c r="E10" s="10" t="s">
         <v>27</v>
       </c>
@@ -4929,7 +5006,9 @@
       <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="13"/>
+      <c r="C11" s="13">
+        <v>3674.37</v>
+      </c>
       <c r="E11" s="15" t="s">
         <v>58</v>
       </c>
@@ -4944,7 +5023,9 @@
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="13">
+        <v>3750.52</v>
+      </c>
       <c r="E12" s="16" t="s">
         <v>60</v>
       </c>
@@ -5122,7 +5203,7 @@
   <dimension ref="B1:N27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5185,14 +5266,14 @@
       </c>
       <c r="F3" s="78">
         <f>COUNTA(Tracker!K:K)-1</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3" s="80" t="s">
         <v>28</v>
       </c>
       <c r="H3" s="72">
         <f>C7/F3</f>
-        <v>24.249999999999886</v>
+        <v>284.99999999999989</v>
       </c>
       <c r="J3" s="22" t="s">
         <v>87</v>
@@ -5219,15 +5300,15 @@
       </c>
       <c r="F4" s="78">
         <f>COUNTIF(Tracker!J:J, "&gt;0")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4" s="81">
         <f>F4/F3</f>
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="H4" s="72">
         <f>(SUMIF(Tracker!H:H, "&gt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&gt;0", Tracker!H2))/F4*100</f>
-        <v>694.66666666666652</v>
+        <v>853.00000000000011</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>88</v>
@@ -5257,7 +5338,7 @@
       </c>
       <c r="G5" s="81">
         <f>F5/F3</f>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="H5" s="72">
         <f>IFERROR((SUMIF(Tracker!H:H, "&lt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&lt;0", Tracker!H2))/F5*100, 0)</f>
@@ -5286,14 +5367,14 @@
       </c>
       <c r="C7" s="72">
         <f>INDEX(Tracker!K:K, COUNTA(Tracker!K:K)+3,1)</f>
-        <v>96.999999999999545</v>
+        <v>1424.9999999999995</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>72</v>
       </c>
       <c r="F7" s="76">
         <f>C7/C4</f>
-        <v>4.0959983784913442E-3</v>
+        <v>6.0173172055156605E-2</v>
       </c>
       <c r="G7" s="76"/>
       <c r="J7" s="22" t="s">
@@ -5312,14 +5393,14 @@
       </c>
       <c r="C8" s="72">
         <f>INDEX(Tracker!L:L, COUNTA(Tracker!L:L)+3,1)</f>
-        <v>3483</v>
+        <v>4811</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>77</v>
       </c>
       <c r="F8" s="76">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>0.23755894099839581</v>
+        <v>20.048414315519199</v>
       </c>
       <c r="G8" s="76"/>
       <c r="J8" s="22" t="s">
@@ -5340,14 +5421,14 @@
       </c>
       <c r="C9" s="76">
         <f>C7/C8</f>
-        <v>2.7849554981337798E-2</v>
+        <v>0.29619621700270204</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>78</v>
       </c>
       <c r="F9" s="76">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>6.1992217001927807E-2</v>
+        <v>1.3626622065913998</v>
       </c>
       <c r="G9" s="76"/>
       <c r="J9" s="22" t="s">
@@ -5387,10 +5468,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C82D01-CC02-4066-B9D6-9DFF5A0A89C9}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5433,15 +5514,15 @@
       </c>
       <c r="C2" s="43">
         <f>Indicator!$C$10</f>
-        <v>0</v>
+        <v>3655.52</v>
       </c>
       <c r="D2" s="43">
         <f>Indicator!$C$11</f>
-        <v>0</v>
+        <v>3674.37</v>
       </c>
       <c r="E2" s="43">
         <f>Indicator!$C$12</f>
-        <v>0</v>
+        <v>3750.52</v>
       </c>
       <c r="F2" s="44">
         <f>Indicator!$C$13</f>
@@ -5453,11 +5534,11 @@
       </c>
       <c r="H2" s="59">
         <f>SUMIF(Trades!A:A,Tracker!A2,Trades!H:H)</f>
-        <v>9.01</v>
+        <v>13.28</v>
       </c>
       <c r="I2" s="60">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A2,  Trades!C:C, "STO")</f>
-        <v>9.01</v>
+        <v>13.28</v>
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="66"/>
@@ -5685,6 +5766,47 @@
         <v>119</v>
       </c>
     </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="58">
+        <v>44830</v>
+      </c>
+      <c r="B9" s="42">
+        <v>3682.72</v>
+      </c>
+      <c r="C9" s="42">
+        <v>3655.52</v>
+      </c>
+      <c r="D9" s="42">
+        <v>3674.37</v>
+      </c>
+      <c r="E9" s="42">
+        <v>3750.52</v>
+      </c>
+      <c r="F9" s="41">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="G9" s="41">
+        <v>0.28269041759555957</v>
+      </c>
+      <c r="H9" s="17">
+        <v>13.28</v>
+      </c>
+      <c r="I9" s="61">
+        <v>13.28</v>
+      </c>
+      <c r="J9" s="21">
+        <f>H9/I9</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="66">
+        <f>K8+H9*100</f>
+        <v>1424.9999999999995</v>
+      </c>
+      <c r="L9">
+        <f>I9*100+L8</f>
+        <v>4811</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5696,7 +5818,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:H15"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5704,7 +5826,7 @@
     <col min="1" max="1" width="9.7109375" style="48" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="49" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" style="102" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.140625" style="50" customWidth="1"/>
@@ -5783,7 +5905,7 @@
         <v>3</v>
       </c>
       <c r="J2" s="73">
-        <f t="shared" ref="J2:J4" si="1">-I2*H2</f>
+        <f t="shared" ref="J2:J4" si="1">-I2*G2</f>
         <v>-12.809999999999999</v>
       </c>
     </row>
@@ -5916,7 +6038,7 @@
         <v>3</v>
       </c>
       <c r="J6" s="73">
-        <f>-I6*H6</f>
+        <f t="shared" ref="J6:J9" si="2">-I6*G6</f>
         <v>-14.91</v>
       </c>
     </row>
@@ -5950,8 +6072,8 @@
         <v>3</v>
       </c>
       <c r="J7" s="73">
-        <f>-I7*H7</f>
-        <v>-14.22</v>
+        <f t="shared" si="2"/>
+        <v>-7.11</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -5984,7 +6106,7 @@
         <v>3</v>
       </c>
       <c r="J8" s="73">
-        <f>-I8*H8</f>
+        <f t="shared" si="2"/>
         <v>-19.41</v>
       </c>
     </row>
@@ -6018,7 +6140,7 @@
         <v>3</v>
       </c>
       <c r="J9" s="73">
-        <f>-I9*H9</f>
+        <f t="shared" si="2"/>
         <v>-11.91</v>
       </c>
     </row>
@@ -6042,7 +6164,7 @@
         <v>-12.43</v>
       </c>
       <c r="H10" s="51">
-        <f t="shared" ref="H10:H15" si="2">G10*F10</f>
+        <f t="shared" ref="H10:H15" si="3">G10*F10</f>
         <v>-12.43</v>
       </c>
     </row>
@@ -6066,7 +6188,7 @@
         <v>-20.100000000000001</v>
       </c>
       <c r="H11" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-20.100000000000001</v>
       </c>
     </row>
@@ -6093,14 +6215,14 @@
         <v>2.2200000000000002</v>
       </c>
       <c r="H12" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.2200000000000002</v>
       </c>
       <c r="I12" s="52">
         <v>3</v>
       </c>
       <c r="J12" s="73">
-        <f>-I12*H12</f>
+        <f>-I12*G12</f>
         <v>-6.66</v>
       </c>
     </row>
@@ -6109,32 +6231,32 @@
         <v>44830</v>
       </c>
       <c r="B13" s="49">
-        <v>742</v>
+        <v>942</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>45</v>
       </c>
       <c r="D13" s="69" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E13" s="102">
         <v>-0.15</v>
       </c>
       <c r="F13" s="31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="50">
         <v>4.2699999999999996</v>
       </c>
       <c r="H13" s="51">
-        <f t="shared" si="2"/>
-        <v>4.2699999999999996</v>
+        <f t="shared" si="3"/>
+        <v>8.5399999999999991</v>
       </c>
       <c r="I13" s="52">
         <v>3</v>
       </c>
       <c r="J13" s="73">
-        <f t="shared" ref="J13:J14" si="3">-I13*H13</f>
+        <f>-I13*G13</f>
         <v>-12.809999999999999</v>
       </c>
     </row>
@@ -6143,7 +6265,7 @@
         <v>44830</v>
       </c>
       <c r="B14" s="49">
-        <v>742</v>
+        <v>942</v>
       </c>
       <c r="C14" s="31" t="s">
         <v>45</v>
@@ -6161,14 +6283,14 @@
         <v>3.27</v>
       </c>
       <c r="H14" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.27</v>
       </c>
       <c r="I14" s="52">
         <v>3</v>
       </c>
       <c r="J14" s="73">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J14:J15" si="4">-I14*G14</f>
         <v>-9.81</v>
       </c>
     </row>
@@ -6177,7 +6299,7 @@
         <v>44830</v>
       </c>
       <c r="B15" s="49">
-        <v>815</v>
+        <v>1015</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>45</v>
@@ -6186,7 +6308,7 @@
         <v>122</v>
       </c>
       <c r="E15" s="102">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="F15" s="31">
         <v>1</v>
@@ -6195,14 +6317,14 @@
         <v>1.47</v>
       </c>
       <c r="H15" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.47</v>
       </c>
       <c r="I15" s="52">
         <v>3</v>
       </c>
       <c r="J15" s="73">
-        <f t="shared" ref="J15" si="4">-I15*H15</f>
+        <f t="shared" si="4"/>
         <v>-4.41</v>
       </c>
     </row>
@@ -6217,7 +6339,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6282,7 +6404,7 @@
         <v>44830</v>
       </c>
       <c r="B2" s="49">
-        <v>742</v>
+        <v>942</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>45</v>
@@ -6320,7 +6442,7 @@
         <v>44830</v>
       </c>
       <c r="B3" s="49">
-        <v>742</v>
+        <v>942</v>
       </c>
       <c r="C3" s="31" t="s">
         <v>45</v>
@@ -6359,7 +6481,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6424,7 +6546,7 @@
         <v>44830</v>
       </c>
       <c r="B2" s="49">
-        <v>742</v>
+        <v>942</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>45</v>
@@ -6462,7 +6584,7 @@
         <v>44830</v>
       </c>
       <c r="B3" s="49">
-        <v>815</v>
+        <v>1015</v>
       </c>
       <c r="C3" s="31" t="s">
         <v>45</v>
@@ -6471,7 +6593,7 @@
         <v>122</v>
       </c>
       <c r="E3" s="102">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="F3" s="31">
         <v>1</v>

</xml_diff>

<commit_message>
Market Open Sep27/2022 - Update 0DTE Experiment.xlsx
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BBA2AC-BB1C-4CE4-B9FC-CB07196DC7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAB79DF-178F-464C-99AA-646CDA6AAF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27270" yWindow="5520" windowWidth="23580" windowHeight="14010" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
+    <workbookView xWindow="25860" yWindow="6480" windowWidth="23580" windowHeight="14010" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="127">
   <si>
     <t>SPX Open</t>
   </si>
@@ -80,9 +80,6 @@
     <t>SPX Prior 2D MA</t>
   </si>
   <si>
-    <t>0 Day - Price Expectations</t>
-  </si>
-  <si>
     <t>2 Day - DTE Price Expectations</t>
   </si>
   <si>
@@ -411,6 +408,18 @@
   </si>
   <si>
     <t>Sep26 3650/3625 Bull Put @ -4.30</t>
+  </si>
+  <si>
+    <t>1 Day - Price Expectations</t>
+  </si>
+  <si>
+    <t>Sep27 3655/3630 Bull Put @ -3.40</t>
+  </si>
+  <si>
+    <t>Sep27 3750/3775 Bear Call @ -3.90</t>
+  </si>
+  <si>
+    <t>Sep27 3730/3755 Bear Call @ -3.00</t>
   </si>
 </sst>
 </file>
@@ -584,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -809,6 +818,9 @@
     </xf>
     <xf numFmtId="39" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4849,7 +4861,7 @@
   <dimension ref="B1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4866,15 +4878,15 @@
         <v>2</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="20">
-        <v>44830</v>
+        <v>44831</v>
       </c>
       <c r="C2" s="65">
-        <v>0.68055555555555547</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4882,19 +4894,19 @@
     </row>
     <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="34" t="s">
-        <v>22</v>
-      </c>
       <c r="G4" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="22"/>
     </row>
@@ -4903,14 +4915,14 @@
         <v>3</v>
       </c>
       <c r="C5" s="12">
-        <v>3727.14</v>
+        <v>3682.72</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="27">
         <f>(C9-C18)/(C17-C18)</f>
-        <v>0.41674616372904594</v>
+        <v>0.74502479403446709</v>
       </c>
       <c r="G5" s="25">
         <v>0.4</v>
@@ -4922,14 +4934,14 @@
         <v>4</v>
       </c>
       <c r="C6" s="13">
-        <v>3693.49</v>
+        <v>3655.52</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="27">
         <f>(C9-C23)/(C22-C23)</f>
-        <v>0.26688600747623897</v>
+        <v>0.56728667959101653</v>
       </c>
       <c r="G6" s="25">
         <v>0.33</v>
@@ -4941,14 +4953,14 @@
         <v>12</v>
       </c>
       <c r="C7" s="13">
-        <v>3725.74</v>
+        <v>3674.37</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7" s="28">
         <f>(C9-C28)/(C27-C28)</f>
-        <v>0.1034058134695641</v>
+        <v>0.27675799239404836</v>
       </c>
       <c r="G7" s="26">
         <v>0.27</v>
@@ -4960,17 +4972,17 @@
         <v>10</v>
       </c>
       <c r="C8" s="13">
-        <v>3799.45</v>
+        <v>3750.52</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="29">
         <f>F5*G5+F6*G6+F7*G7</f>
-        <v>0.28269041759555957</v>
+        <v>0.55993917982521535</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" s="17"/>
     </row>
@@ -4979,7 +4991,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="12">
-        <v>3682.72</v>
+        <v>3686.44</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -4988,32 +5000,28 @@
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13">
-        <v>3655.52</v>
-      </c>
+      <c r="C10" s="13"/>
       <c r="E10" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="37" t="s">
         <v>23</v>
-      </c>
-      <c r="G10" s="37" t="s">
-        <v>24</v>
       </c>
       <c r="K10" s="40"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="13">
-        <v>3674.37</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C11" s="13"/>
       <c r="E11" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11" s="30">
         <v>-0.21</v>
@@ -5023,11 +5031,9 @@
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13">
-        <v>3750.52</v>
-      </c>
+      <c r="C12" s="13"/>
       <c r="E12" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F12" s="31">
         <v>0.09</v>
@@ -5041,10 +5047,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="14">
-        <v>0.27800000000000002</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" s="31">
         <v>0.12</v>
@@ -5055,7 +5061,7 @@
     </row>
     <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E14" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" s="31">
         <v>0.15</v>
@@ -5066,11 +5072,11 @@
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>13</v>
+        <v>123</v>
       </c>
       <c r="C15" s="9"/>
       <c r="E15" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F15" s="31">
         <v>0.15</v>
@@ -5084,11 +5090,11 @@
         <v>9</v>
       </c>
       <c r="C16" s="4">
-        <f>C6*C$13*252^-0.5</f>
-        <v>64.68170406555474</v>
+        <f>C6*C$13*SQRT((24/24)/252)</f>
+        <v>63.095655527110871</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F16" s="31">
         <v>0.18</v>
@@ -5103,16 +5109,16 @@
       </c>
       <c r="C17" s="4">
         <f>C6+C16</f>
-        <v>3758.1717040655544</v>
+        <v>3718.6156555271109</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F17" s="33">
         <v>0.21</v>
       </c>
       <c r="G17" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5121,13 +5127,13 @@
       </c>
       <c r="C18" s="6">
         <f>C6-C16</f>
-        <v>3628.8082959344451</v>
+        <v>3592.4243444728891</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="9"/>
     </row>
@@ -5137,7 +5143,7 @@
       </c>
       <c r="C21" s="4">
         <f>C7*C$13*(2/252)^0.5</f>
-        <v>92.272453348365772</v>
+        <v>89.690857636045607</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -5146,7 +5152,7 @@
       </c>
       <c r="C22" s="4">
         <f>C7+C21</f>
-        <v>3818.0124533483654</v>
+        <v>3764.0608576360455</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5155,13 +5161,13 @@
       </c>
       <c r="C23" s="6">
         <f>C7-C21</f>
-        <v>3633.4675466516342</v>
+        <v>3584.6791423639543</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="9"/>
     </row>
@@ -5171,7 +5177,7 @@
       </c>
       <c r="C26" s="4">
         <f>C17*C$13*(5/252)^0.5</f>
-        <v>147.1655459970313</v>
+        <v>143.52137549557563</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -5180,7 +5186,7 @@
       </c>
       <c r="C27" s="4">
         <f>C8+C26</f>
-        <v>3946.6155459970309</v>
+        <v>3894.0413754955757</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5189,7 +5195,7 @@
       </c>
       <c r="C28" s="6">
         <f>C8-C26</f>
-        <v>3652.2844540029687</v>
+        <v>3606.9986245044242</v>
       </c>
     </row>
   </sheetData>
@@ -5203,7 +5209,7 @@
   <dimension ref="B1:N27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5229,24 +5235,24 @@
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="17">
         <v>2022</v>
       </c>
       <c r="F2" s="84" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="71" t="s">
         <v>84</v>
-      </c>
-      <c r="G2" s="84" t="s">
-        <v>86</v>
-      </c>
-      <c r="H2" s="71" t="s">
-        <v>85</v>
       </c>
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
       <c r="K2" s="70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L2" s="71" t="s">
         <v>6</v>
@@ -5256,27 +5262,27 @@
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="75">
         <v>44824</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" s="78">
         <f>COUNTA(Tracker!K:K)-1</f>
         <v>5</v>
       </c>
       <c r="G3" s="80" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="72">
         <f>C7/F3</f>
         <v>284.99999999999989</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K3" s="68">
         <f>2*1.25%</f>
@@ -5290,13 +5296,13 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="72">
         <v>23681.65</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4" s="78">
         <f>COUNTIF(Tracker!J:J, "&gt;0")</f>
@@ -5311,7 +5317,7 @@
         <v>853.00000000000011</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K4" s="68">
         <f>-3.75%</f>
@@ -5324,13 +5330,13 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="72">
         <v>23681.65</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="78">
         <f>COUNTIF(Tracker!J:J, "&lt;0")</f>
@@ -5345,7 +5351,7 @@
         <v>-1987.0000000000005</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K5" s="68">
         <f>+K3+K4</f>
@@ -5363,14 +5369,14 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="72">
         <f>INDEX(Tracker!K:K, COUNTA(Tracker!K:K)+3,1)</f>
         <v>1424.9999999999995</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="76">
         <f>C7/C4</f>
@@ -5378,7 +5384,7 @@
       </c>
       <c r="G7" s="76"/>
       <c r="J7" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K7" s="82">
         <v>20</v>
@@ -5389,22 +5395,22 @@
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="72">
         <f>INDEX(Tracker!L:L, COUNTA(Tracker!L:L)+3,1)</f>
         <v>4811</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F8" s="76">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>20.048414315519199</v>
+        <v>13.381923052175734</v>
       </c>
       <c r="G8" s="76"/>
       <c r="J8" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K8" s="82">
         <f>FLOOR(MROUND(C4/1000, 5)/20, 1)</f>
@@ -5417,22 +5423,22 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="76">
         <f>C7/C8</f>
         <v>0.29619621700270204</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" s="76">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>1.3626622065913998</v>
+        <v>1.1219074130035542</v>
       </c>
       <c r="G9" s="76"/>
       <c r="J9" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K9" s="83">
         <f>K7*K8*100*2</f>
@@ -5471,7 +5477,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5491,7 +5497,7 @@
   <sheetData>
     <row r="1" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="54"/>
       <c r="C1" s="54"/>
@@ -5506,39 +5512,39 @@
     <row r="2" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="58">
         <f>Indicator!B2</f>
-        <v>44830</v>
+        <v>44831</v>
       </c>
       <c r="B2" s="43">
         <f>Indicator!$C$9</f>
-        <v>3682.72</v>
+        <v>3686.44</v>
       </c>
       <c r="C2" s="43">
         <f>Indicator!$C$10</f>
-        <v>3655.52</v>
+        <v>0</v>
       </c>
       <c r="D2" s="43">
         <f>Indicator!$C$11</f>
-        <v>3674.37</v>
+        <v>0</v>
       </c>
       <c r="E2" s="43">
         <f>Indicator!$C$12</f>
-        <v>3750.52</v>
+        <v>0</v>
       </c>
       <c r="F2" s="44">
         <f>Indicator!$C$13</f>
-        <v>0.27800000000000002</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="G2" s="44">
         <f>Indicator!$F$8</f>
-        <v>0.28269041759555957</v>
+        <v>0.55993917982521535</v>
       </c>
       <c r="H2" s="59">
         <f>SUMIF(Trades!A:A,Tracker!A2,Trades!H:H)</f>
-        <v>13.28</v>
+        <v>13.58</v>
       </c>
       <c r="I2" s="60">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A2,  Trades!C:C, "STO")</f>
-        <v>13.28</v>
+        <v>13.58</v>
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="66"/>
@@ -5557,43 +5563,43 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="E4" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="F4" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="G4" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="H4" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="47" t="s">
-        <v>43</v>
-      </c>
       <c r="I4" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="J4" s="47" t="s">
+      <c r="L4" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="74" t="s">
         <v>48</v>
-      </c>
-      <c r="K4" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="L4" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="M4" s="74" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -5678,7 +5684,7 @@
         <v>1246</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -5763,7 +5769,7 @@
         <v>3483</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -5815,10 +5821,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5839,40 +5845,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="85" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="D1" s="87" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="101" t="s">
+      <c r="F1" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="G1" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="88" t="s">
-        <v>37</v>
-      </c>
       <c r="H1" s="89" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I1" s="90" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J1" s="91" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K1" s="90" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="91" t="s">
         <v>56</v>
-      </c>
-      <c r="L1" s="91" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -5883,10 +5889,10 @@
         <v>949</v>
       </c>
       <c r="C2" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>45</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>46</v>
       </c>
       <c r="E2" s="102">
         <v>-0.15</v>
@@ -5917,10 +5923,10 @@
         <v>950</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="102">
         <v>0.09</v>
@@ -5951,10 +5957,10 @@
         <v>944</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="102">
         <v>-0.15</v>
@@ -5992,10 +5998,10 @@
         <v>243</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" s="31">
         <v>1</v>
@@ -6016,10 +6022,10 @@
         <v>937</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" s="102">
         <v>-0.16</v>
@@ -6050,10 +6056,10 @@
         <v>946</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="69" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E7" s="102">
         <v>0.13</v>
@@ -6084,10 +6090,10 @@
         <v>936</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="69" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E8" s="102">
         <v>-0.3</v>
@@ -6118,10 +6124,10 @@
         <v>949</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="69" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E9" s="102">
         <v>-0.19</v>
@@ -6152,10 +6158,10 @@
         <v>240</v>
       </c>
       <c r="C10" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="69" t="s">
         <v>116</v>
-      </c>
-      <c r="D10" s="69" t="s">
-        <v>117</v>
       </c>
       <c r="F10" s="31">
         <v>1</v>
@@ -6164,7 +6170,7 @@
         <v>-12.43</v>
       </c>
       <c r="H10" s="51">
-        <f t="shared" ref="H10:H15" si="3">G10*F10</f>
+        <f t="shared" ref="H10:H18" si="3">G10*F10</f>
         <v>-12.43</v>
       </c>
     </row>
@@ -6176,10 +6182,10 @@
         <v>255</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D11" s="69" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F11" s="31">
         <v>1</v>
@@ -6200,10 +6206,10 @@
         <v>311</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="69" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E12" s="102">
         <v>-0.19</v>
@@ -6234,10 +6240,10 @@
         <v>942</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" s="69" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E13" s="102">
         <v>-0.15</v>
@@ -6268,10 +6274,10 @@
         <v>942</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="69" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E14" s="102">
         <v>0.15</v>
@@ -6302,10 +6308,10 @@
         <v>1015</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="69" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E15" s="102">
         <v>0.11</v>
@@ -6326,6 +6332,108 @@
       <c r="J15" s="73">
         <f t="shared" si="4"/>
         <v>-4.41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="48">
+        <v>44831</v>
+      </c>
+      <c r="B16" s="49">
+        <v>950</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="103" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" s="102">
+        <v>-0.16</v>
+      </c>
+      <c r="F16" s="31">
+        <v>2</v>
+      </c>
+      <c r="G16" s="50">
+        <v>3.37</v>
+      </c>
+      <c r="H16" s="51">
+        <f t="shared" si="3"/>
+        <v>6.74</v>
+      </c>
+      <c r="I16" s="52">
+        <v>3</v>
+      </c>
+      <c r="J16" s="73">
+        <f t="shared" ref="J16:J18" si="5">-I16*G16</f>
+        <v>-10.11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="48">
+        <v>44831</v>
+      </c>
+      <c r="B17" s="49">
+        <v>940</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="103" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="102">
+        <v>0.17</v>
+      </c>
+      <c r="F17" s="31">
+        <v>1</v>
+      </c>
+      <c r="G17" s="50">
+        <v>3.87</v>
+      </c>
+      <c r="H17" s="51">
+        <f t="shared" si="3"/>
+        <v>3.87</v>
+      </c>
+      <c r="I17" s="52">
+        <v>3</v>
+      </c>
+      <c r="J17" s="73">
+        <f t="shared" si="5"/>
+        <v>-11.61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="48">
+        <v>44831</v>
+      </c>
+      <c r="B18" s="49">
+        <v>1006</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="103" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="102">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F18" s="31">
+        <v>1</v>
+      </c>
+      <c r="G18" s="50">
+        <v>2.97</v>
+      </c>
+      <c r="H18" s="51">
+        <f t="shared" si="3"/>
+        <v>2.97</v>
+      </c>
+      <c r="I18" s="52">
+        <v>3</v>
+      </c>
+      <c r="J18" s="73">
+        <f t="shared" si="5"/>
+        <v>-8.91</v>
       </c>
     </row>
   </sheetData>
@@ -6336,10 +6444,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE4BC4F-EB6D-4F7C-A4AB-32C246F0D899}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6347,7 +6455,7 @@
     <col min="1" max="1" width="9.7109375" style="48" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="49" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" style="102" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.140625" style="50" customWidth="1"/>
@@ -6360,43 +6468,43 @@
   <sheetData>
     <row r="1" spans="1:14" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="85" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="D1" s="87" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="101" t="s">
+      <c r="F1" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="G1" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="88" t="s">
-        <v>37</v>
-      </c>
       <c r="H1" s="89" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I1" s="90" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J1" s="91" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K1" s="90" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="91" t="s">
-        <v>57</v>
-      </c>
       <c r="N1" s="99" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -6407,10 +6515,10 @@
         <v>942</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="69" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E2" s="102">
         <v>-0.15</v>
@@ -6422,7 +6530,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="51">
-        <f t="shared" ref="H2:H3" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H5" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="52">
@@ -6434,7 +6542,7 @@
       </c>
       <c r="N2" s="73">
         <f>SUM(H:H)</f>
-        <v>7.5399999999999991</v>
+        <v>14.33</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -6445,10 +6553,10 @@
         <v>942</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E3" s="102">
         <v>0.15</v>
@@ -6469,6 +6577,74 @@
       <c r="J3" s="73">
         <f t="shared" si="1"/>
         <v>-9.81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="48">
+        <v>44831</v>
+      </c>
+      <c r="B4" s="49">
+        <v>950</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="103" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="102">
+        <v>-0.16</v>
+      </c>
+      <c r="F4" s="31">
+        <v>1</v>
+      </c>
+      <c r="G4" s="50">
+        <v>3.37</v>
+      </c>
+      <c r="H4" s="51">
+        <f t="shared" si="0"/>
+        <v>3.37</v>
+      </c>
+      <c r="I4" s="52">
+        <v>3</v>
+      </c>
+      <c r="J4" s="73">
+        <f t="shared" ref="J4:J5" si="2">-I4*G4</f>
+        <v>-10.11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="48">
+        <v>44831</v>
+      </c>
+      <c r="B5" s="49">
+        <v>940</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="103" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="102">
+        <v>0.17</v>
+      </c>
+      <c r="F5" s="31">
+        <v>1</v>
+      </c>
+      <c r="G5" s="50">
+        <v>3.42</v>
+      </c>
+      <c r="H5" s="51">
+        <f t="shared" si="0"/>
+        <v>3.42</v>
+      </c>
+      <c r="I5" s="52">
+        <v>3</v>
+      </c>
+      <c r="J5" s="73">
+        <f t="shared" si="2"/>
+        <v>-10.26</v>
       </c>
     </row>
   </sheetData>
@@ -6478,10 +6654,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5E4B5F-C3CE-4821-8081-9385439A4F7E}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6489,7 +6665,7 @@
     <col min="1" max="1" width="9.7109375" style="48" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="49" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" style="102" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.140625" style="50" customWidth="1"/>
@@ -6502,43 +6678,43 @@
   <sheetData>
     <row r="1" spans="1:14" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="85" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="D1" s="87" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="101" t="s">
+      <c r="F1" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="G1" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="88" t="s">
-        <v>37</v>
-      </c>
       <c r="H1" s="89" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I1" s="90" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J1" s="91" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K1" s="90" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="91" t="s">
-        <v>57</v>
-      </c>
       <c r="N1" s="99" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -6549,10 +6725,10 @@
         <v>942</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="69" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E2" s="102">
         <v>-0.15</v>
@@ -6564,7 +6740,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="51">
-        <f t="shared" ref="H2:H3" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H5" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="52">
@@ -6576,7 +6752,7 @@
       </c>
       <c r="N2" s="73">
         <f>SUM(H:H)</f>
-        <v>5.7399999999999993</v>
+        <v>12.53</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -6587,10 +6763,10 @@
         <v>1015</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E3" s="102">
         <v>0.11</v>
@@ -6611,6 +6787,74 @@
       <c r="J3" s="73">
         <f t="shared" ref="J3" si="2">-I3*H3</f>
         <v>-4.41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="48">
+        <v>44831</v>
+      </c>
+      <c r="B4" s="49">
+        <v>950</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="103" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="102">
+        <v>-0.16</v>
+      </c>
+      <c r="F4" s="31">
+        <v>1</v>
+      </c>
+      <c r="G4" s="50">
+        <v>3.37</v>
+      </c>
+      <c r="H4" s="51">
+        <f t="shared" si="0"/>
+        <v>3.37</v>
+      </c>
+      <c r="I4" s="52">
+        <v>3</v>
+      </c>
+      <c r="J4" s="73">
+        <f t="shared" ref="J4:J5" si="3">-I4*G4</f>
+        <v>-10.11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="48">
+        <v>44831</v>
+      </c>
+      <c r="B5" s="49">
+        <v>1006</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="103" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="102">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F5" s="31">
+        <v>1</v>
+      </c>
+      <c r="G5" s="50">
+        <v>3.42</v>
+      </c>
+      <c r="H5" s="51">
+        <f t="shared" si="0"/>
+        <v>3.42</v>
+      </c>
+      <c r="I5" s="52">
+        <v>3</v>
+      </c>
+      <c r="J5" s="73">
+        <f t="shared" si="3"/>
+        <v>-10.26</v>
       </c>
     </row>
   </sheetData>
@@ -6623,7 +6867,7 @@
   <dimension ref="B2:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6634,44 +6878,44 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="92"/>
       <c r="C6" s="92" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="92" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="92" t="s">
+      <c r="E6" s="92" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="92" t="s">
+      <c r="F6" s="92" t="s">
         <v>97</v>
       </c>
-      <c r="F6" s="92" t="s">
+      <c r="G6" s="92" t="s">
         <v>98</v>
       </c>
-      <c r="G6" s="92" t="s">
-        <v>99</v>
-      </c>
       <c r="H6" s="92" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I6" s="92"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="92" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" s="93">
         <v>-1.5</v>
@@ -6694,7 +6938,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="92" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8">
         <v>-75</v>
@@ -6717,7 +6961,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="92" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" s="94">
         <v>-0.43319999999999997</v>
@@ -6740,50 +6984,50 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="92" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="95">
-        <v>-250</v>
+        <v>-350</v>
       </c>
       <c r="D10" s="95">
         <v>0</v>
       </c>
       <c r="E10" s="95">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="F10" s="95">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="G10" s="95">
         <v>0</v>
       </c>
       <c r="H10" s="95">
-        <v>-250</v>
+        <v>-350</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="92" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="99" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="99" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="99" t="s">
         <v>103</v>
-      </c>
-      <c r="C13" s="99" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="99" t="s">
-        <v>102</v>
-      </c>
-      <c r="E13" s="99" t="s">
-        <v>104</v>
       </c>
       <c r="F13" s="99"/>
       <c r="G13" s="92"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="96">
         <f>E10</f>
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="D14" s="94">
         <f>F9-E9</f>
@@ -6791,17 +7035,17 @@
       </c>
       <c r="E14" s="96">
         <f>C14*D14</f>
-        <v>341.3</v>
+        <v>238.91</v>
       </c>
       <c r="F14" s="94"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15" s="96">
-        <f>C10</f>
-        <v>-250</v>
+        <f>C10*1.05</f>
+        <v>-367.5</v>
       </c>
       <c r="D15" s="94">
         <f>100%+C9-H9</f>
@@ -6809,13 +7053,13 @@
       </c>
       <c r="E15" s="96">
         <f>D15*C15</f>
-        <v>-33.4</v>
+        <v>-49.097999999999999</v>
       </c>
       <c r="F15" s="94"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" s="96">
         <v>0</v>
@@ -6832,10 +7076,11 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" s="96">
-        <v>-250</v>
+        <f>C15</f>
+        <v>-367.5</v>
       </c>
       <c r="D17" s="94">
         <f>(H9-G9)*2</f>
@@ -6843,7 +7088,7 @@
       </c>
       <c r="E17" s="96">
         <f t="shared" si="0"/>
-        <v>-34.449999999999982</v>
+        <v>-50.641499999999972</v>
       </c>
       <c r="F17" s="94"/>
     </row>
@@ -6854,67 +7099,67 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="92" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="100" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="100" t="s">
+      <c r="D20" s="100" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="100" t="s">
+      <c r="E20" s="100" t="s">
         <v>111</v>
-      </c>
-      <c r="E20" s="100" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="92" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C21" s="96">
         <f>SUM(E14:E17)</f>
-        <v>273.45000000000005</v>
+        <v>139.17050000000003</v>
       </c>
       <c r="D21" s="97">
         <f>C21*21</f>
-        <v>5742.4500000000007</v>
+        <v>2922.5805000000005</v>
       </c>
       <c r="E21" s="96">
         <f>C21*252</f>
-        <v>68909.400000000009</v>
+        <v>35070.966000000008</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="92" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="96">
         <f>E10</f>
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="D22" s="97">
         <f>C22*21</f>
-        <v>10500</v>
+        <v>7350</v>
       </c>
       <c r="E22" s="96">
         <f>C22*252</f>
-        <v>126000</v>
+        <v>88200</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="92" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" s="98">
         <f>C21/C22</f>
-        <v>0.54690000000000005</v>
+        <v>0.39763000000000009</v>
       </c>
       <c r="D23" s="98">
         <f>D21/D22</f>
-        <v>0.54690000000000005</v>
+        <v>0.39763000000000004</v>
       </c>
       <c r="E23" s="98">
         <f>E21/E22</f>
-        <v>0.54690000000000005</v>
+        <v>0.39763000000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Market Close Sep27/2022 - Update 0DTE Experiment.xlsx
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAB79DF-178F-464C-99AA-646CDA6AAF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34D7DF3-33AB-4631-949E-C57A614193B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25860" yWindow="6480" windowWidth="23580" windowHeight="14010" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
+    <workbookView xWindow="11640" yWindow="4605" windowWidth="23580" windowHeight="14010" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="130">
   <si>
     <t>SPX Open</t>
   </si>
@@ -420,6 +420,15 @@
   </si>
   <si>
     <t>Sep27 3730/3755 Bear Call @ -3.00</t>
+  </si>
+  <si>
+    <t>Sep27 3655/3630 Bull Put @ -14.1</t>
+  </si>
+  <si>
+    <t>Sep27 3660/3685 Bear Call @ -4.55</t>
+  </si>
+  <si>
+    <t>Triggered around 3650</t>
   </si>
 </sst>
 </file>
@@ -593,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -822,6 +831,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,6 +948,9 @@
                 <c:pt idx="4">
                   <c:v>44830</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>44831</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -959,6 +974,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1424.9999999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>866.99999999999955</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1043,6 +1061,9 @@
                       <c:pt idx="4">
                         <c:v>44830</c:v>
                       </c:pt>
+                      <c:pt idx="5">
+                        <c:v>44831</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1072,6 +1093,9 @@
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>13.28</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-5.58</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1144,6 +1168,9 @@
                       <c:pt idx="4">
                         <c:v>44830</c:v>
                       </c:pt>
+                      <c:pt idx="5">
+                        <c:v>44831</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1173,6 +1200,9 @@
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>13.28</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>22.619999999999997</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1245,6 +1275,9 @@
                       <c:pt idx="4">
                         <c:v>44830</c:v>
                       </c:pt>
+                      <c:pt idx="5">
+                        <c:v>44831</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1274,6 +1307,9 @@
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-0.24668435013262602</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1561,6 +1597,9 @@
                 <c:pt idx="4">
                   <c:v>44830</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>44831</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1585,6 +1624,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>13.28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.619999999999997</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -1668,6 +1710,9 @@
                       <c:pt idx="4">
                         <c:v>44830</c:v>
                       </c:pt>
+                      <c:pt idx="5">
+                        <c:v>44831</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1697,6 +1742,9 @@
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-0.24668435013262602</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1766,6 +1814,9 @@
                       <c:pt idx="4">
                         <c:v>44830</c:v>
                       </c:pt>
+                      <c:pt idx="5">
+                        <c:v>44831</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1795,6 +1846,9 @@
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1424.9999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>866.99999999999955</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1850,6 +1904,9 @@
                 <c:pt idx="4">
                   <c:v>44830</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>44831</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1874,6 +1931,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>13.28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.58</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2244,6 +2304,9 @@
                 <c:pt idx="4">
                   <c:v>44830</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>44831</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -2268,6 +2331,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.24668435013262602</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2337,6 +2403,9 @@
                       <c:pt idx="4">
                         <c:v>44830</c:v>
                       </c:pt>
+                      <c:pt idx="5">
+                        <c:v>44831</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2366,6 +2435,9 @@
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>13.28</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>22.619999999999997</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2435,6 +2507,9 @@
                       <c:pt idx="4">
                         <c:v>44830</c:v>
                       </c:pt>
+                      <c:pt idx="5">
+                        <c:v>44831</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2464,6 +2539,9 @@
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1424.9999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>866.99999999999955</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2540,6 +2618,9 @@
                       <c:pt idx="4">
                         <c:v>44830</c:v>
                       </c:pt>
+                      <c:pt idx="5">
+                        <c:v>44831</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2569,6 +2650,9 @@
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>13.28</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-5.58</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4861,7 +4945,7 @@
   <dimension ref="B1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4886,7 +4970,7 @@
         <v>44831</v>
       </c>
       <c r="C2" s="65">
-        <v>0.4375</v>
+        <v>0.90694444444444444</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5000,7 +5084,9 @@
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="13">
+        <v>3647.29</v>
+      </c>
       <c r="E10" s="10" t="s">
         <v>26</v>
       </c>
@@ -5016,7 +5102,9 @@
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="13"/>
+      <c r="C11" s="13">
+        <v>3651.17</v>
+      </c>
       <c r="E11" s="15" t="s">
         <v>57</v>
       </c>
@@ -5031,7 +5119,9 @@
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="13">
+        <v>3708.7</v>
+      </c>
       <c r="E12" s="16" t="s">
         <v>59</v>
       </c>
@@ -5272,14 +5362,14 @@
       </c>
       <c r="F3" s="78">
         <f>COUNTA(Tracker!K:K)-1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3" s="80" t="s">
         <v>27</v>
       </c>
       <c r="H3" s="72">
         <f>C7/F3</f>
-        <v>284.99999999999989</v>
+        <v>144.49999999999991</v>
       </c>
       <c r="J3" s="22" t="s">
         <v>86</v>
@@ -5310,11 +5400,11 @@
       </c>
       <c r="G4" s="81">
         <f>F4/F3</f>
-        <v>0.8</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="H4" s="72">
         <f>(SUMIF(Tracker!H:H, "&gt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&gt;0", Tracker!H2))/F4*100</f>
-        <v>853.00000000000011</v>
+        <v>852.99999999999989</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>87</v>
@@ -5340,15 +5430,15 @@
       </c>
       <c r="F5" s="78">
         <f>COUNTIF(Tracker!J:J, "&lt;0")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="81">
         <f>F5/F3</f>
-        <v>0.2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H5" s="72">
         <f>IFERROR((SUMIF(Tracker!H:H, "&lt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&lt;0", Tracker!H2))/F5*100, 0)</f>
-        <v>-1987.0000000000005</v>
+        <v>-1272.5000000000002</v>
       </c>
       <c r="J5" s="22" t="s">
         <v>88</v>
@@ -5373,14 +5463,14 @@
       </c>
       <c r="C7" s="72">
         <f>INDEX(Tracker!K:K, COUNTA(Tracker!K:K)+3,1)</f>
-        <v>1424.9999999999995</v>
+        <v>866.99999999999955</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>71</v>
       </c>
       <c r="F7" s="76">
         <f>C7/C4</f>
-        <v>6.0173172055156605E-2</v>
+        <v>3.6610624681979488E-2</v>
       </c>
       <c r="G7" s="76"/>
       <c r="J7" s="22" t="s">
@@ -5399,14 +5489,14 @@
       </c>
       <c r="C8" s="72">
         <f>INDEX(Tracker!L:L, COUNTA(Tracker!L:L)+3,1)</f>
-        <v>4811</v>
+        <v>7073</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>76</v>
       </c>
       <c r="F8" s="76">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>13.381923052175734</v>
+        <v>4.157797603196757</v>
       </c>
       <c r="G8" s="76"/>
       <c r="J8" s="22" t="s">
@@ -5427,14 +5517,14 @@
       </c>
       <c r="C9" s="76">
         <f>C7/C8</f>
-        <v>0.29619621700270204</v>
+        <v>0.12257882086808986</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>77</v>
       </c>
       <c r="F9" s="76">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>1.1219074130035542</v>
+        <v>0.58873538507272904</v>
       </c>
       <c r="G9" s="76"/>
       <c r="J9" s="22" t="s">
@@ -5474,10 +5564,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C82D01-CC02-4066-B9D6-9DFF5A0A89C9}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5520,15 +5610,15 @@
       </c>
       <c r="C2" s="43">
         <f>Indicator!$C$10</f>
-        <v>0</v>
+        <v>3647.29</v>
       </c>
       <c r="D2" s="43">
         <f>Indicator!$C$11</f>
-        <v>0</v>
+        <v>3651.17</v>
       </c>
       <c r="E2" s="43">
         <f>Indicator!$C$12</f>
-        <v>0</v>
+        <v>3708.7</v>
       </c>
       <c r="F2" s="44">
         <f>Indicator!$C$13</f>
@@ -5540,11 +5630,11 @@
       </c>
       <c r="H2" s="59">
         <f>SUMIF(Trades!A:A,Tracker!A2,Trades!H:H)</f>
-        <v>13.58</v>
+        <v>-5.58</v>
       </c>
       <c r="I2" s="60">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A2,  Trades!C:C, "STO")</f>
-        <v>13.58</v>
+        <v>22.619999999999997</v>
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="66"/>
@@ -5631,7 +5721,7 @@
         <v>7.2899999999999991</v>
       </c>
       <c r="J5" s="21">
-        <f>H5/I5</f>
+        <f t="shared" ref="J5:J10" si="0">H5/I5</f>
         <v>1</v>
       </c>
       <c r="K5" s="66">
@@ -5672,7 +5762,7 @@
         <v>5.17</v>
       </c>
       <c r="J6" s="21">
-        <f>H6/I6</f>
+        <f t="shared" si="0"/>
         <v>0.74274661508704065</v>
       </c>
       <c r="K6" s="66">
@@ -5716,7 +5806,7 @@
         <v>9.7100000000000009</v>
       </c>
       <c r="J7" s="21">
-        <f>H7/I7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K7" s="66">
@@ -5757,7 +5847,7 @@
         <v>12.66</v>
       </c>
       <c r="J8" s="21">
-        <f>H8/I8</f>
+        <f t="shared" si="0"/>
         <v>-1.5695102685624016</v>
       </c>
       <c r="K8" s="66">
@@ -5801,7 +5891,7 @@
         <v>13.28</v>
       </c>
       <c r="J9" s="21">
-        <f>H9/I9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K9" s="66">
@@ -5811,6 +5901,50 @@
       <c r="L9">
         <f>I9*100+L8</f>
         <v>4811</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="58">
+        <v>44831</v>
+      </c>
+      <c r="B10" s="42">
+        <v>3686.44</v>
+      </c>
+      <c r="C10" s="42">
+        <v>3647.29</v>
+      </c>
+      <c r="D10" s="42">
+        <v>3651.17</v>
+      </c>
+      <c r="E10" s="42">
+        <v>3708.7</v>
+      </c>
+      <c r="F10" s="41">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="G10" s="41">
+        <v>0.55993917982521535</v>
+      </c>
+      <c r="H10" s="17">
+        <v>-5.58</v>
+      </c>
+      <c r="I10" s="61">
+        <v>22.619999999999997</v>
+      </c>
+      <c r="J10" s="21">
+        <f t="shared" si="0"/>
+        <v>-0.24668435013262602</v>
+      </c>
+      <c r="K10" s="66">
+        <f>K9+H10*100</f>
+        <v>866.99999999999955</v>
+      </c>
+      <c r="L10">
+        <f>I10*100+L9</f>
+        <v>7073</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -5821,10 +5955,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6436,6 +6570,57 @@
         <v>-8.91</v>
       </c>
     </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="48">
+        <v>44831</v>
+      </c>
+      <c r="B19" s="49">
+        <v>1218</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="103" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="31">
+        <v>2</v>
+      </c>
+      <c r="G19" s="50">
+        <v>-14.1</v>
+      </c>
+      <c r="H19" s="51">
+        <f t="shared" ref="H19:H20" si="6">G19*F19</f>
+        <v>-28.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="48">
+        <v>44831</v>
+      </c>
+      <c r="B20" s="49">
+        <v>1224</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="104" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" s="102">
+        <v>0.15</v>
+      </c>
+      <c r="F20" s="31">
+        <v>2</v>
+      </c>
+      <c r="G20" s="50">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="H20" s="51">
+        <f t="shared" si="6"/>
+        <v>9.0399999999999991</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6444,10 +6629,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE4BC4F-EB6D-4F7C-A4AB-32C246F0D899}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6530,7 +6715,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="51">
-        <f t="shared" ref="H2:H5" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H6" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="52">
@@ -6542,7 +6727,7 @@
       </c>
       <c r="N2" s="73">
         <f>SUM(H:H)</f>
-        <v>14.33</v>
+        <v>3.9000000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -6645,6 +6830,30 @@
       <c r="J5" s="73">
         <f t="shared" si="2"/>
         <v>-10.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="48">
+        <v>44831</v>
+      </c>
+      <c r="B6" s="49">
+        <v>1218</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="103" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="31">
+        <v>1</v>
+      </c>
+      <c r="G6" s="50">
+        <v>-10.43</v>
+      </c>
+      <c r="H6" s="51">
+        <f t="shared" si="0"/>
+        <v>-10.43</v>
       </c>
     </row>
   </sheetData>
@@ -6654,10 +6863,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5E4B5F-C3CE-4821-8081-9385439A4F7E}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6740,7 +6949,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="51">
-        <f t="shared" ref="H2:H5" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H6" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="52">
@@ -6752,7 +6961,7 @@
       </c>
       <c r="N2" s="73">
         <f>SUM(H:H)</f>
-        <v>12.53</v>
+        <v>2.0999999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -6855,6 +7064,30 @@
       <c r="J5" s="73">
         <f t="shared" si="3"/>
         <v>-10.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="48">
+        <v>44831</v>
+      </c>
+      <c r="B6" s="49">
+        <v>1218</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="103" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="31">
+        <v>1</v>
+      </c>
+      <c r="G6" s="50">
+        <v>-10.43</v>
+      </c>
+      <c r="H6" s="51">
+        <f t="shared" si="0"/>
+        <v>-10.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Market Open Sep28/2022 - Update 0DTE Experiment.xlsx
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34D7DF3-33AB-4631-949E-C57A614193B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DB5B01-A397-4D0C-84CD-C9A2FB584513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="4605" windowWidth="23580" windowHeight="14010" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
+    <workbookView xWindow="34590" yWindow="6255" windowWidth="16560" windowHeight="12045" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="134">
   <si>
     <t>SPX Open</t>
   </si>
@@ -429,6 +429,18 @@
   </si>
   <si>
     <t>Triggered around 3650</t>
+  </si>
+  <si>
+    <t>Developing new indicator</t>
+  </si>
+  <si>
+    <t>Sep28 3690/3715 Bear Call @ -4.3</t>
+  </si>
+  <si>
+    <t>Sep28 3605/3580 Bull Put @ -5.3</t>
+  </si>
+  <si>
+    <t>Sep28 3590/3565 Bull Put @ -3.9</t>
   </si>
 </sst>
 </file>
@@ -746,10 +758,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -833,6 +841,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -929,7 +941,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tracker!$A$5:$A$700</c:f>
+              <c:f>Tracker!$A$19:$A$714</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="696"/>
@@ -956,7 +968,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tracker!$K$5:$K$700</c:f>
+              <c:f>Tracker!$K$19:$K$714</c:f>
               <c:numCache>
                 <c:formatCode>#,##0_);\(#,##0\)</c:formatCode>
                 <c:ptCount val="696"/>
@@ -1039,7 +1051,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$A$5:$A$700</c15:sqref>
+                          <c15:sqref>Tracker!$A$19:$A$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1072,7 +1084,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$H$5:$H$700</c15:sqref>
+                          <c15:sqref>Tracker!$H$19:$H$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1146,7 +1158,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$A$5:$A$700</c15:sqref>
+                          <c15:sqref>Tracker!$A$19:$A$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1179,7 +1191,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$I$5:$I$700</c15:sqref>
+                          <c15:sqref>Tracker!$I$19:$I$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1253,7 +1265,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$A$5:$A$700</c15:sqref>
+                          <c15:sqref>Tracker!$A$19:$A$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1286,7 +1298,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$J$5:$J$700</c15:sqref>
+                          <c15:sqref>Tracker!$J$19:$J$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1578,7 +1590,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Tracker!$A$5:$A$700</c:f>
+              <c:f>Tracker!$A$19:$A$714</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="696"/>
@@ -1606,7 +1618,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tracker!$I$5:$I$700</c:f>
+              <c:f>Tracker!$I$19:$I$714</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="696"/>
@@ -1688,7 +1700,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$A$5:$A$700</c15:sqref>
+                          <c15:sqref>Tracker!$A$19:$A$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1721,7 +1733,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$J$5:$J$700</c15:sqref>
+                          <c15:sqref>Tracker!$J$19:$J$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1792,7 +1804,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$A$5:$A$700</c15:sqref>
+                          <c15:sqref>Tracker!$A$19:$A$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1825,7 +1837,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$K$5:$K$700</c15:sqref>
+                          <c15:sqref>Tracker!$K$19:$K$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1885,7 +1897,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Tracker!$A$5:$A$700</c:f>
+              <c:f>Tracker!$A$19:$A$714</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="696"/>
@@ -1913,7 +1925,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tracker!$H$5:$H$700</c:f>
+              <c:f>Tracker!$H$19:$H$714</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="696"/>
@@ -2213,11 +2225,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Daily P/L</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> and Potential Max Premium</a:t>
+              <a:t>Premium Capture</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2285,7 +2293,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Tracker!$A$5:$A$700</c:f>
+              <c:f>Tracker!$A$19:$A$714</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="696"/>
@@ -2313,7 +2321,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tracker!$J$5:$J$700</c:f>
+              <c:f>Tracker!$J$19:$J$714</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="696"/>
@@ -2381,7 +2389,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$A$5:$A$700</c15:sqref>
+                          <c15:sqref>Tracker!$A$19:$A$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2414,7 +2422,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$I$5:$I$700</c15:sqref>
+                          <c15:sqref>Tracker!$I$19:$I$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2485,7 +2493,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$A$5:$A$700</c15:sqref>
+                          <c15:sqref>Tracker!$A$19:$A$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2518,7 +2526,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$K$5:$K$700</c15:sqref>
+                          <c15:sqref>Tracker!$K$19:$K$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2596,7 +2604,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$A$5:$A$700</c15:sqref>
+                          <c15:sqref>Tracker!$A$19:$A$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2629,7 +2637,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tracker!$H$5:$H$700</c15:sqref>
+                          <c15:sqref>Tracker!$H$19:$H$714</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4945,7 +4953,7 @@
   <dimension ref="B1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4967,10 +4975,10 @@
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="20">
-        <v>44831</v>
-      </c>
-      <c r="C2" s="65">
-        <v>0.90694444444444444</v>
+        <v>44832</v>
+      </c>
+      <c r="C2" s="104">
+        <v>1021</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4999,14 +5007,14 @@
         <v>3</v>
       </c>
       <c r="C5" s="12">
-        <v>3682.72</v>
+        <v>3686.44</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="27">
         <f>(C9-C18)/(C17-C18)</f>
-        <v>0.74502479403446709</v>
+        <v>0.53430290619708476</v>
       </c>
       <c r="G5" s="25">
         <v>0.4</v>
@@ -5018,14 +5026,14 @@
         <v>4</v>
       </c>
       <c r="C6" s="13">
-        <v>3655.52</v>
+        <v>3647.29</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="27">
         <f>(C9-C23)/(C22-C23)</f>
-        <v>0.56728667959101653</v>
+        <v>0.50401228645558727</v>
       </c>
       <c r="G6" s="25">
         <v>0.33</v>
@@ -5037,14 +5045,14 @@
         <v>12</v>
       </c>
       <c r="C7" s="13">
-        <v>3674.37</v>
+        <v>3651.17</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="28">
         <f>(C9-C28)/(C27-C28)</f>
-        <v>0.27675799239404836</v>
+        <v>0.31616050604746726</v>
       </c>
       <c r="G7" s="26">
         <v>0.27</v>
@@ -5056,14 +5064,14 @@
         <v>10</v>
       </c>
       <c r="C8" s="13">
-        <v>3750.52</v>
+        <v>3708.7</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="29">
         <f>F5*G5+F6*G6+F7*G7</f>
-        <v>0.55993917982521535</v>
+        <v>0.46540855364199385</v>
       </c>
       <c r="G8" s="24" t="s">
         <v>27</v>
@@ -5075,7 +5083,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="12">
-        <v>3686.44</v>
+        <v>3651.94</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -5084,9 +5092,7 @@
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13">
-        <v>3647.29</v>
-      </c>
+      <c r="C10" s="13"/>
       <c r="E10" s="10" t="s">
         <v>26</v>
       </c>
@@ -5102,9 +5108,7 @@
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="13">
-        <v>3651.17</v>
-      </c>
+      <c r="C11" s="13"/>
       <c r="E11" s="15" t="s">
         <v>57</v>
       </c>
@@ -5119,9 +5123,7 @@
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13">
-        <v>3708.7</v>
-      </c>
+      <c r="C12" s="13"/>
       <c r="E12" s="16" t="s">
         <v>59</v>
       </c>
@@ -5137,7 +5139,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="14">
-        <v>0.27400000000000002</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>60</v>
@@ -5181,7 +5183,7 @@
       </c>
       <c r="C16" s="4">
         <f>C6*C$13*SQRT((24/24)/252)</f>
-        <v>63.095655527110871</v>
+        <v>67.778513769123037</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>62</v>
@@ -5199,7 +5201,7 @@
       </c>
       <c r="C17" s="4">
         <f>C6+C16</f>
-        <v>3718.6156555271109</v>
+        <v>3715.068513769123</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>58</v>
@@ -5217,7 +5219,7 @@
       </c>
       <c r="C18" s="6">
         <f>C6-C16</f>
-        <v>3592.4243444728891</v>
+        <v>3579.5114862308769</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5233,7 +5235,7 @@
       </c>
       <c r="C21" s="4">
         <f>C7*C$13*(2/252)^0.5</f>
-        <v>89.690857636045607</v>
+        <v>95.955262482283004</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -5242,7 +5244,7 @@
       </c>
       <c r="C22" s="4">
         <f>C7+C21</f>
-        <v>3764.0608576360455</v>
+        <v>3747.1252624822832</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5251,7 +5253,7 @@
       </c>
       <c r="C23" s="6">
         <f>C7-C21</f>
-        <v>3584.6791423639543</v>
+        <v>3555.2147375177169</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5267,7 +5269,7 @@
       </c>
       <c r="C26" s="4">
         <f>C17*C$13*(5/252)^0.5</f>
-        <v>143.52137549557563</v>
+        <v>154.37379308347943</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -5276,7 +5278,7 @@
       </c>
       <c r="C27" s="4">
         <f>C8+C26</f>
-        <v>3894.0413754955757</v>
+        <v>3863.0737930834794</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5285,7 +5287,7 @@
       </c>
       <c r="C28" s="6">
         <f>C8-C26</f>
-        <v>3606.9986245044242</v>
+        <v>3554.3262069165203</v>
       </c>
     </row>
   </sheetData>
@@ -5299,7 +5301,7 @@
   <dimension ref="B1:N27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5309,8 +5311,8 @@
     <col min="3" max="3" width="11.28515625" style="17" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="17"/>
     <col min="5" max="5" width="23" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" style="68" customWidth="1"/>
-    <col min="7" max="7" width="7" style="68" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" style="67" customWidth="1"/>
+    <col min="7" max="7" width="7" style="67" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="17"/>
     <col min="10" max="10" width="26.28515625" style="17" bestFit="1" customWidth="1"/>
@@ -5319,7 +5321,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C1" s="75"/>
+      <c r="C1" s="74"/>
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
     </row>
@@ -5330,21 +5332,21 @@
       <c r="C2" s="17">
         <v>2022</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="71" t="s">
+      <c r="H2" s="70" t="s">
         <v>84</v>
       </c>
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
-      <c r="K2" s="70" t="s">
+      <c r="K2" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="L2" s="71" t="s">
+      <c r="L2" s="70" t="s">
         <v>6</v>
       </c>
       <c r="M2" s="22"/>
@@ -5354,66 +5356,66 @@
       <c r="B3" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="75">
+      <c r="C3" s="74">
         <v>44824</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="78">
+      <c r="F3" s="77">
         <f>COUNTA(Tracker!K:K)-1</f>
         <v>6</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="72">
+      <c r="H3" s="71">
         <f>C7/F3</f>
         <v>144.49999999999991</v>
       </c>
       <c r="J3" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="K3" s="68">
+      <c r="K3" s="67">
         <f>2*1.25%</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="L3" s="72">
+      <c r="L3" s="71">
         <f>K3*C5</f>
         <v>592.0412500000001</v>
       </c>
-      <c r="M3" s="77"/>
+      <c r="M3" s="76"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="72">
+      <c r="C4" s="71">
         <v>23681.65</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="78">
+      <c r="F4" s="77">
         <f>COUNTIF(Tracker!J:J, "&gt;0")</f>
         <v>4</v>
       </c>
-      <c r="G4" s="81">
+      <c r="G4" s="80">
         <f>F4/F3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="H4" s="72">
+      <c r="H4" s="71">
         <f>(SUMIF(Tracker!H:H, "&gt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&gt;0", Tracker!H2))/F4*100</f>
         <v>852.99999999999989</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="K4" s="68">
+      <c r="K4" s="67">
         <f>-3.75%</f>
         <v>-3.7499999999999999E-2</v>
       </c>
-      <c r="L4" s="72">
+      <c r="L4" s="71">
         <f>K4*C5</f>
         <v>-888.06187499999999</v>
       </c>
@@ -5422,36 +5424,36 @@
       <c r="B5" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="72">
+      <c r="C5" s="71">
         <v>23681.65</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="78">
+      <c r="F5" s="77">
         <f>COUNTIF(Tracker!J:J, "&lt;0")</f>
         <v>2</v>
       </c>
-      <c r="G5" s="81">
+      <c r="G5" s="80">
         <f>F5/F3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="H5" s="72">
+      <c r="H5" s="71">
         <f>IFERROR((SUMIF(Tracker!H:H, "&lt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&lt;0", Tracker!H2))/F5*100, 0)</f>
         <v>-1272.5000000000002</v>
       </c>
       <c r="J5" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="68">
+      <c r="K5" s="67">
         <f>+K3+K4</f>
         <v>-1.2499999999999997E-2</v>
       </c>
-      <c r="L5" s="72">
+      <c r="L5" s="71">
         <f>+L3+L4</f>
         <v>-296.02062499999988</v>
       </c>
-      <c r="M5" s="77"/>
+      <c r="M5" s="76"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="22"/>
@@ -5461,25 +5463,25 @@
       <c r="B7" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="72">
-        <f>INDEX(Tracker!K:K, COUNTA(Tracker!K:K)+3,1)</f>
+      <c r="C7" s="71">
+        <f>INDEX(Tracker!K:K, COUNTA(Tracker!K:K)+17,1)</f>
         <v>866.99999999999955</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F7" s="75">
         <f>C7/C4</f>
         <v>3.6610624681979488E-2</v>
       </c>
-      <c r="G7" s="76"/>
+      <c r="G7" s="75"/>
       <c r="J7" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="K7" s="82">
+      <c r="K7" s="81">
         <v>20</v>
       </c>
-      <c r="L7" s="82">
+      <c r="L7" s="81">
         <v>25</v>
       </c>
     </row>
@@ -5487,26 +5489,26 @@
       <c r="B8" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="72">
-        <f>INDEX(Tracker!L:L, COUNTA(Tracker!L:L)+3,1)</f>
+      <c r="C8" s="71">
+        <f>INDEX(Tracker!L:L, COUNTA(Tracker!L:L)+17,1)</f>
         <v>7073</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="76">
+      <c r="F8" s="75">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>4.157797603196757</v>
-      </c>
-      <c r="G8" s="76"/>
+        <v>3.2983482258239629</v>
+      </c>
+      <c r="G8" s="75"/>
       <c r="J8" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="K8" s="82">
+      <c r="K8" s="81">
         <f>FLOOR(MROUND(C4/1000, 5)/20, 1)</f>
         <v>1</v>
       </c>
-      <c r="L8" s="79">
+      <c r="L8" s="78">
         <f>FLOOR(MROUND(C4/1000, 5)/25, 1)</f>
         <v>1</v>
       </c>
@@ -5515,45 +5517,45 @@
       <c r="B9" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="76">
+      <c r="C9" s="75">
         <f>C7/C8</f>
         <v>0.12257882086808986</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F9" s="76">
+      <c r="F9" s="75">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>0.58873538507272904</v>
-      </c>
-      <c r="G9" s="76"/>
+        <v>0.50908084058328629</v>
+      </c>
+      <c r="G9" s="75"/>
       <c r="J9" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="K9" s="83">
+      <c r="K9" s="82">
         <f>K7*K8*100*2</f>
         <v>4000</v>
       </c>
-      <c r="L9" s="83">
+      <c r="L9" s="82">
         <f>L7*L8*100*2</f>
         <v>5000</v>
       </c>
     </row>
     <row r="24" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K24" s="69"/>
-      <c r="L24" s="69"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="68"/>
     </row>
     <row r="25" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
+      <c r="K25" s="68"/>
+      <c r="L25" s="68"/>
     </row>
     <row r="26" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K26" s="69"/>
-      <c r="L26" s="69"/>
+      <c r="K26" s="68"/>
+      <c r="L26" s="68"/>
     </row>
     <row r="27" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K27" s="69"/>
-      <c r="L27" s="69"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="68"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5564,10 +5566,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C82D01-CC02-4066-B9D6-9DFF5A0A89C9}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5579,7 +5581,7 @@
     <col min="8" max="8" width="9.140625" style="17"/>
     <col min="9" max="9" width="9.140625" style="61"/>
     <col min="10" max="10" width="10" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="66" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="55.140625" style="17" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="17"/>
@@ -5597,47 +5599,47 @@
       <c r="G1" s="55"/>
       <c r="H1" s="56"/>
       <c r="I1" s="57"/>
-      <c r="K1" s="66"/>
+      <c r="K1" s="65"/>
     </row>
     <row r="2" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="58">
         <f>Indicator!B2</f>
-        <v>44831</v>
+        <v>44832</v>
       </c>
       <c r="B2" s="43">
         <f>Indicator!$C$9</f>
-        <v>3686.44</v>
+        <v>3651.94</v>
       </c>
       <c r="C2" s="43">
         <f>Indicator!$C$10</f>
-        <v>3647.29</v>
+        <v>0</v>
       </c>
       <c r="D2" s="43">
         <f>Indicator!$C$11</f>
-        <v>3651.17</v>
+        <v>0</v>
       </c>
       <c r="E2" s="43">
         <f>Indicator!$C$12</f>
-        <v>3708.7</v>
+        <v>0</v>
       </c>
       <c r="F2" s="44">
         <f>Indicator!$C$13</f>
-        <v>0.27400000000000002</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="G2" s="44">
         <f>Indicator!$F$8</f>
-        <v>0.55993917982521535</v>
+        <v>0.46540855364199385</v>
       </c>
       <c r="H2" s="59">
         <f>SUMIF(Trades!A:A,Tracker!A2,Trades!H:H)</f>
-        <v>-5.58</v>
+        <v>17.68</v>
       </c>
       <c r="I2" s="60">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A2,  Trades!C:C, "STO")</f>
-        <v>22.619999999999997</v>
+        <v>17.68</v>
       </c>
       <c r="J2" s="21"/>
-      <c r="K2" s="66"/>
+      <c r="K2" s="65"/>
     </row>
     <row r="3" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="58"/>
@@ -5649,7 +5651,7 @@
       <c r="G3" s="41"/>
       <c r="H3" s="50"/>
       <c r="I3" s="61"/>
-      <c r="K3" s="66"/>
+      <c r="K3" s="65"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
@@ -5682,272 +5684,434 @@
       <c r="J4" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="67" t="s">
+      <c r="K4" s="66" t="s">
         <v>64</v>
       </c>
       <c r="L4" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="M4" s="74" t="s">
+      <c r="M4" s="73" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="58">
-        <v>44824</v>
+        <v>44803</v>
       </c>
       <c r="B5" s="42">
-        <v>3876.23</v>
+        <v>4041.25</v>
       </c>
       <c r="C5" s="42">
-        <v>3856.04</v>
-      </c>
-      <c r="D5" s="42">
-        <v>3877.96</v>
-      </c>
-      <c r="E5" s="42">
-        <v>3895.32</v>
-      </c>
-      <c r="F5" s="41">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="G5" s="41">
-        <v>0.25700000000000001</v>
-      </c>
-      <c r="H5" s="17">
-        <v>7.2899999999999991</v>
-      </c>
-      <c r="I5" s="61">
-        <v>7.2899999999999991</v>
-      </c>
-      <c r="J5" s="21">
-        <f t="shared" ref="J5:J10" si="0">H5/I5</f>
-        <v>1</v>
-      </c>
-      <c r="K5" s="66">
-        <f>H5*100</f>
-        <v>728.99999999999989</v>
-      </c>
-      <c r="L5">
-        <f>I5*100</f>
-        <v>728.99999999999989</v>
+        <v>3986.16</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="58">
+        <v>44804</v>
+      </c>
+      <c r="B6" s="42">
+        <v>4000.67</v>
+      </c>
+      <c r="C6" s="42">
+        <v>3955</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="58">
+        <v>44805</v>
+      </c>
+      <c r="B7" s="42">
+        <v>3936.73</v>
+      </c>
+      <c r="C7" s="42">
+        <v>3966.85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="58">
+        <v>44806</v>
+      </c>
+      <c r="B8" s="42">
+        <v>3994.66</v>
+      </c>
+      <c r="C8" s="42">
+        <v>3924.26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="58">
+        <v>44810</v>
+      </c>
+      <c r="B9" s="42">
+        <v>3930.89</v>
+      </c>
+      <c r="C9" s="42">
+        <v>3908.19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="58">
+        <v>44811</v>
+      </c>
+      <c r="B10" s="42">
+        <v>3909.43</v>
+      </c>
+      <c r="C10" s="42">
+        <v>3979.87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="58">
+        <v>44812</v>
+      </c>
+      <c r="B11" s="42">
+        <v>3959.94</v>
+      </c>
+      <c r="C11" s="42">
+        <v>4006.18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="58">
+        <v>44813</v>
+      </c>
+      <c r="B12" s="42">
+        <v>4022.94</v>
+      </c>
+      <c r="C12" s="42">
+        <v>4067.36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="58">
+        <v>44816</v>
+      </c>
+      <c r="B13" s="42">
+        <v>4083.67</v>
+      </c>
+      <c r="C13" s="42">
+        <v>4110.41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="58">
+        <v>44817</v>
+      </c>
+      <c r="B14" s="42">
+        <v>4037.12</v>
+      </c>
+      <c r="C14" s="42">
+        <v>3932.69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="58">
+        <v>44818</v>
+      </c>
+      <c r="B15" s="42">
+        <v>3940.73</v>
+      </c>
+      <c r="C15" s="42">
+        <v>3946.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="58">
+        <v>44819</v>
+      </c>
+      <c r="B16" s="42">
+        <v>3932.41</v>
+      </c>
+      <c r="C16" s="42">
+        <v>3901.35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="58">
+        <v>44820</v>
+      </c>
+      <c r="B17" s="42">
+        <v>3880.95</v>
+      </c>
+      <c r="C17" s="42">
+        <v>3873.33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="58">
+        <v>44823</v>
+      </c>
+      <c r="B18" s="42">
+        <v>3849.91</v>
+      </c>
+      <c r="C18" s="42">
+        <v>3899.89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="58">
+        <v>44824</v>
+      </c>
+      <c r="B19" s="42">
+        <v>3876.23</v>
+      </c>
+      <c r="C19" s="42">
+        <v>3856.04</v>
+      </c>
+      <c r="D19" s="42">
+        <v>3877.96</v>
+      </c>
+      <c r="E19" s="42">
+        <v>3895.32</v>
+      </c>
+      <c r="F19" s="41">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="G19" s="41">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="H19" s="17">
+        <v>7.2899999999999991</v>
+      </c>
+      <c r="I19" s="61">
+        <v>7.2899999999999991</v>
+      </c>
+      <c r="J19" s="21">
+        <f t="shared" ref="J19:J24" si="0">H19/I19</f>
+        <v>1</v>
+      </c>
+      <c r="K19" s="65">
+        <f>H19*100</f>
+        <v>728.99999999999989</v>
+      </c>
+      <c r="L19">
+        <f>I19*100</f>
+        <v>728.99999999999989</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="58">
         <v>44825</v>
       </c>
-      <c r="B6" s="42">
+      <c r="B20" s="42">
         <v>3871.4</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C20" s="42">
         <v>3789.93</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D20" s="42">
         <v>3822.93</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E20" s="42">
         <v>3864.09</v>
       </c>
-      <c r="F6" s="41">
+      <c r="F20" s="41">
         <v>0.249</v>
       </c>
-      <c r="G6" s="41">
+      <c r="G20" s="41">
         <v>0.51517990352733356</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H20" s="17">
         <v>3.84</v>
       </c>
-      <c r="I6" s="61">
+      <c r="I20" s="61">
         <v>5.17</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J20" s="21">
         <f t="shared" si="0"/>
         <v>0.74274661508704065</v>
       </c>
-      <c r="K6" s="66">
-        <f>K5+H6*100</f>
+      <c r="K20" s="65">
+        <f>K19+H20*100</f>
         <v>1113</v>
       </c>
-      <c r="L6">
-        <f>I6*100+L5</f>
+      <c r="L20">
+        <f>I20*100+L19</f>
         <v>1246</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M20" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="58">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="58">
         <v>44826</v>
       </c>
-      <c r="B7" s="42">
+      <c r="B21" s="42">
         <v>3782.36</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C21" s="42">
         <v>3757.99</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D21" s="42">
         <v>3773.96</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E21" s="42">
         <v>3835.41</v>
       </c>
-      <c r="F7" s="41">
+      <c r="F21" s="41">
         <v>0.25900000000000001</v>
       </c>
-      <c r="G7" s="41">
+      <c r="G21" s="41">
         <v>0.32110807324379981</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H21" s="17">
         <v>9.7100000000000009</v>
       </c>
-      <c r="I7" s="61">
+      <c r="I21" s="61">
         <v>9.7100000000000009</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J21" s="21">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K7" s="66">
-        <f>K6+H7*100</f>
+      <c r="K21" s="65">
+        <f>K20+H21*100</f>
         <v>2084</v>
       </c>
-      <c r="L7">
-        <f>I7*100+L6</f>
+      <c r="L21">
+        <f>I21*100+L20</f>
         <v>2217</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="58">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="58">
         <v>44827</v>
       </c>
-      <c r="B8" s="42">
+      <c r="B22" s="42">
         <v>3727.14</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C22" s="42">
         <v>3693.49</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D22" s="42">
         <v>3725.74</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E22" s="42">
         <v>3799.45</v>
       </c>
-      <c r="F8" s="41">
+      <c r="F22" s="41">
         <v>0.26400000000000001</v>
       </c>
-      <c r="G8" s="41">
+      <c r="G22" s="41">
         <v>0.22597893531506713</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H22" s="17">
         <v>-19.870000000000005</v>
       </c>
-      <c r="I8" s="61">
+      <c r="I22" s="61">
         <v>12.66</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J22" s="21">
         <f t="shared" si="0"/>
         <v>-1.5695102685624016</v>
       </c>
-      <c r="K8" s="66">
-        <f>K7+H8*100</f>
+      <c r="K22" s="65">
+        <f>K21+H22*100</f>
         <v>96.999999999999545</v>
       </c>
-      <c r="L8">
-        <f>I8*100+L7</f>
+      <c r="L22">
+        <f>I22*100+L21</f>
         <v>3483</v>
       </c>
-      <c r="M8" s="17" t="s">
+      <c r="M22" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="58">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="58">
         <v>44830</v>
       </c>
-      <c r="B9" s="42">
+      <c r="B23" s="42">
         <v>3682.72</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C23" s="42">
         <v>3655.52</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D23" s="42">
         <v>3674.37</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E23" s="42">
         <v>3750.52</v>
       </c>
-      <c r="F9" s="41">
+      <c r="F23" s="41">
         <v>0.27800000000000002</v>
       </c>
-      <c r="G9" s="41">
+      <c r="G23" s="41">
         <v>0.28269041759555957</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H23" s="17">
         <v>13.28</v>
       </c>
-      <c r="I9" s="61">
+      <c r="I23" s="61">
         <v>13.28</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J23" s="21">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K9" s="66">
-        <f>K8+H9*100</f>
+      <c r="K23" s="65">
+        <f>K22+H23*100</f>
         <v>1424.9999999999995</v>
       </c>
-      <c r="L9">
-        <f>I9*100+L8</f>
+      <c r="L23">
+        <f>I23*100+L22</f>
         <v>4811</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="58">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="58">
         <v>44831</v>
       </c>
-      <c r="B10" s="42">
+      <c r="B24" s="42">
         <v>3686.44</v>
       </c>
-      <c r="C10" s="42">
+      <c r="C24" s="42">
         <v>3647.29</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D24" s="42">
         <v>3651.17</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E24" s="42">
         <v>3708.7</v>
       </c>
-      <c r="F10" s="41">
+      <c r="F24" s="41">
         <v>0.27400000000000002</v>
       </c>
-      <c r="G10" s="41">
+      <c r="G24" s="41">
         <v>0.55993917982521535</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H24" s="17">
         <v>-5.58</v>
       </c>
-      <c r="I10" s="61">
+      <c r="I24" s="61">
         <v>22.619999999999997</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J24" s="21">
         <f t="shared" si="0"/>
         <v>-0.24668435013262602</v>
       </c>
-      <c r="K10" s="66">
-        <f>K9+H10*100</f>
+      <c r="K24" s="65">
+        <f>K23+H24*100</f>
         <v>866.99999999999955</v>
       </c>
-      <c r="L10">
-        <f>I10*100+L9</f>
+      <c r="L24">
+        <f>I24*100+L23</f>
         <v>7073</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="M24" s="17" t="s">
         <v>129</v>
       </c>
     </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M25" s="68" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:C18">
+    <sortCondition ref="A5:A18"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -5955,10 +6119,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5967,51 +6131,51 @@
     <col min="2" max="2" width="9.7109375" style="49" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" style="102" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" style="101" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.140625" style="50" customWidth="1"/>
     <col min="8" max="8" width="7.140625" style="51" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" style="72" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" style="52" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" style="72" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="92" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+    <row r="1" spans="1:12" s="91" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="85" t="s">
         <v>33</v>
       </c>
       <c r="C1" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="100" t="s">
         <v>34</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="88" t="s">
+      <c r="G1" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="90" t="s">
+      <c r="I1" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="91" t="s">
+      <c r="J1" s="90" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="90" t="s">
+      <c r="K1" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="91" t="s">
+      <c r="L1" s="90" t="s">
         <v>56</v>
       </c>
     </row>
@@ -6028,7 +6192,7 @@
       <c r="D2" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="102">
+      <c r="E2" s="101">
         <v>-0.15</v>
       </c>
       <c r="F2" s="31">
@@ -6044,7 +6208,7 @@
       <c r="I2" s="52">
         <v>3</v>
       </c>
-      <c r="J2" s="73">
+      <c r="J2" s="72">
         <f t="shared" ref="J2:J4" si="1">-I2*G2</f>
         <v>-12.809999999999999</v>
       </c>
@@ -6062,7 +6226,7 @@
       <c r="D3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="102">
+      <c r="E3" s="101">
         <v>0.09</v>
       </c>
       <c r="F3" s="31">
@@ -6078,7 +6242,7 @@
       <c r="I3" s="52">
         <v>3</v>
       </c>
-      <c r="J3" s="73">
+      <c r="J3" s="72">
         <f t="shared" si="1"/>
         <v>-9.06</v>
       </c>
@@ -6096,7 +6260,7 @@
       <c r="D4" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="102">
+      <c r="E4" s="101">
         <v>-0.15</v>
       </c>
       <c r="F4" s="31">
@@ -6112,14 +6276,14 @@
       <c r="I4" s="52">
         <v>2.5</v>
       </c>
-      <c r="J4" s="73">
+      <c r="J4" s="72">
         <f t="shared" si="1"/>
         <v>-12.925000000000001</v>
       </c>
       <c r="K4" s="52">
         <v>0.75</v>
       </c>
-      <c r="L4" s="73">
+      <c r="L4" s="72">
         <f>-G4+K4*G4</f>
         <v>-1.2925</v>
       </c>
@@ -6158,10 +6322,10 @@
       <c r="C6" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="69" t="s">
+      <c r="D6" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="102">
+      <c r="E6" s="101">
         <v>-0.16</v>
       </c>
       <c r="F6" s="31">
@@ -6177,7 +6341,7 @@
       <c r="I6" s="52">
         <v>3</v>
       </c>
-      <c r="J6" s="73">
+      <c r="J6" s="72">
         <f t="shared" ref="J6:J9" si="2">-I6*G6</f>
         <v>-14.91</v>
       </c>
@@ -6192,10 +6356,10 @@
       <c r="C7" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="69" t="s">
+      <c r="D7" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="102">
+      <c r="E7" s="101">
         <v>0.13</v>
       </c>
       <c r="F7" s="31">
@@ -6211,7 +6375,7 @@
       <c r="I7" s="52">
         <v>3</v>
       </c>
-      <c r="J7" s="73">
+      <c r="J7" s="72">
         <f t="shared" si="2"/>
         <v>-7.11</v>
       </c>
@@ -6226,10 +6390,10 @@
       <c r="C8" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="69" t="s">
+      <c r="D8" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="E8" s="102">
+      <c r="E8" s="101">
         <v>-0.3</v>
       </c>
       <c r="F8" s="31">
@@ -6245,7 +6409,7 @@
       <c r="I8" s="52">
         <v>3</v>
       </c>
-      <c r="J8" s="73">
+      <c r="J8" s="72">
         <f t="shared" si="2"/>
         <v>-19.41</v>
       </c>
@@ -6260,10 +6424,10 @@
       <c r="C9" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="69" t="s">
+      <c r="D9" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="E9" s="102">
+      <c r="E9" s="101">
         <v>-0.19</v>
       </c>
       <c r="F9" s="31">
@@ -6279,7 +6443,7 @@
       <c r="I9" s="52">
         <v>3</v>
       </c>
-      <c r="J9" s="73">
+      <c r="J9" s="72">
         <f t="shared" si="2"/>
         <v>-11.91</v>
       </c>
@@ -6294,7 +6458,7 @@
       <c r="C10" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="68" t="s">
         <v>116</v>
       </c>
       <c r="F10" s="31">
@@ -6318,7 +6482,7 @@
       <c r="C11" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="D11" s="69" t="s">
+      <c r="D11" s="68" t="s">
         <v>113</v>
       </c>
       <c r="F11" s="31">
@@ -6342,10 +6506,10 @@
       <c r="C12" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="69" t="s">
+      <c r="D12" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="E12" s="102">
+      <c r="E12" s="101">
         <v>-0.19</v>
       </c>
       <c r="F12" s="31">
@@ -6361,7 +6525,7 @@
       <c r="I12" s="52">
         <v>3</v>
       </c>
-      <c r="J12" s="73">
+      <c r="J12" s="72">
         <f>-I12*G12</f>
         <v>-6.66</v>
       </c>
@@ -6376,10 +6540,10 @@
       <c r="C13" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="69" t="s">
+      <c r="D13" s="68" t="s">
         <v>122</v>
       </c>
-      <c r="E13" s="102">
+      <c r="E13" s="101">
         <v>-0.15</v>
       </c>
       <c r="F13" s="31">
@@ -6395,7 +6559,7 @@
       <c r="I13" s="52">
         <v>3</v>
       </c>
-      <c r="J13" s="73">
+      <c r="J13" s="72">
         <f>-I13*G13</f>
         <v>-12.809999999999999</v>
       </c>
@@ -6410,10 +6574,10 @@
       <c r="C14" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="69" t="s">
+      <c r="D14" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="E14" s="102">
+      <c r="E14" s="101">
         <v>0.15</v>
       </c>
       <c r="F14" s="31">
@@ -6429,7 +6593,7 @@
       <c r="I14" s="52">
         <v>3</v>
       </c>
-      <c r="J14" s="73">
+      <c r="J14" s="72">
         <f t="shared" ref="J14:J15" si="4">-I14*G14</f>
         <v>-9.81</v>
       </c>
@@ -6444,10 +6608,10 @@
       <c r="C15" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="69" t="s">
+      <c r="D15" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="E15" s="102">
+      <c r="E15" s="101">
         <v>0.11</v>
       </c>
       <c r="F15" s="31">
@@ -6463,7 +6627,7 @@
       <c r="I15" s="52">
         <v>3</v>
       </c>
-      <c r="J15" s="73">
+      <c r="J15" s="72">
         <f t="shared" si="4"/>
         <v>-4.41</v>
       </c>
@@ -6478,10 +6642,10 @@
       <c r="C16" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="103" t="s">
+      <c r="D16" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="E16" s="102">
+      <c r="E16" s="101">
         <v>-0.16</v>
       </c>
       <c r="F16" s="31">
@@ -6497,7 +6661,7 @@
       <c r="I16" s="52">
         <v>3</v>
       </c>
-      <c r="J16" s="73">
+      <c r="J16" s="72">
         <f t="shared" ref="J16:J18" si="5">-I16*G16</f>
         <v>-10.11</v>
       </c>
@@ -6512,10 +6676,10 @@
       <c r="C17" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="103" t="s">
+      <c r="D17" s="102" t="s">
         <v>125</v>
       </c>
-      <c r="E17" s="102">
+      <c r="E17" s="101">
         <v>0.17</v>
       </c>
       <c r="F17" s="31">
@@ -6531,7 +6695,7 @@
       <c r="I17" s="52">
         <v>3</v>
       </c>
-      <c r="J17" s="73">
+      <c r="J17" s="72">
         <f t="shared" si="5"/>
         <v>-11.61</v>
       </c>
@@ -6546,10 +6710,10 @@
       <c r="C18" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="103" t="s">
+      <c r="D18" s="102" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="102">
+      <c r="E18" s="101">
         <v>0.14000000000000001</v>
       </c>
       <c r="F18" s="31">
@@ -6565,7 +6729,7 @@
       <c r="I18" s="52">
         <v>3</v>
       </c>
-      <c r="J18" s="73">
+      <c r="J18" s="72">
         <f t="shared" si="5"/>
         <v>-8.91</v>
       </c>
@@ -6580,7 +6744,7 @@
       <c r="C19" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="D19" s="103" t="s">
+      <c r="D19" s="102" t="s">
         <v>127</v>
       </c>
       <c r="F19" s="31">
@@ -6590,7 +6754,7 @@
         <v>-14.1</v>
       </c>
       <c r="H19" s="51">
-        <f t="shared" ref="H19:H20" si="6">G19*F19</f>
+        <f t="shared" ref="H19:H23" si="6">G19*F19</f>
         <v>-28.2</v>
       </c>
     </row>
@@ -6604,10 +6768,10 @@
       <c r="C20" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="104" t="s">
+      <c r="D20" s="103" t="s">
         <v>128</v>
       </c>
-      <c r="E20" s="102">
+      <c r="E20" s="101">
         <v>0.15</v>
       </c>
       <c r="F20" s="31">
@@ -6619,6 +6783,115 @@
       <c r="H20" s="51">
         <f t="shared" si="6"/>
         <v>9.0399999999999991</v>
+      </c>
+      <c r="I20" s="52">
+        <v>3</v>
+      </c>
+      <c r="J20" s="72">
+        <f t="shared" ref="J20" si="7">-I20*G20</f>
+        <v>-13.559999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="48">
+        <v>44832</v>
+      </c>
+      <c r="B21" s="49">
+        <v>934</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="103" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" s="101">
+        <v>0.15</v>
+      </c>
+      <c r="F21" s="31">
+        <v>2</v>
+      </c>
+      <c r="G21" s="50">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="H21" s="51">
+        <f t="shared" si="6"/>
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="I21" s="52">
+        <v>3</v>
+      </c>
+      <c r="J21" s="72">
+        <f t="shared" ref="J21:J23" si="8">-I21*G21</f>
+        <v>-12.809999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="48">
+        <v>44832</v>
+      </c>
+      <c r="B22" s="49">
+        <v>938</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="103" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" s="101">
+        <v>-0.15</v>
+      </c>
+      <c r="F22" s="31">
+        <v>1</v>
+      </c>
+      <c r="G22" s="50">
+        <v>5.27</v>
+      </c>
+      <c r="H22" s="51">
+        <f t="shared" si="6"/>
+        <v>5.27</v>
+      </c>
+      <c r="I22" s="52">
+        <v>3</v>
+      </c>
+      <c r="J22" s="72">
+        <f t="shared" si="8"/>
+        <v>-15.809999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="48">
+        <v>44832</v>
+      </c>
+      <c r="B23" s="49">
+        <v>940</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="103" t="s">
+        <v>133</v>
+      </c>
+      <c r="E23" s="101">
+        <v>-0.09</v>
+      </c>
+      <c r="F23" s="31">
+        <v>1</v>
+      </c>
+      <c r="G23" s="50">
+        <v>3.87</v>
+      </c>
+      <c r="H23" s="51">
+        <f t="shared" si="6"/>
+        <v>3.87</v>
+      </c>
+      <c r="I23" s="52">
+        <v>3</v>
+      </c>
+      <c r="J23" s="72">
+        <f t="shared" si="8"/>
+        <v>-11.61</v>
       </c>
     </row>
   </sheetData>
@@ -6629,10 +6902,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE4BC4F-EB6D-4F7C-A4AB-32C246F0D899}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6641,54 +6914,54 @@
     <col min="2" max="2" width="9.7109375" style="49" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" style="102" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" style="101" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.140625" style="50" customWidth="1"/>
     <col min="8" max="8" width="7.140625" style="51" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" style="72" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" style="52" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" style="72" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="92" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+    <row r="1" spans="1:14" s="91" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="85" t="s">
         <v>33</v>
       </c>
       <c r="C1" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="100" t="s">
         <v>34</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="88" t="s">
+      <c r="G1" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="90" t="s">
+      <c r="I1" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="91" t="s">
+      <c r="J1" s="90" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="90" t="s">
+      <c r="K1" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="91" t="s">
+      <c r="L1" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="99" t="s">
+      <c r="N1" s="98" t="s">
         <v>42</v>
       </c>
     </row>
@@ -6702,10 +6975,10 @@
       <c r="C2" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="102">
+      <c r="E2" s="101">
         <v>-0.15</v>
       </c>
       <c r="F2" s="31">
@@ -6715,19 +6988,19 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="51">
-        <f t="shared" ref="H2:H6" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H8" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="52">
         <v>3</v>
       </c>
-      <c r="J2" s="73">
+      <c r="J2" s="72">
         <f t="shared" ref="J2:J3" si="1">-I2*H2</f>
         <v>-12.809999999999999</v>
       </c>
-      <c r="N2" s="73">
+      <c r="N2" s="72">
         <f>SUM(H:H)</f>
-        <v>3.9000000000000004</v>
+        <v>13.44</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -6740,10 +7013,10 @@
       <c r="C3" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="E3" s="102">
+      <c r="E3" s="101">
         <v>0.15</v>
       </c>
       <c r="F3" s="31">
@@ -6759,7 +7032,7 @@
       <c r="I3" s="52">
         <v>3</v>
       </c>
-      <c r="J3" s="73">
+      <c r="J3" s="72">
         <f t="shared" si="1"/>
         <v>-9.81</v>
       </c>
@@ -6774,10 +7047,10 @@
       <c r="C4" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="E4" s="102">
+      <c r="E4" s="101">
         <v>-0.16</v>
       </c>
       <c r="F4" s="31">
@@ -6793,7 +7066,7 @@
       <c r="I4" s="52">
         <v>3</v>
       </c>
-      <c r="J4" s="73">
+      <c r="J4" s="72">
         <f t="shared" ref="J4:J5" si="2">-I4*G4</f>
         <v>-10.11</v>
       </c>
@@ -6808,10 +7081,10 @@
       <c r="C5" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="103" t="s">
+      <c r="D5" s="102" t="s">
         <v>125</v>
       </c>
-      <c r="E5" s="102">
+      <c r="E5" s="101">
         <v>0.17</v>
       </c>
       <c r="F5" s="31">
@@ -6827,7 +7100,7 @@
       <c r="I5" s="52">
         <v>3</v>
       </c>
-      <c r="J5" s="73">
+      <c r="J5" s="72">
         <f t="shared" si="2"/>
         <v>-10.26</v>
       </c>
@@ -6842,7 +7115,7 @@
       <c r="C6" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="103" t="s">
+      <c r="D6" s="102" t="s">
         <v>127</v>
       </c>
       <c r="F6" s="31">
@@ -6854,6 +7127,74 @@
       <c r="H6" s="51">
         <f t="shared" si="0"/>
         <v>-10.43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="48">
+        <v>44832</v>
+      </c>
+      <c r="B7" s="49">
+        <v>934</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="103" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="101">
+        <v>0.15</v>
+      </c>
+      <c r="F7" s="31">
+        <v>1</v>
+      </c>
+      <c r="G7" s="50">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="H7" s="51">
+        <f t="shared" si="0"/>
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="I7" s="52">
+        <v>3</v>
+      </c>
+      <c r="J7" s="72">
+        <f t="shared" ref="J7:J8" si="3">-I7*G7</f>
+        <v>-12.809999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="48">
+        <v>44832</v>
+      </c>
+      <c r="B8" s="49">
+        <v>938</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="103" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="101">
+        <v>-0.15</v>
+      </c>
+      <c r="F8" s="31">
+        <v>1</v>
+      </c>
+      <c r="G8" s="50">
+        <v>5.27</v>
+      </c>
+      <c r="H8" s="51">
+        <f t="shared" si="0"/>
+        <v>5.27</v>
+      </c>
+      <c r="I8" s="52">
+        <v>3</v>
+      </c>
+      <c r="J8" s="72">
+        <f t="shared" si="3"/>
+        <v>-15.809999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -6863,10 +7204,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5E4B5F-C3CE-4821-8081-9385439A4F7E}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6875,54 +7216,54 @@
     <col min="2" max="2" width="9.7109375" style="49" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" style="102" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" style="101" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.140625" style="50" customWidth="1"/>
     <col min="8" max="8" width="7.140625" style="51" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" style="72" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" style="52" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" style="73" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" style="72" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="92" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+    <row r="1" spans="1:14" s="91" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="85" t="s">
         <v>33</v>
       </c>
       <c r="C1" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="100" t="s">
         <v>34</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="88" t="s">
+      <c r="G1" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="90" t="s">
+      <c r="I1" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="91" t="s">
+      <c r="J1" s="90" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="90" t="s">
+      <c r="K1" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="91" t="s">
+      <c r="L1" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="99" t="s">
+      <c r="N1" s="98" t="s">
         <v>42</v>
       </c>
     </row>
@@ -6936,10 +7277,10 @@
       <c r="C2" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="102">
+      <c r="E2" s="101">
         <v>-0.15</v>
       </c>
       <c r="F2" s="31">
@@ -6949,19 +7290,19 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="51">
-        <f t="shared" ref="H2:H6" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H8" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="52">
         <v>3</v>
       </c>
-      <c r="J2" s="73">
+      <c r="J2" s="72">
         <f t="shared" ref="J2" si="1">-I2*H2</f>
         <v>-12.809999999999999</v>
       </c>
-      <c r="N2" s="73">
+      <c r="N2" s="72">
         <f>SUM(H:H)</f>
-        <v>2.0999999999999996</v>
+        <v>10.239999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -6974,10 +7315,10 @@
       <c r="C3" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="102">
+      <c r="E3" s="101">
         <v>0.11</v>
       </c>
       <c r="F3" s="31">
@@ -6993,7 +7334,7 @@
       <c r="I3" s="52">
         <v>3</v>
       </c>
-      <c r="J3" s="73">
+      <c r="J3" s="72">
         <f t="shared" ref="J3" si="2">-I3*H3</f>
         <v>-4.41</v>
       </c>
@@ -7008,10 +7349,10 @@
       <c r="C4" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="E4" s="102">
+      <c r="E4" s="101">
         <v>-0.16</v>
       </c>
       <c r="F4" s="31">
@@ -7027,7 +7368,7 @@
       <c r="I4" s="52">
         <v>3</v>
       </c>
-      <c r="J4" s="73">
+      <c r="J4" s="72">
         <f t="shared" ref="J4:J5" si="3">-I4*G4</f>
         <v>-10.11</v>
       </c>
@@ -7042,10 +7383,10 @@
       <c r="C5" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="103" t="s">
+      <c r="D5" s="102" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="102">
+      <c r="E5" s="101">
         <v>0.14000000000000001</v>
       </c>
       <c r="F5" s="31">
@@ -7061,7 +7402,7 @@
       <c r="I5" s="52">
         <v>3</v>
       </c>
-      <c r="J5" s="73">
+      <c r="J5" s="72">
         <f t="shared" si="3"/>
         <v>-10.26</v>
       </c>
@@ -7076,7 +7417,7 @@
       <c r="C6" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="103" t="s">
+      <c r="D6" s="102" t="s">
         <v>127</v>
       </c>
       <c r="F6" s="31">
@@ -7088,6 +7429,74 @@
       <c r="H6" s="51">
         <f t="shared" si="0"/>
         <v>-10.43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="48">
+        <v>44832</v>
+      </c>
+      <c r="B7" s="49">
+        <v>934</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="103" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="101">
+        <v>0.15</v>
+      </c>
+      <c r="F7" s="31">
+        <v>1</v>
+      </c>
+      <c r="G7" s="50">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="H7" s="51">
+        <f t="shared" si="0"/>
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="I7" s="52">
+        <v>3</v>
+      </c>
+      <c r="J7" s="72">
+        <f t="shared" ref="J7:J8" si="4">-I7*G7</f>
+        <v>-12.809999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="48">
+        <v>44832</v>
+      </c>
+      <c r="B8" s="49">
+        <v>940</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="103" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="101">
+        <v>-0.09</v>
+      </c>
+      <c r="F8" s="31">
+        <v>1</v>
+      </c>
+      <c r="G8" s="50">
+        <v>3.87</v>
+      </c>
+      <c r="H8" s="51">
+        <f t="shared" si="0"/>
+        <v>3.87</v>
+      </c>
+      <c r="I8" s="52">
+        <v>3</v>
+      </c>
+      <c r="J8" s="72">
+        <f t="shared" si="4"/>
+        <v>-11.61</v>
       </c>
     </row>
   </sheetData>
@@ -7125,52 +7534,52 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="92"/>
-      <c r="C6" s="92" t="s">
+      <c r="B6" s="91"/>
+      <c r="C6" s="91" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="92" t="s">
+      <c r="D6" s="91" t="s">
         <v>95</v>
       </c>
-      <c r="E6" s="92" t="s">
+      <c r="E6" s="91" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="92" t="s">
+      <c r="F6" s="91" t="s">
         <v>97</v>
       </c>
-      <c r="G6" s="92" t="s">
+      <c r="G6" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="H6" s="92" t="s">
+      <c r="H6" s="91" t="s">
         <v>94</v>
       </c>
-      <c r="I6" s="92"/>
+      <c r="I6" s="91"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="91" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="93">
+      <c r="C7" s="92">
         <v>-1.5</v>
       </c>
-      <c r="D7" s="93">
+      <c r="D7" s="92">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="E7" s="93">
+      <c r="E7" s="92">
         <v>-1</v>
       </c>
-      <c r="F7" s="93">
+      <c r="F7" s="92">
         <v>1</v>
       </c>
-      <c r="G7" s="93">
+      <c r="G7" s="92">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H7" s="93">
+      <c r="H7" s="92">
         <v>1.5</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="91" t="s">
         <v>100</v>
       </c>
       <c r="C8">
@@ -7193,204 +7602,204 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="91" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="94">
+      <c r="C9" s="93">
         <v>-0.43319999999999997</v>
       </c>
-      <c r="D9" s="94">
+      <c r="D9" s="93">
         <v>-0.36430000000000001</v>
       </c>
-      <c r="E9" s="94">
+      <c r="E9" s="93">
         <v>-0.34129999999999999</v>
       </c>
-      <c r="F9" s="94">
+      <c r="F9" s="93">
         <v>0.34129999999999999</v>
       </c>
-      <c r="G9" s="94">
+      <c r="G9" s="93">
         <v>0.36430000000000001</v>
       </c>
-      <c r="H9" s="94">
+      <c r="H9" s="93">
         <v>0.43319999999999997</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="95">
+      <c r="C10" s="94">
         <v>-350</v>
       </c>
-      <c r="D10" s="95">
+      <c r="D10" s="94">
         <v>0</v>
       </c>
-      <c r="E10" s="95">
+      <c r="E10" s="94">
         <v>350</v>
       </c>
-      <c r="F10" s="95">
+      <c r="F10" s="94">
         <v>350</v>
       </c>
-      <c r="G10" s="95">
+      <c r="G10" s="94">
         <v>0</v>
       </c>
-      <c r="H10" s="95">
+      <c r="H10" s="94">
         <v>-350</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="92" t="s">
+      <c r="B13" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="99" t="s">
+      <c r="C13" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="99" t="s">
+      <c r="D13" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="99" t="s">
+      <c r="E13" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="F13" s="99"/>
-      <c r="G13" s="92"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="91"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>104</v>
       </c>
-      <c r="C14" s="96">
+      <c r="C14" s="95">
         <f>E10</f>
         <v>350</v>
       </c>
-      <c r="D14" s="94">
+      <c r="D14" s="93">
         <f>F9-E9</f>
         <v>0.68259999999999998</v>
       </c>
-      <c r="E14" s="96">
+      <c r="E14" s="95">
         <f>C14*D14</f>
         <v>238.91</v>
       </c>
-      <c r="F14" s="94"/>
+      <c r="F14" s="93"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="96">
+      <c r="C15" s="95">
         <f>C10*1.05</f>
         <v>-367.5</v>
       </c>
-      <c r="D15" s="94">
+      <c r="D15" s="93">
         <f>100%+C9-H9</f>
         <v>0.1336</v>
       </c>
-      <c r="E15" s="96">
+      <c r="E15" s="95">
         <f>D15*C15</f>
         <v>-49.097999999999999</v>
       </c>
-      <c r="F15" s="94"/>
+      <c r="F15" s="93"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="96">
+      <c r="C16" s="95">
         <v>0</v>
       </c>
-      <c r="D16" s="94">
+      <c r="D16" s="93">
         <f>G9-D9-D14</f>
         <v>4.6000000000000041E-2</v>
       </c>
-      <c r="E16" s="96">
+      <c r="E16" s="95">
         <f t="shared" ref="E16:E17" si="0">D16*C16</f>
         <v>0</v>
       </c>
-      <c r="F16" s="94"/>
+      <c r="F16" s="93"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="96">
+      <c r="C17" s="95">
         <f>C15</f>
         <v>-367.5</v>
       </c>
-      <c r="D17" s="94">
+      <c r="D17" s="93">
         <f>(H9-G9)*2</f>
         <v>0.13779999999999992</v>
       </c>
-      <c r="E17" s="96">
+      <c r="E17" s="95">
         <f t="shared" si="0"/>
         <v>-50.641499999999972</v>
       </c>
-      <c r="F17" s="94"/>
+      <c r="F17" s="93"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="95"/>
-      <c r="D18" s="94"/>
-      <c r="E18" s="95"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="94"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="92" t="s">
+      <c r="B20" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="100" t="s">
+      <c r="C20" s="99" t="s">
         <v>109</v>
       </c>
-      <c r="D20" s="100" t="s">
+      <c r="D20" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="100" t="s">
+      <c r="E20" s="99" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="92" t="s">
+      <c r="B21" s="91" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="96">
+      <c r="C21" s="95">
         <f>SUM(E14:E17)</f>
         <v>139.17050000000003</v>
       </c>
-      <c r="D21" s="97">
+      <c r="D21" s="96">
         <f>C21*21</f>
         <v>2922.5805000000005</v>
       </c>
-      <c r="E21" s="96">
+      <c r="E21" s="95">
         <f>C21*252</f>
         <v>35070.966000000008</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="92" t="s">
+      <c r="B22" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="96">
+      <c r="C22" s="95">
         <f>E10</f>
         <v>350</v>
       </c>
-      <c r="D22" s="97">
+      <c r="D22" s="96">
         <f>C22*21</f>
         <v>7350</v>
       </c>
-      <c r="E22" s="96">
+      <c r="E22" s="95">
         <f>C22*252</f>
         <v>88200</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="92" t="s">
+      <c r="B23" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="98">
+      <c r="C23" s="97">
         <f>C21/C22</f>
         <v>0.39763000000000009</v>
       </c>
-      <c r="D23" s="98">
+      <c r="D23" s="97">
         <f>D21/D22</f>
         <v>0.39763000000000004</v>
       </c>
-      <c r="E23" s="98">
+      <c r="E23" s="97">
         <f>E21/E22</f>
         <v>0.39763000000000009</v>
       </c>

</xml_diff>

<commit_message>
Market Close Sep28/2022 - Update 0DTE Experiment.xlsx
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DB5B01-A397-4D0C-84CD-C9A2FB584513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B9C5DD-226F-41FC-A3C9-859D3D1E22EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34590" yWindow="6255" windowWidth="16560" windowHeight="12045" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
+    <workbookView xWindow="16740" yWindow="1485" windowWidth="16560" windowHeight="12045" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="137">
   <si>
     <t>SPX Open</t>
   </si>
@@ -441,6 +441,15 @@
   </si>
   <si>
     <t>Sep28 3590/3565 Bull Put @ -3.9</t>
+  </si>
+  <si>
+    <t>Sep28 3730/3755 Bear Call @-4.0</t>
+  </si>
+  <si>
+    <t>Sep28 3690/3715 Bear Call @ -13.2</t>
+  </si>
+  <si>
+    <t>SPX Trigger</t>
   </si>
 </sst>
 </file>
@@ -963,6 +972,9 @@
                 <c:pt idx="5">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>44832</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -989,6 +1001,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>866.99999999999955</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>385.99999999999949</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1076,6 +1091,9 @@
                       <c:pt idx="5">
                         <c:v>44831</c:v>
                       </c:pt>
+                      <c:pt idx="6">
+                        <c:v>44832</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1108,6 +1126,9 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>-5.58</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-4.8100000000000005</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1183,6 +1204,9 @@
                       <c:pt idx="5">
                         <c:v>44831</c:v>
                       </c:pt>
+                      <c:pt idx="6">
+                        <c:v>44832</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1215,6 +1239,9 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>22.619999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>21.65</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1290,6 +1317,9 @@
                       <c:pt idx="5">
                         <c:v>44831</c:v>
                       </c:pt>
+                      <c:pt idx="6">
+                        <c:v>44832</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1322,6 +1352,9 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>-0.24668435013262602</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-0.22217090069284068</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1612,6 +1645,9 @@
                 <c:pt idx="5">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>44832</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1639,6 +1675,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>22.619999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.65</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -1725,6 +1764,9 @@
                       <c:pt idx="5">
                         <c:v>44831</c:v>
                       </c:pt>
+                      <c:pt idx="6">
+                        <c:v>44832</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1757,6 +1799,9 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>-0.24668435013262602</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-0.22217090069284068</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1829,6 +1874,9 @@
                       <c:pt idx="5">
                         <c:v>44831</c:v>
                       </c:pt>
+                      <c:pt idx="6">
+                        <c:v>44832</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1861,6 +1909,9 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>866.99999999999955</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>385.99999999999949</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1919,6 +1970,9 @@
                 <c:pt idx="5">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>44832</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1946,6 +2000,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-5.58</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.8100000000000005</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2315,6 +2372,9 @@
                 <c:pt idx="5">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>44832</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -2342,6 +2402,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-0.24668435013262602</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.22217090069284068</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2414,6 +2477,9 @@
                       <c:pt idx="5">
                         <c:v>44831</c:v>
                       </c:pt>
+                      <c:pt idx="6">
+                        <c:v>44832</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2446,6 +2512,9 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>22.619999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>21.65</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2518,6 +2587,9 @@
                       <c:pt idx="5">
                         <c:v>44831</c:v>
                       </c:pt>
+                      <c:pt idx="6">
+                        <c:v>44832</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2550,6 +2622,9 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>866.99999999999955</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>385.99999999999949</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2629,6 +2704,9 @@
                       <c:pt idx="5">
                         <c:v>44831</c:v>
                       </c:pt>
+                      <c:pt idx="6">
+                        <c:v>44832</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2661,6 +2739,9 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>-5.58</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-4.8100000000000005</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4953,7 +5034,7 @@
   <dimension ref="B1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4978,7 +5059,7 @@
         <v>44832</v>
       </c>
       <c r="C2" s="104">
-        <v>1021</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5092,7 +5173,9 @@
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="13">
+        <v>3719.04</v>
+      </c>
       <c r="E10" s="10" t="s">
         <v>26</v>
       </c>
@@ -5108,7 +5191,9 @@
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="13"/>
+      <c r="C11" s="13">
+        <v>3683.17</v>
+      </c>
       <c r="E11" s="15" t="s">
         <v>57</v>
       </c>
@@ -5123,7 +5208,9 @@
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="13">
+        <v>3694.52</v>
+      </c>
       <c r="E12" s="16" t="s">
         <v>59</v>
       </c>
@@ -5301,7 +5388,7 @@
   <dimension ref="B1:N27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5364,14 +5451,14 @@
       </c>
       <c r="F3" s="77">
         <f>COUNTA(Tracker!K:K)-1</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G3" s="79" t="s">
         <v>27</v>
       </c>
       <c r="H3" s="71">
         <f>C7/F3</f>
-        <v>144.49999999999991</v>
+        <v>55.142857142857068</v>
       </c>
       <c r="J3" s="22" t="s">
         <v>86</v>
@@ -5402,7 +5489,7 @@
       </c>
       <c r="G4" s="80">
         <f>F4/F3</f>
-        <v>0.66666666666666663</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="H4" s="71">
         <f>(SUMIF(Tracker!H:H, "&gt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&gt;0", Tracker!H2))/F4*100</f>
@@ -5432,15 +5519,15 @@
       </c>
       <c r="F5" s="77">
         <f>COUNTIF(Tracker!J:J, "&lt;0")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" s="80">
         <f>F5/F3</f>
-        <v>0.33333333333333331</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="H5" s="71">
         <f>IFERROR((SUMIF(Tracker!H:H, "&lt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&lt;0", Tracker!H2))/F5*100, 0)</f>
-        <v>-1272.5000000000002</v>
+        <v>-1008.6666666666667</v>
       </c>
       <c r="J5" s="22" t="s">
         <v>88</v>
@@ -5465,14 +5552,14 @@
       </c>
       <c r="C7" s="71">
         <f>INDEX(Tracker!K:K, COUNTA(Tracker!K:K)+17,1)</f>
-        <v>866.99999999999955</v>
+        <v>385.99999999999949</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>71</v>
       </c>
       <c r="F7" s="75">
         <f>C7/C4</f>
-        <v>3.6610624681979488E-2</v>
+        <v>1.6299539939151175E-2</v>
       </c>
       <c r="G7" s="75"/>
       <c r="J7" s="22" t="s">
@@ -5491,14 +5578,14 @@
       </c>
       <c r="C8" s="71">
         <f>INDEX(Tracker!L:L, COUNTA(Tracker!L:L)+17,1)</f>
-        <v>7073</v>
+        <v>9238</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>76</v>
       </c>
       <c r="F8" s="75">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>3.2983482258239629</v>
+        <v>0.92650490813029029</v>
       </c>
       <c r="G8" s="75"/>
       <c r="J8" s="22" t="s">
@@ -5519,14 +5606,14 @@
       </c>
       <c r="C9" s="75">
         <f>C7/C8</f>
-        <v>0.12257882086808986</v>
+        <v>4.1783935916865064E-2</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>77</v>
       </c>
       <c r="F9" s="75">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>0.50908084058328629</v>
+        <v>0.20326085210232137</v>
       </c>
       <c r="G9" s="75"/>
       <c r="J9" s="22" t="s">
@@ -5569,7 +5656,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5612,15 +5699,15 @@
       </c>
       <c r="C2" s="43">
         <f>Indicator!$C$10</f>
-        <v>0</v>
+        <v>3719.04</v>
       </c>
       <c r="D2" s="43">
         <f>Indicator!$C$11</f>
-        <v>0</v>
+        <v>3683.17</v>
       </c>
       <c r="E2" s="43">
         <f>Indicator!$C$12</f>
-        <v>0</v>
+        <v>3694.52</v>
       </c>
       <c r="F2" s="44">
         <f>Indicator!$C$13</f>
@@ -5632,11 +5719,11 @@
       </c>
       <c r="H2" s="59">
         <f>SUMIF(Trades!A:A,Tracker!A2,Trades!H:H)</f>
-        <v>17.68</v>
+        <v>-4.8100000000000005</v>
       </c>
       <c r="I2" s="60">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A2,  Trades!C:C, "STO")</f>
-        <v>17.68</v>
+        <v>21.65</v>
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="65"/>
@@ -6104,6 +6191,45 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="58">
+        <v>44832</v>
+      </c>
+      <c r="B25" s="42">
+        <v>3651.94</v>
+      </c>
+      <c r="C25" s="42">
+        <v>3719.04</v>
+      </c>
+      <c r="D25" s="42">
+        <v>3683.17</v>
+      </c>
+      <c r="E25" s="42">
+        <v>3694.52</v>
+      </c>
+      <c r="F25" s="41">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="G25" s="41">
+        <v>0.46540855364199385</v>
+      </c>
+      <c r="H25" s="17">
+        <v>-4.8100000000000005</v>
+      </c>
+      <c r="I25" s="61">
+        <v>21.65</v>
+      </c>
+      <c r="J25" s="21">
+        <f t="shared" ref="J25" si="1">H25/I25</f>
+        <v>-0.22217090069284068</v>
+      </c>
+      <c r="K25" s="65">
+        <f>K24+H25*100</f>
+        <v>385.99999999999949</v>
+      </c>
+      <c r="L25">
+        <f>I25*100+L24</f>
+        <v>9238</v>
+      </c>
       <c r="M25" s="68" t="s">
         <v>130</v>
       </c>
@@ -6119,10 +6245,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6139,9 +6265,10 @@
     <col min="10" max="10" width="14.85546875" style="72" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" style="52" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.28515625" style="72" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="91" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="84" t="s">
         <v>30</v>
       </c>
@@ -6178,8 +6305,11 @@
       <c r="L1" s="90" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="91" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="48">
         <v>44824</v>
       </c>
@@ -6213,7 +6343,7 @@
         <v>-12.809999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="48">
         <v>44824</v>
       </c>
@@ -6247,7 +6377,7 @@
         <v>-9.06</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="48">
         <v>44825</v>
       </c>
@@ -6288,7 +6418,7 @@
         <v>-1.2925</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="48">
         <v>44825</v>
       </c>
@@ -6312,7 +6442,7 @@
         <v>-1.33</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="48">
         <v>44826</v>
       </c>
@@ -6346,7 +6476,7 @@
         <v>-14.91</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="48">
         <v>44826</v>
       </c>
@@ -6380,7 +6510,7 @@
         <v>-7.11</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="48">
         <v>44827</v>
       </c>
@@ -6414,7 +6544,7 @@
         <v>-19.41</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="48">
         <v>44827</v>
       </c>
@@ -6448,7 +6578,7 @@
         <v>-11.91</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="48">
         <v>44827</v>
       </c>
@@ -6472,7 +6602,7 @@
         <v>-12.43</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="48">
         <v>44827</v>
       </c>
@@ -6496,7 +6626,7 @@
         <v>-20.100000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="48">
         <v>44827</v>
       </c>
@@ -6530,7 +6660,7 @@
         <v>-6.66</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="48">
         <v>44830</v>
       </c>
@@ -6564,7 +6694,7 @@
         <v>-12.809999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="48">
         <v>44830</v>
       </c>
@@ -6598,7 +6728,7 @@
         <v>-9.81</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="48">
         <v>44830</v>
       </c>
@@ -6632,7 +6762,7 @@
         <v>-4.41</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="48">
         <v>44831</v>
       </c>
@@ -6666,7 +6796,7 @@
         <v>-10.11</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="48">
         <v>44831</v>
       </c>
@@ -6700,7 +6830,7 @@
         <v>-11.61</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="48">
         <v>44831</v>
       </c>
@@ -6734,7 +6864,7 @@
         <v>-8.91</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="48">
         <v>44831</v>
       </c>
@@ -6754,11 +6884,11 @@
         <v>-14.1</v>
       </c>
       <c r="H19" s="51">
-        <f t="shared" ref="H19:H23" si="6">G19*F19</f>
+        <f t="shared" ref="H19:H25" si="6">G19*F19</f>
         <v>-28.2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="48">
         <v>44831</v>
       </c>
@@ -6792,7 +6922,7 @@
         <v>-13.559999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="48">
         <v>44832</v>
       </c>
@@ -6826,7 +6956,7 @@
         <v>-12.809999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="48">
         <v>44832</v>
       </c>
@@ -6860,7 +6990,7 @@
         <v>-15.809999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="48">
         <v>44832</v>
       </c>
@@ -6892,6 +7022,67 @@
       <c r="J23" s="72">
         <f t="shared" si="8"/>
         <v>-11.61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="48">
+        <v>44832</v>
+      </c>
+      <c r="B24" s="49">
+        <v>1212</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="103" t="s">
+        <v>135</v>
+      </c>
+      <c r="F24" s="31">
+        <v>2</v>
+      </c>
+      <c r="G24" s="50">
+        <v>-13.23</v>
+      </c>
+      <c r="H24" s="51">
+        <f t="shared" si="6"/>
+        <v>-26.46</v>
+      </c>
+      <c r="M24">
+        <v>3702</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="48">
+        <v>44832</v>
+      </c>
+      <c r="B25" s="49">
+        <v>1318</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="103" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" s="101">
+        <v>0.3</v>
+      </c>
+      <c r="F25" s="31">
+        <v>1</v>
+      </c>
+      <c r="G25" s="50">
+        <v>3.97</v>
+      </c>
+      <c r="H25" s="51">
+        <f t="shared" si="6"/>
+        <v>3.97</v>
+      </c>
+      <c r="I25" s="52">
+        <v>3</v>
+      </c>
+      <c r="J25" s="72">
+        <f t="shared" ref="J25" si="9">-I25*G25</f>
+        <v>-11.91</v>
       </c>
     </row>
   </sheetData>
@@ -6902,10 +7093,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE4BC4F-EB6D-4F7C-A4AB-32C246F0D899}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6988,7 +7179,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="51">
-        <f t="shared" ref="H2:H8" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H9" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="52">
@@ -7000,7 +7191,7 @@
       </c>
       <c r="N2" s="72">
         <f>SUM(H:H)</f>
-        <v>13.44</v>
+        <v>0.20999999999999908</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -7195,6 +7386,30 @@
       <c r="J8" s="72">
         <f t="shared" si="3"/>
         <v>-15.809999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="48">
+        <v>44832</v>
+      </c>
+      <c r="B9" s="49">
+        <v>1212</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="103" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="31">
+        <v>1</v>
+      </c>
+      <c r="G9" s="50">
+        <v>-13.23</v>
+      </c>
+      <c r="H9" s="51">
+        <f t="shared" si="0"/>
+        <v>-13.23</v>
       </c>
     </row>
   </sheetData>
@@ -7204,10 +7419,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5E4B5F-C3CE-4821-8081-9385439A4F7E}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7290,7 +7505,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="51">
-        <f t="shared" ref="H2:H8" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H9" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="52">
@@ -7302,7 +7517,7 @@
       </c>
       <c r="N2" s="72">
         <f>SUM(H:H)</f>
-        <v>10.239999999999998</v>
+        <v>-2.990000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -7497,6 +7712,30 @@
       <c r="J8" s="72">
         <f t="shared" si="4"/>
         <v>-11.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="48">
+        <v>44832</v>
+      </c>
+      <c r="B9" s="49">
+        <v>1212</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="103" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="31">
+        <v>1</v>
+      </c>
+      <c r="G9" s="50">
+        <v>-13.23</v>
+      </c>
+      <c r="H9" s="51">
+        <f t="shared" si="0"/>
+        <v>-13.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Market Open Sep29/2022 - Update 0DTE Experiment.xlsx
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B9C5DD-226F-41FC-A3C9-859D3D1E22EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F2178D-F441-4A46-AC88-68066B720BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16740" yWindow="1485" windowWidth="16560" windowHeight="12045" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
+    <workbookView xWindow="22440" yWindow="1890" windowWidth="16560" windowHeight="12045" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="140">
   <si>
     <t>SPX Open</t>
   </si>
@@ -450,6 +450,15 @@
   </si>
   <si>
     <t>SPX Trigger</t>
+  </si>
+  <si>
+    <t>Sep29 3715/3740 Bear Call @-4.3</t>
+  </si>
+  <si>
+    <t>Sep29 3610/3585 Bull Put @ -3.9</t>
+  </si>
+  <si>
+    <t>Sep29 3595/3570 Bull Put @ -2.5</t>
   </si>
 </sst>
 </file>
@@ -5034,7 +5043,7 @@
   <dimension ref="B1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5056,10 +5065,10 @@
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="20">
-        <v>44832</v>
+        <v>44833</v>
       </c>
       <c r="C2" s="104">
-        <v>2340</v>
+        <v>952</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5088,14 +5097,14 @@
         <v>3</v>
       </c>
       <c r="C5" s="12">
-        <v>3686.44</v>
+        <v>3651.94</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="27">
         <f>(C9-C18)/(C17-C18)</f>
-        <v>0.53430290619708476</v>
+        <v>0.25759182850951268</v>
       </c>
       <c r="G5" s="25">
         <v>0.4</v>
@@ -5107,14 +5116,14 @@
         <v>4</v>
       </c>
       <c r="C6" s="13">
-        <v>3647.29</v>
+        <v>3719.04</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="27">
         <f>(C9-C23)/(C22-C23)</f>
-        <v>0.50401228645558727</v>
+        <v>0.52074988185941773</v>
       </c>
       <c r="G6" s="25">
         <v>0.33</v>
@@ -5126,14 +5135,14 @@
         <v>12</v>
       </c>
       <c r="C7" s="13">
-        <v>3651.17</v>
+        <v>3683.17</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="28">
         <f>(C9-C28)/(C27-C28)</f>
-        <v>0.31616050604746726</v>
+        <v>0.47502542963644029</v>
       </c>
       <c r="G7" s="26">
         <v>0.27</v>
@@ -5145,14 +5154,14 @@
         <v>10</v>
       </c>
       <c r="C8" s="13">
-        <v>3708.7</v>
+        <v>3694.52</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="29">
         <f>F5*G5+F6*G6+F7*G7</f>
-        <v>0.46540855364199385</v>
+        <v>0.40314105841925185</v>
       </c>
       <c r="G8" s="24" t="s">
         <v>27</v>
@@ -5164,7 +5173,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="12">
-        <v>3651.94</v>
+        <v>3687.01</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -5173,9 +5182,7 @@
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13">
-        <v>3719.04</v>
-      </c>
+      <c r="C10" s="13"/>
       <c r="E10" s="10" t="s">
         <v>26</v>
       </c>
@@ -5191,9 +5198,7 @@
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="13">
-        <v>3683.17</v>
-      </c>
+      <c r="C11" s="13"/>
       <c r="E11" s="15" t="s">
         <v>57</v>
       </c>
@@ -5208,9 +5213,7 @@
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13">
-        <v>3694.52</v>
-      </c>
+      <c r="C12" s="13"/>
       <c r="E12" s="16" t="s">
         <v>59</v>
       </c>
@@ -5226,7 +5229,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="14">
-        <v>0.29499999999999998</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>60</v>
@@ -5270,7 +5273,7 @@
       </c>
       <c r="C16" s="4">
         <f>C6*C$13*SQRT((24/24)/252)</f>
-        <v>67.778513769123037</v>
+        <v>66.066254703911113</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>62</v>
@@ -5288,7 +5291,7 @@
       </c>
       <c r="C17" s="4">
         <f>C6+C16</f>
-        <v>3715.068513769123</v>
+        <v>3785.106254703911</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>58</v>
@@ -5306,7 +5309,7 @@
       </c>
       <c r="C18" s="6">
         <f>C6-C16</f>
-        <v>3579.5114862308769</v>
+        <v>3652.973745296089</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5322,7 +5325,7 @@
       </c>
       <c r="C21" s="4">
         <f>C7*C$13*(2/252)^0.5</f>
-        <v>95.955262482283004</v>
+        <v>92.530647307210899</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -5331,7 +5334,7 @@
       </c>
       <c r="C22" s="4">
         <f>C7+C21</f>
-        <v>3747.1252624822832</v>
+        <v>3775.7006473072111</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5340,7 +5343,7 @@
       </c>
       <c r="C23" s="6">
         <f>C7-C21</f>
-        <v>3555.2147375177169</v>
+        <v>3590.6393526927891</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5356,7 +5359,7 @@
       </c>
       <c r="C26" s="4">
         <f>C17*C$13*(5/252)^0.5</f>
-        <v>154.37379308347943</v>
+        <v>150.35293682083889</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -5365,7 +5368,7 @@
       </c>
       <c r="C27" s="4">
         <f>C8+C26</f>
-        <v>3863.0737930834794</v>
+        <v>3844.8729368208387</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5374,7 +5377,7 @@
       </c>
       <c r="C28" s="6">
         <f>C8-C26</f>
-        <v>3554.3262069165203</v>
+        <v>3544.1670631791612</v>
       </c>
     </row>
   </sheetData>
@@ -5585,7 +5588,7 @@
       </c>
       <c r="F8" s="75">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>0.92650490813029029</v>
+        <v>0.80423501851936674</v>
       </c>
       <c r="G8" s="75"/>
       <c r="J8" s="22" t="s">
@@ -5613,7 +5616,7 @@
       </c>
       <c r="F9" s="75">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>0.20326085210232137</v>
+        <v>0.18120100691399932</v>
       </c>
       <c r="G9" s="75"/>
       <c r="J9" s="22" t="s">
@@ -5691,39 +5694,39 @@
     <row r="2" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="58">
         <f>Indicator!B2</f>
-        <v>44832</v>
+        <v>44833</v>
       </c>
       <c r="B2" s="43">
         <f>Indicator!$C$9</f>
-        <v>3651.94</v>
+        <v>3687.01</v>
       </c>
       <c r="C2" s="43">
         <f>Indicator!$C$10</f>
-        <v>3719.04</v>
+        <v>0</v>
       </c>
       <c r="D2" s="43">
         <f>Indicator!$C$11</f>
-        <v>3683.17</v>
+        <v>0</v>
       </c>
       <c r="E2" s="43">
         <f>Indicator!$C$12</f>
-        <v>3694.52</v>
+        <v>0</v>
       </c>
       <c r="F2" s="44">
         <f>Indicator!$C$13</f>
-        <v>0.29499999999999998</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="G2" s="44">
         <f>Indicator!$F$8</f>
-        <v>0.46540855364199385</v>
+        <v>0.40314105841925185</v>
       </c>
       <c r="H2" s="59">
         <f>SUMIF(Trades!A:A,Tracker!A2,Trades!H:H)</f>
-        <v>-4.8100000000000005</v>
+        <v>14.88</v>
       </c>
       <c r="I2" s="60">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A2,  Trades!C:C, "STO")</f>
-        <v>21.65</v>
+        <v>14.88</v>
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="65"/>
@@ -6009,11 +6012,11 @@
         <v>0.74274661508704065</v>
       </c>
       <c r="K20" s="65">
-        <f>K19+H20*100</f>
+        <f t="shared" ref="K20:K25" si="1">K19+H20*100</f>
         <v>1113</v>
       </c>
       <c r="L20">
-        <f>I20*100+L19</f>
+        <f t="shared" ref="L20:L25" si="2">I20*100+L19</f>
         <v>1246</v>
       </c>
       <c r="M20" s="17" t="s">
@@ -6053,11 +6056,11 @@
         <v>1</v>
       </c>
       <c r="K21" s="65">
-        <f>K20+H21*100</f>
+        <f t="shared" si="1"/>
         <v>2084</v>
       </c>
       <c r="L21">
-        <f>I21*100+L20</f>
+        <f t="shared" si="2"/>
         <v>2217</v>
       </c>
     </row>
@@ -6094,11 +6097,11 @@
         <v>-1.5695102685624016</v>
       </c>
       <c r="K22" s="65">
-        <f>K21+H22*100</f>
+        <f t="shared" si="1"/>
         <v>96.999999999999545</v>
       </c>
       <c r="L22">
-        <f>I22*100+L21</f>
+        <f t="shared" si="2"/>
         <v>3483</v>
       </c>
       <c r="M22" s="17" t="s">
@@ -6138,11 +6141,11 @@
         <v>1</v>
       </c>
       <c r="K23" s="65">
-        <f>K22+H23*100</f>
+        <f t="shared" si="1"/>
         <v>1424.9999999999995</v>
       </c>
       <c r="L23">
-        <f>I23*100+L22</f>
+        <f t="shared" si="2"/>
         <v>4811</v>
       </c>
     </row>
@@ -6179,11 +6182,11 @@
         <v>-0.24668435013262602</v>
       </c>
       <c r="K24" s="65">
-        <f>K23+H24*100</f>
+        <f t="shared" si="1"/>
         <v>866.99999999999955</v>
       </c>
       <c r="L24">
-        <f>I24*100+L23</f>
+        <f t="shared" si="2"/>
         <v>7073</v>
       </c>
       <c r="M24" s="17" t="s">
@@ -6219,15 +6222,15 @@
         <v>21.65</v>
       </c>
       <c r="J25" s="21">
-        <f t="shared" ref="J25" si="1">H25/I25</f>
+        <f t="shared" ref="J25" si="3">H25/I25</f>
         <v>-0.22217090069284068</v>
       </c>
       <c r="K25" s="65">
-        <f>K24+H25*100</f>
+        <f t="shared" si="1"/>
         <v>385.99999999999949</v>
       </c>
       <c r="L25">
-        <f>I25*100+L24</f>
+        <f t="shared" si="2"/>
         <v>9238</v>
       </c>
       <c r="M25" s="68" t="s">
@@ -6245,10 +6248,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6884,7 +6887,7 @@
         <v>-14.1</v>
       </c>
       <c r="H19" s="51">
-        <f t="shared" ref="H19:H25" si="6">G19*F19</f>
+        <f t="shared" ref="H19:H28" si="6">G19*F19</f>
         <v>-28.2</v>
       </c>
     </row>
@@ -7083,6 +7086,87 @@
       <c r="J25" s="72">
         <f t="shared" ref="J25" si="9">-I25*G25</f>
         <v>-11.91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="48">
+        <v>44833</v>
+      </c>
+      <c r="B26" s="49">
+        <v>933</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="103" t="s">
+        <v>137</v>
+      </c>
+      <c r="E26" s="101">
+        <v>-0.15</v>
+      </c>
+      <c r="F26" s="31">
+        <v>2</v>
+      </c>
+      <c r="G26" s="50">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="H26" s="51">
+        <f t="shared" si="6"/>
+        <v>8.5399999999999991</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="48">
+        <v>44833</v>
+      </c>
+      <c r="B27" s="49">
+        <v>943</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="103" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" s="101">
+        <v>0.15</v>
+      </c>
+      <c r="F27" s="31">
+        <v>1</v>
+      </c>
+      <c r="G27" s="50">
+        <v>3.87</v>
+      </c>
+      <c r="H27" s="51">
+        <f t="shared" si="6"/>
+        <v>3.87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="48">
+        <v>44833</v>
+      </c>
+      <c r="B28" s="49">
+        <v>944</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="103" t="s">
+        <v>139</v>
+      </c>
+      <c r="E28" s="101">
+        <v>0.09</v>
+      </c>
+      <c r="F28" s="31">
+        <v>1</v>
+      </c>
+      <c r="G28" s="50">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="H28" s="51">
+        <f t="shared" si="6"/>
+        <v>2.4700000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Market Close Sep29/2022 - Update 0DTE Experiment.xlsx
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F2178D-F441-4A46-AC88-68066B720BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6424CDE3-1A91-47E4-B3DB-6C63B2B42926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22440" yWindow="1890" windowWidth="16560" windowHeight="12045" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
+    <workbookView xWindow="27465" yWindow="2070" windowWidth="19035" windowHeight="17100" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="143">
   <si>
     <t>SPX Open</t>
   </si>
@@ -459,6 +459,15 @@
   </si>
   <si>
     <t>Sep29 3595/3570 Bull Put @ -2.5</t>
+  </si>
+  <si>
+    <t>Sep29 3610/3585 Bull Put @ -7.2</t>
+  </si>
+  <si>
+    <t>BTC</t>
+  </si>
+  <si>
+    <t>Sep29 3580/3555 Bull Put @ -2.8</t>
   </si>
 </sst>
 </file>
@@ -870,6 +879,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF800000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -984,6 +998,9 @@
                 <c:pt idx="6">
                   <c:v>44832</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>44833</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1013,6 +1030,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>385.99999999999949</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1427.9999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1103,6 +1123,9 @@
                       <c:pt idx="6">
                         <c:v>44832</c:v>
                       </c:pt>
+                      <c:pt idx="7">
+                        <c:v>44833</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1138,6 +1161,9 @@
                       </c:pt>
                       <c:pt idx="6">
                         <c:v>-4.8100000000000005</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>10.42</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1216,6 +1242,9 @@
                       <c:pt idx="6">
                         <c:v>44832</c:v>
                       </c:pt>
+                      <c:pt idx="7">
+                        <c:v>44833</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1251,6 +1280,9 @@
                       </c:pt>
                       <c:pt idx="6">
                         <c:v>21.65</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>17.650000000000002</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1329,6 +1361,9 @@
                       <c:pt idx="6">
                         <c:v>44832</c:v>
                       </c:pt>
+                      <c:pt idx="7">
+                        <c:v>44833</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1364,6 +1399,9 @@
                       </c:pt>
                       <c:pt idx="6">
                         <c:v>-0.22217090069284068</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.59036827195467412</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1622,7 +1660,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
             <a:ln w="25400">
               <a:noFill/>
@@ -1657,6 +1695,9 @@
                 <c:pt idx="6">
                   <c:v>44832</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>44833</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1687,6 +1728,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>21.65</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.650000000000002</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -1776,6 +1820,9 @@
                       <c:pt idx="6">
                         <c:v>44832</c:v>
                       </c:pt>
+                      <c:pt idx="7">
+                        <c:v>44833</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1811,6 +1858,9 @@
                       </c:pt>
                       <c:pt idx="6">
                         <c:v>-0.22217090069284068</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.59036827195467412</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1886,6 +1936,9 @@
                       <c:pt idx="6">
                         <c:v>44832</c:v>
                       </c:pt>
+                      <c:pt idx="7">
+                        <c:v>44833</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1921,6 +1974,9 @@
                       </c:pt>
                       <c:pt idx="6">
                         <c:v>385.99999999999949</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1427.9999999999995</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1947,14 +2003,14 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:srgbClr val="70AD47"/>
             </a:solidFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:invertIfNegative val="1"/>
           <c:cat>
             <c:numRef>
               <c:f>Tracker!$A$19:$A$714</c:f>
@@ -1981,6 +2037,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>44832</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44833</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2013,11 +2072,27 @@
                 <c:pt idx="6">
                   <c:v>-4.8100000000000005</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.42</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:val>
           <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="C00000"/>
+                  </a:solidFill>
+                  <a:ln w="25400">
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-68A7-4CF3-92F1-579C12FDEE2D}"/>
             </c:ext>
@@ -2384,6 +2459,9 @@
                 <c:pt idx="6">
                   <c:v>44832</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>44833</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -2414,6 +2492,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-0.22217090069284068</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.59036827195467412</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2489,6 +2570,9 @@
                       <c:pt idx="6">
                         <c:v>44832</c:v>
                       </c:pt>
+                      <c:pt idx="7">
+                        <c:v>44833</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2524,6 +2608,9 @@
                       </c:pt>
                       <c:pt idx="6">
                         <c:v>21.65</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>17.650000000000002</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2599,6 +2686,9 @@
                       <c:pt idx="6">
                         <c:v>44832</c:v>
                       </c:pt>
+                      <c:pt idx="7">
+                        <c:v>44833</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2634,6 +2724,9 @@
                       </c:pt>
                       <c:pt idx="6">
                         <c:v>385.99999999999949</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1427.9999999999995</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2716,6 +2809,9 @@
                       <c:pt idx="6">
                         <c:v>44832</c:v>
                       </c:pt>
+                      <c:pt idx="7">
+                        <c:v>44833</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2751,6 +2847,9 @@
                       </c:pt>
                       <c:pt idx="6">
                         <c:v>-4.8100000000000005</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>10.42</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -5043,7 +5142,7 @@
   <dimension ref="B1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5068,7 +5167,7 @@
         <v>44833</v>
       </c>
       <c r="C2" s="104">
-        <v>952</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5182,7 +5281,9 @@
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="13">
+        <v>3640.71</v>
+      </c>
       <c r="E10" s="10" t="s">
         <v>26</v>
       </c>
@@ -5198,7 +5299,9 @@
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="13"/>
+      <c r="C11" s="13">
+        <v>3679.88</v>
+      </c>
       <c r="E11" s="15" t="s">
         <v>57</v>
       </c>
@@ -5213,7 +5316,9 @@
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="13">
+        <v>3671.06</v>
+      </c>
       <c r="E12" s="16" t="s">
         <v>59</v>
       </c>
@@ -5391,7 +5496,7 @@
   <dimension ref="B1:N27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5454,14 +5559,14 @@
       </c>
       <c r="F3" s="77">
         <f>COUNTA(Tracker!K:K)-1</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" s="79" t="s">
         <v>27</v>
       </c>
       <c r="H3" s="71">
         <f>C7/F3</f>
-        <v>55.142857142857068</v>
+        <v>178.49999999999994</v>
       </c>
       <c r="J3" s="22" t="s">
         <v>86</v>
@@ -5488,15 +5593,15 @@
       </c>
       <c r="F4" s="77">
         <f>COUNTIF(Tracker!J:J, "&gt;0")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G4" s="80">
         <f>F4/F3</f>
-        <v>0.5714285714285714</v>
+        <v>0.625</v>
       </c>
       <c r="H4" s="71">
         <f>(SUMIF(Tracker!H:H, "&gt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&gt;0", Tracker!H2))/F4*100</f>
-        <v>852.99999999999989</v>
+        <v>890.8</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>87</v>
@@ -5526,7 +5631,7 @@
       </c>
       <c r="G5" s="80">
         <f>F5/F3</f>
-        <v>0.42857142857142855</v>
+        <v>0.375</v>
       </c>
       <c r="H5" s="71">
         <f>IFERROR((SUMIF(Tracker!H:H, "&lt;0", Tracker!H:H)-SUMIF(Tracker!H2,"&lt;0", Tracker!H2))/F5*100, 0)</f>
@@ -5555,14 +5660,14 @@
       </c>
       <c r="C7" s="71">
         <f>INDEX(Tracker!K:K, COUNTA(Tracker!K:K)+17,1)</f>
-        <v>385.99999999999949</v>
+        <v>1427.9999999999995</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>71</v>
       </c>
       <c r="F7" s="75">
         <f>C7/C4</f>
-        <v>1.6299539939151175E-2</v>
+        <v>6.0299852417377987E-2</v>
       </c>
       <c r="G7" s="75"/>
       <c r="J7" s="22" t="s">
@@ -5581,14 +5686,14 @@
       </c>
       <c r="C8" s="71">
         <f>INDEX(Tracker!L:L, COUNTA(Tracker!L:L)+17,1)</f>
-        <v>9238</v>
+        <v>11003</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>76</v>
       </c>
       <c r="F8" s="75">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>0.80423501851936674</v>
+        <v>7.4751537377037973</v>
       </c>
       <c r="G8" s="75"/>
       <c r="J8" s="22" t="s">
@@ -5609,14 +5714,14 @@
       </c>
       <c r="C9" s="75">
         <f>C7/C8</f>
-        <v>4.1783935916865064E-2</v>
+        <v>0.1297827865127692</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>77</v>
       </c>
       <c r="F9" s="75">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>0.18120100691399932</v>
+        <v>0.82774506460251418</v>
       </c>
       <c r="G9" s="75"/>
       <c r="J9" s="22" t="s">
@@ -5656,10 +5761,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C82D01-CC02-4066-B9D6-9DFF5A0A89C9}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5702,15 +5807,15 @@
       </c>
       <c r="C2" s="43">
         <f>Indicator!$C$10</f>
-        <v>0</v>
+        <v>3640.71</v>
       </c>
       <c r="D2" s="43">
         <f>Indicator!$C$11</f>
-        <v>0</v>
+        <v>3679.88</v>
       </c>
       <c r="E2" s="43">
         <f>Indicator!$C$12</f>
-        <v>0</v>
+        <v>3671.06</v>
       </c>
       <c r="F2" s="44">
         <f>Indicator!$C$13</f>
@@ -5722,11 +5827,11 @@
       </c>
       <c r="H2" s="59">
         <f>SUMIF(Trades!A:A,Tracker!A2,Trades!H:H)</f>
-        <v>14.88</v>
+        <v>10.42</v>
       </c>
       <c r="I2" s="60">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A2,  Trades!C:C, "STO")</f>
-        <v>14.88</v>
+        <v>17.650000000000002</v>
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="65"/>
@@ -6237,6 +6342,47 @@
         <v>130</v>
       </c>
     </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="58">
+        <v>44833</v>
+      </c>
+      <c r="B26" s="42">
+        <v>3687.01</v>
+      </c>
+      <c r="C26" s="42">
+        <v>3640.71</v>
+      </c>
+      <c r="D26" s="42">
+        <v>3679.88</v>
+      </c>
+      <c r="E26" s="42">
+        <v>3671.06</v>
+      </c>
+      <c r="F26" s="41">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="G26" s="41">
+        <v>0.40314105841925185</v>
+      </c>
+      <c r="H26" s="17">
+        <v>10.42</v>
+      </c>
+      <c r="I26" s="61">
+        <v>17.650000000000002</v>
+      </c>
+      <c r="J26" s="21">
+        <f t="shared" ref="J26" si="4">H26/I26</f>
+        <v>0.59036827195467412</v>
+      </c>
+      <c r="K26" s="65">
+        <f t="shared" ref="K26" si="5">K25+H26*100</f>
+        <v>1427.9999999999995</v>
+      </c>
+      <c r="L26">
+        <f t="shared" ref="L26" si="6">I26*100+L25</f>
+        <v>11003</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:C18">
     <sortCondition ref="A5:A18"/>
@@ -6248,10 +6394,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6887,7 +7033,7 @@
         <v>-14.1</v>
       </c>
       <c r="H19" s="51">
-        <f t="shared" ref="H19:H28" si="6">G19*F19</f>
+        <f t="shared" ref="H19:H30" si="6">G19*F19</f>
         <v>-28.2</v>
       </c>
     </row>
@@ -7167,6 +7313,57 @@
       <c r="H28" s="51">
         <f t="shared" si="6"/>
         <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="48">
+        <v>44833</v>
+      </c>
+      <c r="B29" s="49">
+        <v>1016</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="103" t="s">
+        <v>140</v>
+      </c>
+      <c r="F29" s="31">
+        <v>1</v>
+      </c>
+      <c r="G29" s="50">
+        <v>-7.23</v>
+      </c>
+      <c r="H29" s="51">
+        <f t="shared" si="6"/>
+        <v>-7.23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="48">
+        <v>44833</v>
+      </c>
+      <c r="B30" s="49">
+        <v>1035</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="103" t="s">
+        <v>142</v>
+      </c>
+      <c r="E30" s="101">
+        <v>0.15</v>
+      </c>
+      <c r="F30" s="31">
+        <v>1</v>
+      </c>
+      <c r="G30" s="50">
+        <v>2.77</v>
+      </c>
+      <c r="H30" s="51">
+        <f t="shared" si="6"/>
+        <v>2.77</v>
       </c>
     </row>
   </sheetData>
@@ -7177,10 +7374,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE4BC4F-EB6D-4F7C-A4AB-32C246F0D899}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7263,7 +7460,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="51">
-        <f t="shared" ref="H2:H9" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H11" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="52">
@@ -7275,7 +7472,7 @@
       </c>
       <c r="N2" s="72">
         <f>SUM(H:H)</f>
-        <v>0.20999999999999908</v>
+        <v>8.3499999999999979</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -7494,6 +7691,74 @@
       <c r="H9" s="51">
         <f t="shared" si="0"/>
         <v>-13.23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="48">
+        <v>44833</v>
+      </c>
+      <c r="B10" s="49">
+        <v>933</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="103" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="101">
+        <v>-0.15</v>
+      </c>
+      <c r="F10" s="31">
+        <v>1</v>
+      </c>
+      <c r="G10" s="50">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="H10" s="51">
+        <f t="shared" si="0"/>
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="I10" s="52">
+        <v>3</v>
+      </c>
+      <c r="J10" s="72">
+        <f t="shared" ref="J10:J11" si="4">-I10*G10</f>
+        <v>-12.809999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="48">
+        <v>44833</v>
+      </c>
+      <c r="B11" s="49">
+        <v>943</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="103" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="101">
+        <v>0.15</v>
+      </c>
+      <c r="F11" s="31">
+        <v>1</v>
+      </c>
+      <c r="G11" s="50">
+        <v>3.87</v>
+      </c>
+      <c r="H11" s="51">
+        <f t="shared" si="0"/>
+        <v>3.87</v>
+      </c>
+      <c r="I11" s="52">
+        <v>3</v>
+      </c>
+      <c r="J11" s="72">
+        <f t="shared" si="4"/>
+        <v>-11.61</v>
       </c>
     </row>
   </sheetData>
@@ -7503,10 +7768,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5E4B5F-C3CE-4821-8081-9385439A4F7E}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7589,7 +7854,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="51">
-        <f t="shared" ref="H2:H9" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H11" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="52">
@@ -7601,7 +7866,7 @@
       </c>
       <c r="N2" s="72">
         <f>SUM(H:H)</f>
-        <v>-2.990000000000002</v>
+        <v>3.7499999999999978</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -7820,6 +8085,74 @@
       <c r="H9" s="51">
         <f t="shared" si="0"/>
         <v>-13.23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="48">
+        <v>44833</v>
+      </c>
+      <c r="B10" s="49">
+        <v>933</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="103" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="101">
+        <v>-0.15</v>
+      </c>
+      <c r="F10" s="31">
+        <v>1</v>
+      </c>
+      <c r="G10" s="50">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="H10" s="51">
+        <f t="shared" si="0"/>
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="I10" s="52">
+        <v>3</v>
+      </c>
+      <c r="J10" s="72">
+        <f t="shared" ref="J10:J11" si="5">-I10*G10</f>
+        <v>-12.809999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="48">
+        <v>44833</v>
+      </c>
+      <c r="B11" s="49">
+        <v>944</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="103" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="101">
+        <v>0.09</v>
+      </c>
+      <c r="F11" s="31">
+        <v>1</v>
+      </c>
+      <c r="G11" s="50">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="H11" s="51">
+        <f t="shared" si="0"/>
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="I11" s="52">
+        <v>3</v>
+      </c>
+      <c r="J11" s="72">
+        <f t="shared" si="5"/>
+        <v>-7.41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Market Close Oct 06 2022
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F3C30D-17FB-4019-90F5-782CF69DA42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E788F3F-E874-4334-B101-864CF7734D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="4155" windowWidth="20505" windowHeight="14460" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
+    <workbookView xWindow="10260" yWindow="2610" windowWidth="20505" windowHeight="14460" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator" sheetId="1" r:id="rId1"/>
@@ -980,6 +980,9 @@
                 <c:pt idx="11">
                   <c:v>44839</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1024,6 +1027,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>-1499.0000000000009</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-491.00000000000091</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1129,6 +1135,9 @@
                       <c:pt idx="11">
                         <c:v>44839</c:v>
                       </c:pt>
+                      <c:pt idx="12">
+                        <c:v>44840</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1179,6 +1188,9 @@
                       </c:pt>
                       <c:pt idx="11">
                         <c:v>-7.08</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>10.08</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1272,6 +1284,9 @@
                       <c:pt idx="11">
                         <c:v>44839</c:v>
                       </c:pt>
+                      <c:pt idx="12">
+                        <c:v>44840</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1322,6 +1337,9 @@
                       </c:pt>
                       <c:pt idx="11">
                         <c:v>12.08</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>10.08</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1415,6 +1433,9 @@
                       <c:pt idx="11">
                         <c:v>44839</c:v>
                       </c:pt>
+                      <c:pt idx="12">
+                        <c:v>44840</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1465,6 +1486,9 @@
                       </c:pt>
                       <c:pt idx="11">
                         <c:v>-0.58609271523178808</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>1</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1773,6 +1797,9 @@
                 <c:pt idx="11">
                   <c:v>44839</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1818,6 +1845,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12.08</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.08</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -1922,6 +1952,9 @@
                       <c:pt idx="11">
                         <c:v>44839</c:v>
                       </c:pt>
+                      <c:pt idx="12">
+                        <c:v>44840</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1972,6 +2005,9 @@
                       </c:pt>
                       <c:pt idx="11">
                         <c:v>-0.58609271523178808</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>1</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2062,6 +2098,9 @@
                       <c:pt idx="11">
                         <c:v>44839</c:v>
                       </c:pt>
+                      <c:pt idx="12">
+                        <c:v>44840</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2112,6 +2151,9 @@
                       </c:pt>
                       <c:pt idx="11">
                         <c:v>-1499.0000000000009</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>-491.00000000000091</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2188,6 +2230,9 @@
                 <c:pt idx="11">
                   <c:v>44839</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -2233,6 +2278,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>-7.08</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.08</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2633,6 +2681,9 @@
                 <c:pt idx="11">
                   <c:v>44839</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -2678,6 +2729,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>-0.58609271523178808</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2768,6 +2822,9 @@
                       <c:pt idx="11">
                         <c:v>44839</c:v>
                       </c:pt>
+                      <c:pt idx="12">
+                        <c:v>44840</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2818,6 +2875,9 @@
                       </c:pt>
                       <c:pt idx="11">
                         <c:v>12.08</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>10.08</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2908,6 +2968,9 @@
                       <c:pt idx="11">
                         <c:v>44839</c:v>
                       </c:pt>
+                      <c:pt idx="12">
+                        <c:v>44840</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2958,6 +3021,9 @@
                       </c:pt>
                       <c:pt idx="11">
                         <c:v>-1499.0000000000009</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>-491.00000000000091</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3055,6 +3121,9 @@
                       <c:pt idx="11">
                         <c:v>44839</c:v>
                       </c:pt>
+                      <c:pt idx="12">
+                        <c:v>44840</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -3105,6 +3174,9 @@
                       </c:pt>
                       <c:pt idx="11">
                         <c:v>-7.08</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>10.08</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -5398,7 +5470,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5422,7 +5494,7 @@
         <v>44840</v>
       </c>
       <c r="C2" s="67">
-        <v>1010</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -5448,7 +5520,7 @@
       </c>
       <c r="F5" s="80">
         <f>SUM(F26:F28)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5457,7 +5529,7 @@
       </c>
       <c r="C6" s="96">
         <f>INDEX(Tracker!B:B,COUNTA(Tracker!B:B)+0)</f>
-        <v>3726.46</v>
+        <v>3753.25</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5466,7 +5538,7 @@
       </c>
       <c r="C7" s="97">
         <f>INDEX(Tracker!B:B,COUNTA(Tracker!B:B)+1)</f>
-        <v>3753.25</v>
+        <v>3771.97</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>104</v>
@@ -5483,14 +5555,14 @@
         <v>116</v>
       </c>
       <c r="C8" s="11">
-        <v>3777</v>
+        <v>3771.97</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F8" s="74">
         <f>MROUND(MAX(F10:F11),5)</f>
-        <v>3820</v>
+        <v>3815</v>
       </c>
       <c r="G8" s="75"/>
       <c r="H8" s="13" t="s">
@@ -5498,14 +5570,16 @@
       </c>
       <c r="I8" s="72">
         <f>MROUND(MIN(I10:I11),5)</f>
-        <v>3730</v>
+        <v>3725</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="11">
+        <v>3744.52</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="13"/>
       <c r="G9" s="76"/>
@@ -5524,7 +5598,7 @@
       </c>
       <c r="F10" s="74">
         <f>C8+C13</f>
-        <v>3819.2025533426227</v>
+        <v>3814.1163503128864</v>
       </c>
       <c r="G10" s="75"/>
       <c r="H10" s="13" t="s">
@@ -5532,7 +5606,7 @@
       </c>
       <c r="I10" s="72">
         <f>C8-C13</f>
-        <v>3734.7974466573773</v>
+        <v>3729.8236496871132</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5541,7 +5615,7 @@
       </c>
       <c r="F11" s="77">
         <f>C14+C13</f>
-        <v>3816.6718289562482</v>
+        <v>3811.3275328439263</v>
       </c>
       <c r="G11" s="78"/>
       <c r="H11" s="79" t="s">
@@ -5549,7 +5623,7 @@
       </c>
       <c r="I11" s="73">
         <f>C14-C13</f>
-        <v>3732.2667222710029</v>
+        <v>3727.034832218153</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -5564,7 +5638,7 @@
       </c>
       <c r="C13" s="3">
         <f>$C$8*C$10*SQRT((11/24)/252)</f>
-        <v>42.202553342622586</v>
+        <v>42.146350312886447</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5573,7 +5647,7 @@
       </c>
       <c r="C14" s="5">
         <f>C23*(1-F24)+C24*F24</f>
-        <v>3774.4692756136255</v>
+        <v>3769.1811825310397</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5589,7 +5663,7 @@
       </c>
       <c r="C17" s="3">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)*C$10*SQRT((24/24)/252)</f>
-        <v>62.440950506490587</v>
+        <v>61.801238076633012</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -5598,7 +5672,7 @@
       </c>
       <c r="C18" s="3">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)+C17</f>
-        <v>3845.7209505064907</v>
+        <v>3806.3212380766331</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5607,7 +5681,7 @@
       </c>
       <c r="C19" s="5">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)-C17</f>
-        <v>3720.8390494935097</v>
+        <v>3682.7187619233669</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -5616,7 +5690,7 @@
       </c>
       <c r="C22" s="85">
         <f>SLOPE(INDEX(Tracker!C:C,COUNTA(Tracker!C:C)-23):INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1),  INDEX(Tracker!A:A,COUNTA(Tracker!A:A)-23):INDEX(Tracker!A:A,COUNTA(Tracker!A:A)+1))</f>
-        <v>-10.710321167883212</v>
+        <v>-10.711179096482352</v>
       </c>
       <c r="E22" s="84" t="s">
         <v>112</v>
@@ -5634,7 +5708,7 @@
       </c>
       <c r="C23" s="85">
         <f>$C$8+C22*F22</f>
-        <v>3772.8229747445257</v>
+        <v>3767.7926401523719</v>
       </c>
       <c r="E23" s="84" t="s">
         <v>113</v>
@@ -5652,7 +5726,7 @@
       </c>
       <c r="C24" s="85">
         <f>_xlfn.FORECAST.LINEAR(G24+F23, C6:C8, G22:G24)</f>
-        <v>3784.5822666666663</v>
+        <v>3777.7107999999994</v>
       </c>
       <c r="E24" s="84" t="s">
         <v>111</v>
@@ -5686,14 +5760,14 @@
       </c>
       <c r="C27" s="85">
         <f>SUM(INDEX(Tracker!C:F,COUNTA(Tracker!C:C)-1,4):INDEX(Tracker!C:F,COUNTA(Tracker!C:C)+1,4))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" s="83" t="s">
         <v>97</v>
       </c>
       <c r="F27" s="83">
         <f>IF(C27&gt;=2, 0, 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -5702,7 +5776,7 @@
       </c>
       <c r="C28" s="85">
         <f>SUM(INDEX(Tracker!C:F,COUNTA(Tracker!C:C)+0,4):INDEX(Tracker!C:F,COUNTA(Tracker!C:C)+1,4))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="83" t="s">
         <v>110</v>
@@ -5737,7 +5811,7 @@
   <dimension ref="B1:N27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5800,14 +5874,14 @@
       </c>
       <c r="F3" s="47">
         <f>COUNTA(Tracker!J:J)-1</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="49" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="41">
         <f>C7/F3</f>
-        <v>-124.91666666666674</v>
+        <v>-37.769230769230838</v>
       </c>
       <c r="J3" s="17" t="s">
         <v>55</v>
@@ -5834,15 +5908,15 @@
       </c>
       <c r="F4" s="47">
         <f>COUNTIF(Tracker!I:I, "&gt;0")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G4" s="50">
         <f>F4/F3</f>
-        <v>0.5</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="H4" s="41">
         <f>(SUMIF(Tracker!G:G, "&gt;0", Tracker!G:G)-SUMIF(Tracker!G1,"&gt;0", Tracker!G1))/F4*100</f>
-        <v>1046.1666666666665</v>
+        <v>1040.7142857142856</v>
       </c>
       <c r="J4" s="17" t="s">
         <v>56</v>
@@ -5872,7 +5946,7 @@
       </c>
       <c r="G5" s="50">
         <f>F5/F3</f>
-        <v>0.5</v>
+        <v>0.46153846153846156</v>
       </c>
       <c r="H5" s="41">
         <f>IFERROR((SUMIF(Tracker!G:G, "&lt;0", Tracker!G:G)-SUMIF(Tracker!G1,"&lt;0", Tracker!G1))/F5*100, 0)</f>
@@ -5901,14 +5975,14 @@
       </c>
       <c r="C7" s="41">
         <f>INDEX(Tracker!J:J, COUNTA(Tracker!J:J)+18)</f>
-        <v>-1499.0000000000009</v>
+        <v>-491.00000000000091</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="45">
         <f>C7/C4</f>
-        <v>-6.3297954323284097E-2</v>
+        <v>-2.0733352616899618E-2</v>
       </c>
       <c r="G7" s="45"/>
       <c r="J7" s="17" t="s">
@@ -5927,14 +6001,14 @@
       </c>
       <c r="C8" s="41">
         <f>INDEX(Tracker!K:K, COUNTA(Tracker!K:K)+18)</f>
-        <v>16780</v>
+        <v>17788</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="45">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>-0.75437824630874639</v>
+        <v>-0.36226782595202978</v>
       </c>
       <c r="G8" s="45"/>
       <c r="J8" s="17" t="s">
@@ -5955,14 +6029,14 @@
       </c>
       <c r="C9" s="45">
         <f>C7/C8</f>
-        <v>-8.9332538736591235E-2</v>
+        <v>-2.7602878344951703E-2</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>46</v>
       </c>
       <c r="F9" s="45">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>-0.32711893039872053</v>
+        <v>-0.11921371825263494</v>
       </c>
       <c r="G9" s="45"/>
       <c r="J9" s="17" t="s">
@@ -6003,11 +6077,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C82D01-CC02-4066-B9D6-9DFF5A0A89C9}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6032,15 +6106,15 @@
       </c>
       <c r="B1" s="87">
         <f>Indicator!$C$8</f>
-        <v>3777</v>
+        <v>3771.97</v>
       </c>
       <c r="C1" s="87">
         <f>Indicator!$C$9</f>
-        <v>0</v>
+        <v>3744.52</v>
       </c>
       <c r="D1" s="87">
         <f>Indicator!$C$14</f>
-        <v>3774.4692756136255</v>
+        <v>3769.1811825310397</v>
       </c>
       <c r="E1" s="88">
         <f>Indicator!$C$10</f>
@@ -6048,7 +6122,7 @@
       </c>
       <c r="F1" s="71">
         <f>IF(ABS(D1-C1)&gt;=SQRT((7/24)/252)*E1*B1,       1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1" s="89">
         <f>SUMIF(Trades!A:A,Tracker!A1,Trades!H:H)</f>
@@ -6785,6 +6859,44 @@
       <c r="K31" s="68">
         <f t="shared" ref="K31" si="19">H31*100+K30</f>
         <v>16780</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="30">
+        <v>44840</v>
+      </c>
+      <c r="B32" s="21">
+        <v>3771.97</v>
+      </c>
+      <c r="C32" s="21">
+        <v>3744.52</v>
+      </c>
+      <c r="D32" s="21">
+        <v>3769.4580542802919</v>
+      </c>
+      <c r="E32" s="20">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="F32" s="71">
+        <v>0</v>
+      </c>
+      <c r="G32" s="13">
+        <v>10.08</v>
+      </c>
+      <c r="H32" s="31">
+        <v>10.08</v>
+      </c>
+      <c r="I32" s="16">
+        <f t="shared" ref="I32" si="20">G32/H32</f>
+        <v>1</v>
+      </c>
+      <c r="J32" s="35">
+        <f t="shared" ref="J32" si="21">J31+G32*100</f>
+        <v>-491.00000000000091</v>
+      </c>
+      <c r="K32" s="68">
+        <f t="shared" ref="K32" si="22">H32*100+K31</f>
+        <v>17788</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Market Open Oct 07 2022
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E788F3F-E874-4334-B101-864CF7734D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44480D51-3E8A-45E7-BD98-8B2361AB8F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10260" yWindow="2610" windowWidth="20505" windowHeight="14460" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="138">
   <si>
     <t>Updated</t>
   </si>
@@ -446,6 +446,12 @@
   </si>
   <si>
     <t>Oct06 3735/3710 Bull Put @-2.5</t>
+  </si>
+  <si>
+    <t>Oct07 3740/3765 Bear Call @ -4</t>
+  </si>
+  <si>
+    <t>Oct07 3645/3620 Bull Put @ -3.5</t>
   </si>
 </sst>
 </file>
@@ -5470,7 +5476,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5491,10 +5497,10 @@
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="15">
-        <v>44840</v>
+        <v>44841</v>
       </c>
       <c r="C2" s="67">
-        <v>1625</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -5555,14 +5561,14 @@
         <v>116</v>
       </c>
       <c r="C8" s="11">
-        <v>3771.97</v>
+        <v>3690</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F8" s="74">
         <f>MROUND(MAX(F10:F11),5)</f>
-        <v>3815</v>
+        <v>3735</v>
       </c>
       <c r="G8" s="75"/>
       <c r="H8" s="13" t="s">
@@ -5570,16 +5576,14 @@
       </c>
       <c r="I8" s="72">
         <f>MROUND(MIN(I10:I11),5)</f>
-        <v>3725</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="11">
-        <v>3744.52</v>
-      </c>
+      <c r="C9" s="11"/>
       <c r="E9" s="2"/>
       <c r="F9" s="13"/>
       <c r="G9" s="76"/>
@@ -5591,14 +5595,14 @@
         <v>1</v>
       </c>
       <c r="C10" s="12">
-        <v>0.26200000000000001</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>101</v>
       </c>
       <c r="F10" s="74">
         <f>C8+C13</f>
-        <v>3814.1163503128864</v>
+        <v>3732.8041346467503</v>
       </c>
       <c r="G10" s="75"/>
       <c r="H10" s="13" t="s">
@@ -5606,7 +5610,7 @@
       </c>
       <c r="I10" s="72">
         <f>C8-C13</f>
-        <v>3729.8236496871132</v>
+        <v>3647.1958653532497</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5615,7 +5619,7 @@
       </c>
       <c r="F11" s="77">
         <f>C14+C13</f>
-        <v>3811.3275328439263</v>
+        <v>3730.3213385111235</v>
       </c>
       <c r="G11" s="78"/>
       <c r="H11" s="79" t="s">
@@ -5623,7 +5627,7 @@
       </c>
       <c r="I11" s="73">
         <f>C14-C13</f>
-        <v>3727.034832218153</v>
+        <v>3644.7130692176229</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -5638,7 +5642,7 @@
       </c>
       <c r="C13" s="3">
         <f>$C$8*C$10*SQRT((11/24)/252)</f>
-        <v>42.146350312886447</v>
+        <v>42.804134646750462</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5647,7 +5651,7 @@
       </c>
       <c r="C14" s="5">
         <f>C23*(1-F24)+C24*F24</f>
-        <v>3769.1811825310397</v>
+        <v>3687.5172038643732</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5663,7 +5667,7 @@
       </c>
       <c r="C17" s="3">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)*C$10*SQRT((24/24)/252)</f>
-        <v>61.801238076633012</v>
+        <v>64.160063957420533</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -5672,7 +5676,7 @@
       </c>
       <c r="C18" s="3">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)+C17</f>
-        <v>3806.3212380766331</v>
+        <v>3808.6800639574203</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5681,7 +5685,7 @@
       </c>
       <c r="C19" s="5">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)-C17</f>
-        <v>3682.7187619233669</v>
+        <v>3680.3599360425796</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -5708,7 +5712,7 @@
       </c>
       <c r="C23" s="85">
         <f>$C$8+C22*F22</f>
-        <v>3767.7926401523719</v>
+        <v>3685.8226401523721</v>
       </c>
       <c r="E23" s="84" t="s">
         <v>113</v>
@@ -5726,7 +5730,7 @@
       </c>
       <c r="C24" s="85">
         <f>_xlfn.FORECAST.LINEAR(G24+F23, C6:C8, G22:G24)</f>
-        <v>3777.7107999999994</v>
+        <v>3697.9266666666663</v>
       </c>
       <c r="E24" s="84" t="s">
         <v>111</v>
@@ -5916,7 +5920,7 @@
       </c>
       <c r="H4" s="41">
         <f>(SUMIF(Tracker!G:G, "&gt;0", Tracker!G:G)-SUMIF(Tracker!G1,"&gt;0", Tracker!G1))/F4*100</f>
-        <v>1040.7142857142856</v>
+        <v>1040.7142857142858</v>
       </c>
       <c r="J4" s="17" t="s">
         <v>56</v>
@@ -6008,7 +6012,7 @@
       </c>
       <c r="F8" s="45">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>-0.36226782595202978</v>
+        <v>-0.34612948488050754</v>
       </c>
       <c r="G8" s="45"/>
       <c r="J8" s="17" t="s">
@@ -6036,7 +6040,7 @@
       </c>
       <c r="F9" s="45">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>-0.11921371825263494</v>
+        <v>-0.11298025041497672</v>
       </c>
       <c r="G9" s="45"/>
       <c r="J9" s="17" t="s">
@@ -6102,35 +6106,35 @@
     <row r="1" spans="1:12" s="94" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="86">
         <f>Indicator!$B$2</f>
-        <v>44840</v>
+        <v>44841</v>
       </c>
       <c r="B1" s="87">
         <f>Indicator!$C$8</f>
-        <v>3771.97</v>
+        <v>3690</v>
       </c>
       <c r="C1" s="87">
         <f>Indicator!$C$9</f>
-        <v>3744.52</v>
+        <v>0</v>
       </c>
       <c r="D1" s="87">
         <f>Indicator!$C$14</f>
-        <v>3769.1811825310397</v>
+        <v>3687.5172038643732</v>
       </c>
       <c r="E1" s="88">
         <f>Indicator!$C$10</f>
-        <v>0.26200000000000001</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="F1" s="71">
         <f>IF(ABS(D1-C1)&gt;=SQRT((7/24)/252)*E1*B1,       1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1" s="89">
         <f>SUMIF(Trades!A:A,Tracker!A1,Trades!H:H)</f>
-        <v>10.08</v>
+        <v>14.88</v>
       </c>
       <c r="H1" s="90">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A1,  Trades!C:C, "STO")</f>
-        <v>10.08</v>
+        <v>14.88</v>
       </c>
       <c r="I1" s="91"/>
       <c r="J1" s="92"/>
@@ -6911,11 +6915,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45:XFD46"/>
+      <selection pane="bottomLeft" activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7950,7 +7954,7 @@
         <v>4.87</v>
       </c>
       <c r="H31" s="28">
-        <f t="shared" ref="H31:H46" si="12">G31*F31</f>
+        <f t="shared" ref="H31:H48" si="12">G31*F31</f>
         <v>9.74</v>
       </c>
       <c r="I31" s="29">
@@ -8450,6 +8454,68 @@
       <c r="J46" s="42">
         <f t="shared" si="17"/>
         <v>-7.41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="25">
+        <v>44841</v>
+      </c>
+      <c r="B47" s="26">
+        <v>936</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="F47" s="18">
+        <v>2</v>
+      </c>
+      <c r="G47" s="27">
+        <v>3.97</v>
+      </c>
+      <c r="H47" s="28">
+        <f t="shared" si="12"/>
+        <v>7.94</v>
+      </c>
+      <c r="I47" s="29">
+        <v>3</v>
+      </c>
+      <c r="J47" s="42">
+        <f t="shared" ref="J47:J48" si="18">-I47*G47</f>
+        <v>-11.91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="25">
+        <v>44841</v>
+      </c>
+      <c r="B48" s="26">
+        <v>944</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="66" t="s">
+        <v>137</v>
+      </c>
+      <c r="F48" s="18">
+        <v>2</v>
+      </c>
+      <c r="G48" s="27">
+        <v>3.47</v>
+      </c>
+      <c r="H48" s="28">
+        <f t="shared" si="12"/>
+        <v>6.94</v>
+      </c>
+      <c r="I48" s="29">
+        <v>3</v>
+      </c>
+      <c r="J48" s="42">
+        <f t="shared" si="18"/>
+        <v>-10.41</v>
       </c>
     </row>
   </sheetData>
@@ -8461,11 +8527,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE4BC4F-EB6D-4F7C-A4AB-32C246F0D899}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomLeft" activeCell="J29" activeCellId="1" sqref="I24:J25 J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8560,7 +8626,7 @@
       </c>
       <c r="N2" s="42">
         <f>SUM(H:H)</f>
-        <v>10.44</v>
+        <v>17.88</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -9005,7 +9071,7 @@
         <v>-9.8800000000000008</v>
       </c>
       <c r="H16" s="28">
-        <f t="shared" ref="H16:H23" si="6">G16*F16</f>
+        <f t="shared" ref="H16:H25" si="6">G16*F16</f>
         <v>-9.8800000000000008</v>
       </c>
     </row>
@@ -9222,6 +9288,68 @@
       <c r="J23" s="42">
         <f t="shared" si="9"/>
         <v>-7.41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="25">
+        <v>44841</v>
+      </c>
+      <c r="B24" s="26">
+        <v>936</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="F24" s="18">
+        <v>1</v>
+      </c>
+      <c r="G24" s="27">
+        <v>3.97</v>
+      </c>
+      <c r="H24" s="28">
+        <f t="shared" si="6"/>
+        <v>3.97</v>
+      </c>
+      <c r="I24" s="29">
+        <v>3</v>
+      </c>
+      <c r="J24" s="42">
+        <f t="shared" ref="J24:J25" si="10">-I24*G24</f>
+        <v>-11.91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="25">
+        <v>44841</v>
+      </c>
+      <c r="B25" s="26">
+        <v>944</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="66" t="s">
+        <v>137</v>
+      </c>
+      <c r="F25" s="18">
+        <v>1</v>
+      </c>
+      <c r="G25" s="27">
+        <v>3.47</v>
+      </c>
+      <c r="H25" s="28">
+        <f t="shared" si="6"/>
+        <v>3.47</v>
+      </c>
+      <c r="I25" s="29">
+        <v>3</v>
+      </c>
+      <c r="J25" s="42">
+        <f t="shared" si="10"/>
+        <v>-10.41</v>
       </c>
     </row>
   </sheetData>
@@ -9232,11 +9360,11 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5E4B5F-C3CE-4821-8081-9385439A4F7E}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9319,7 +9447,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="28">
-        <f t="shared" ref="H2:H23" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H25" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="29">
@@ -9331,7 +9459,7 @@
       </c>
       <c r="N2" s="42">
         <f>SUM(H:H)</f>
-        <v>2.9899999999999958</v>
+        <v>10.429999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -9989,6 +10117,68 @@
       <c r="J23" s="42">
         <f t="shared" si="8"/>
         <v>-7.41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="25">
+        <v>44841</v>
+      </c>
+      <c r="B24" s="26">
+        <v>936</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="F24" s="18">
+        <v>1</v>
+      </c>
+      <c r="G24" s="27">
+        <v>3.97</v>
+      </c>
+      <c r="H24" s="28">
+        <f t="shared" si="0"/>
+        <v>3.97</v>
+      </c>
+      <c r="I24" s="29">
+        <v>3</v>
+      </c>
+      <c r="J24" s="42">
+        <f t="shared" ref="J24:J25" si="9">-I24*G24</f>
+        <v>-11.91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="25">
+        <v>44841</v>
+      </c>
+      <c r="B25" s="26">
+        <v>944</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="66" t="s">
+        <v>137</v>
+      </c>
+      <c r="F25" s="18">
+        <v>1</v>
+      </c>
+      <c r="G25" s="27">
+        <v>3.47</v>
+      </c>
+      <c r="H25" s="28">
+        <f t="shared" si="0"/>
+        <v>3.47</v>
+      </c>
+      <c r="I25" s="29">
+        <v>3</v>
+      </c>
+      <c r="J25" s="42">
+        <f t="shared" si="9"/>
+        <v>-10.41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Market Close Oct 07 2022
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44480D51-3E8A-45E7-BD98-8B2361AB8F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA26D18-6BA8-456A-9F08-DF2FF518E871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10260" yWindow="2610" windowWidth="20505" windowHeight="14460" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
+    <workbookView xWindow="32445" yWindow="4995" windowWidth="20505" windowHeight="14460" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="139">
   <si>
     <t>Updated</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>Oct07 3645/3620 Bull Put @ -3.5</t>
+  </si>
+  <si>
+    <t>Oct07 3645/3620 Bull Put @ -10.65</t>
   </si>
 </sst>
 </file>
@@ -989,6 +992,9 @@
                 <c:pt idx="12">
                   <c:v>44840</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>44841</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1036,6 +1042,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>-491.00000000000091</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1139.0000000000009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1144,6 +1153,9 @@
                       <c:pt idx="12">
                         <c:v>44840</c:v>
                       </c:pt>
+                      <c:pt idx="13">
+                        <c:v>44841</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1197,6 +1209,9 @@
                       </c:pt>
                       <c:pt idx="12">
                         <c:v>10.08</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-6.4799999999999986</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1293,6 +1308,9 @@
                       <c:pt idx="12">
                         <c:v>44840</c:v>
                       </c:pt>
+                      <c:pt idx="13">
+                        <c:v>44841</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1346,6 +1364,9 @@
                       </c:pt>
                       <c:pt idx="12">
                         <c:v>10.08</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>14.88</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1442,6 +1463,9 @@
                       <c:pt idx="12">
                         <c:v>44840</c:v>
                       </c:pt>
+                      <c:pt idx="13">
+                        <c:v>44841</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1495,6 +1519,9 @@
                       </c:pt>
                       <c:pt idx="12">
                         <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-0.43548387096774183</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1806,6 +1833,9 @@
                 <c:pt idx="12">
                   <c:v>44840</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>44841</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1854,6 +1884,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>10.08</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.88</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -1961,6 +1994,9 @@
                       <c:pt idx="12">
                         <c:v>44840</c:v>
                       </c:pt>
+                      <c:pt idx="13">
+                        <c:v>44841</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2014,6 +2050,9 @@
                       </c:pt>
                       <c:pt idx="12">
                         <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-0.43548387096774183</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2107,6 +2146,9 @@
                       <c:pt idx="12">
                         <c:v>44840</c:v>
                       </c:pt>
+                      <c:pt idx="13">
+                        <c:v>44841</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2160,6 +2202,9 @@
                       </c:pt>
                       <c:pt idx="12">
                         <c:v>-491.00000000000091</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-1139.0000000000009</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2239,6 +2284,9 @@
                 <c:pt idx="12">
                   <c:v>44840</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>44841</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -2287,6 +2335,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>10.08</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-6.4799999999999986</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2690,6 +2741,9 @@
                 <c:pt idx="12">
                   <c:v>44840</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>44841</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -2738,6 +2792,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.43548387096774183</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2831,6 +2888,9 @@
                       <c:pt idx="12">
                         <c:v>44840</c:v>
                       </c:pt>
+                      <c:pt idx="13">
+                        <c:v>44841</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2884,6 +2944,9 @@
                       </c:pt>
                       <c:pt idx="12">
                         <c:v>10.08</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>14.88</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2977,6 +3040,9 @@
                       <c:pt idx="12">
                         <c:v>44840</c:v>
                       </c:pt>
+                      <c:pt idx="13">
+                        <c:v>44841</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -3030,6 +3096,9 @@
                       </c:pt>
                       <c:pt idx="12">
                         <c:v>-491.00000000000091</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-1139.0000000000009</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3130,6 +3199,9 @@
                       <c:pt idx="12">
                         <c:v>44840</c:v>
                       </c:pt>
+                      <c:pt idx="13">
+                        <c:v>44841</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -3183,6 +3255,9 @@
                       </c:pt>
                       <c:pt idx="12">
                         <c:v>10.08</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-6.4799999999999986</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -5476,7 +5551,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5497,10 +5572,10 @@
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="15">
-        <v>44841</v>
+        <v>44844</v>
       </c>
       <c r="C2" s="67">
-        <v>1040</v>
+        <v>925</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -5535,7 +5610,7 @@
       </c>
       <c r="C6" s="96">
         <f>INDEX(Tracker!B:B,COUNTA(Tracker!B:B)+0)</f>
-        <v>3753.25</v>
+        <v>3771.97</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5544,7 +5619,7 @@
       </c>
       <c r="C7" s="97">
         <f>INDEX(Tracker!B:B,COUNTA(Tracker!B:B)+1)</f>
-        <v>3771.97</v>
+        <v>3706.74</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>104</v>
@@ -5561,14 +5636,14 @@
         <v>116</v>
       </c>
       <c r="C8" s="11">
-        <v>3690</v>
+        <v>3706.74</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F8" s="74">
         <f>MROUND(MAX(F10:F11),5)</f>
-        <v>3735</v>
+        <v>3750</v>
       </c>
       <c r="G8" s="75"/>
       <c r="H8" s="13" t="s">
@@ -5576,14 +5651,16 @@
       </c>
       <c r="I8" s="72">
         <f>MROUND(MIN(I10:I11),5)</f>
-        <v>3645</v>
+        <v>3655</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="11">
+        <v>3639.66</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="13"/>
       <c r="G9" s="76"/>
@@ -5602,7 +5679,7 @@
       </c>
       <c r="F10" s="74">
         <f>C8+C13</f>
-        <v>3732.8041346467503</v>
+        <v>3749.7383192575867</v>
       </c>
       <c r="G10" s="75"/>
       <c r="H10" s="13" t="s">
@@ -5610,7 +5687,7 @@
       </c>
       <c r="I10" s="72">
         <f>C8-C13</f>
-        <v>3647.1958653532497</v>
+        <v>3663.7416807424129</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5619,7 +5696,7 @@
       </c>
       <c r="F11" s="77">
         <f>C14+C13</f>
-        <v>3730.3213385111235</v>
+        <v>3743.1648744190929</v>
       </c>
       <c r="G11" s="78"/>
       <c r="H11" s="79" t="s">
@@ -5627,7 +5704,7 @@
       </c>
       <c r="I11" s="73">
         <f>C14-C13</f>
-        <v>3644.7130692176229</v>
+        <v>3657.1682359039191</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -5642,7 +5719,7 @@
       </c>
       <c r="C13" s="3">
         <f>$C$8*C$10*SQRT((11/24)/252)</f>
-        <v>42.804134646750462</v>
+        <v>42.998319257586935</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5651,7 +5728,7 @@
       </c>
       <c r="C14" s="5">
         <f>C23*(1-F24)+C24*F24</f>
-        <v>3687.5172038643732</v>
+        <v>3700.166555161506</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5667,7 +5744,7 @@
       </c>
       <c r="C17" s="3">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)*C$10*SQRT((24/24)/252)</f>
-        <v>64.160063957420533</v>
+        <v>62.363351880418641</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -5676,7 +5753,7 @@
       </c>
       <c r="C18" s="3">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)+C17</f>
-        <v>3808.6800639574203</v>
+        <v>3702.0233518804184</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5685,7 +5762,7 @@
       </c>
       <c r="C19" s="5">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)-C17</f>
-        <v>3680.3599360425796</v>
+        <v>3577.2966481195813</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -5694,7 +5771,7 @@
       </c>
       <c r="C22" s="85">
         <f>SLOPE(INDEX(Tracker!C:C,COUNTA(Tracker!C:C)-23):INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1),  INDEX(Tracker!A:A,COUNTA(Tracker!A:A)-23):INDEX(Tracker!A:A,COUNTA(Tracker!A:A)+1))</f>
-        <v>-10.711179096482352</v>
+        <v>-11.248966920572517</v>
       </c>
       <c r="E22" s="84" t="s">
         <v>112</v>
@@ -5712,7 +5789,7 @@
       </c>
       <c r="C23" s="85">
         <f>$C$8+C22*F22</f>
-        <v>3685.8226401523721</v>
+        <v>3702.3529029009765</v>
       </c>
       <c r="E23" s="84" t="s">
         <v>113</v>
@@ -5730,7 +5807,7 @@
       </c>
       <c r="C24" s="85">
         <f>_xlfn.FORECAST.LINEAR(G24+F23, C6:C8, G22:G24)</f>
-        <v>3697.9266666666663</v>
+        <v>3686.7361333333329</v>
       </c>
       <c r="E24" s="84" t="s">
         <v>111</v>
@@ -5780,7 +5857,7 @@
       </c>
       <c r="C28" s="85">
         <f>SUM(INDEX(Tracker!C:F,COUNTA(Tracker!C:C)+0,4):INDEX(Tracker!C:F,COUNTA(Tracker!C:C)+1,4))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="83" t="s">
         <v>110</v>
@@ -5800,7 +5877,7 @@
       </c>
       <c r="C30" s="83" t="b">
         <f>WEEKDAY(B2)=2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5878,14 +5955,14 @@
       </c>
       <c r="F3" s="47">
         <f>COUNTA(Tracker!J:J)-1</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="49" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="41">
         <f>C7/F3</f>
-        <v>-37.769230769230838</v>
+        <v>-81.357142857142918</v>
       </c>
       <c r="J3" s="17" t="s">
         <v>55</v>
@@ -5916,11 +5993,11 @@
       </c>
       <c r="G4" s="50">
         <f>F4/F3</f>
-        <v>0.53846153846153844</v>
+        <v>0.5</v>
       </c>
       <c r="H4" s="41">
         <f>(SUMIF(Tracker!G:G, "&gt;0", Tracker!G:G)-SUMIF(Tracker!G1,"&gt;0", Tracker!G1))/F4*100</f>
-        <v>1040.7142857142858</v>
+        <v>1040.7142857142856</v>
       </c>
       <c r="J4" s="17" t="s">
         <v>56</v>
@@ -5946,15 +6023,15 @@
       </c>
       <c r="F5" s="47">
         <f>COUNTIF(Tracker!I:I, "&lt;0")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G5" s="50">
         <f>F5/F3</f>
-        <v>0.46153846153846156</v>
+        <v>0.5</v>
       </c>
       <c r="H5" s="41">
         <f>IFERROR((SUMIF(Tracker!G:G, "&lt;0", Tracker!G:G)-SUMIF(Tracker!G1,"&lt;0", Tracker!G1))/F5*100, 0)</f>
-        <v>-1296</v>
+        <v>-1203.4285714285716</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>57</v>
@@ -5979,14 +6056,14 @@
       </c>
       <c r="C7" s="41">
         <f>INDEX(Tracker!J:J, COUNTA(Tracker!J:J)+18)</f>
-        <v>-491.00000000000091</v>
+        <v>-1139.0000000000009</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="45">
         <f>C7/C4</f>
-        <v>-2.0733352616899618E-2</v>
+        <v>-4.8096310856718213E-2</v>
       </c>
       <c r="G7" s="45"/>
       <c r="J7" s="17" t="s">
@@ -6005,14 +6082,14 @@
       </c>
       <c r="C8" s="41">
         <f>INDEX(Tracker!K:K, COUNTA(Tracker!K:K)+18)</f>
-        <v>17788</v>
+        <v>19276</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="45">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>-0.34612948488050754</v>
+        <v>-0.57545265885784314</v>
       </c>
       <c r="G8" s="45"/>
       <c r="J8" s="17" t="s">
@@ -6033,14 +6110,14 @@
       </c>
       <c r="C9" s="45">
         <f>C7/C8</f>
-        <v>-2.7602878344951703E-2</v>
+        <v>-5.9089022618800627E-2</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>46</v>
       </c>
       <c r="F9" s="45">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>-0.11298025041497672</v>
+        <v>-0.21475747532648704</v>
       </c>
       <c r="G9" s="45"/>
       <c r="J9" s="17" t="s">
@@ -6081,11 +6158,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C82D01-CC02-4066-B9D6-9DFF5A0A89C9}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
+      <selection pane="bottomLeft" activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6106,19 +6183,19 @@
     <row r="1" spans="1:12" s="94" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="86">
         <f>Indicator!$B$2</f>
-        <v>44841</v>
+        <v>44844</v>
       </c>
       <c r="B1" s="87">
         <f>Indicator!$C$8</f>
-        <v>3690</v>
+        <v>3706.74</v>
       </c>
       <c r="C1" s="87">
         <f>Indicator!$C$9</f>
-        <v>0</v>
+        <v>3639.66</v>
       </c>
       <c r="D1" s="87">
         <f>Indicator!$C$14</f>
-        <v>3687.5172038643732</v>
+        <v>3700.166555161506</v>
       </c>
       <c r="E1" s="88">
         <f>Indicator!$C$10</f>
@@ -6130,11 +6207,11 @@
       </c>
       <c r="G1" s="89">
         <f>SUMIF(Trades!A:A,Tracker!A1,Trades!H:H)</f>
-        <v>14.88</v>
+        <v>0</v>
       </c>
       <c r="H1" s="90">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A1,  Trades!C:C, "STO")</f>
-        <v>14.88</v>
+        <v>0</v>
       </c>
       <c r="I1" s="91"/>
       <c r="J1" s="92"/>
@@ -6903,6 +6980,44 @@
         <v>17788</v>
       </c>
     </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="30">
+        <v>44841</v>
+      </c>
+      <c r="B33" s="21">
+        <v>3706.74</v>
+      </c>
+      <c r="C33" s="21">
+        <v>3639.66</v>
+      </c>
+      <c r="D33" s="21">
+        <v>3704.194707864373</v>
+      </c>
+      <c r="E33" s="20">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="F33" s="71">
+        <v>1</v>
+      </c>
+      <c r="G33" s="13">
+        <v>-6.4799999999999986</v>
+      </c>
+      <c r="H33" s="31">
+        <v>14.88</v>
+      </c>
+      <c r="I33" s="16">
+        <f t="shared" ref="I33" si="23">G33/H33</f>
+        <v>-0.43548387096774183</v>
+      </c>
+      <c r="J33" s="35">
+        <f t="shared" ref="J33" si="24">J32+G33*100</f>
+        <v>-1139.0000000000009</v>
+      </c>
+      <c r="K33" s="68">
+        <f t="shared" ref="K33" si="25">H33*100+K32</f>
+        <v>19276</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:C19">
     <sortCondition ref="A6:A19"/>
@@ -6915,11 +7030,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L46" sqref="L46"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7954,7 +8069,7 @@
         <v>4.87</v>
       </c>
       <c r="H31" s="28">
-        <f t="shared" ref="H31:H48" si="12">G31*F31</f>
+        <f t="shared" ref="H31:H49" si="12">G31*F31</f>
         <v>9.74</v>
       </c>
       <c r="I31" s="29">
@@ -8516,6 +8631,36 @@
       <c r="J48" s="42">
         <f t="shared" si="18"/>
         <v>-10.41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="25">
+        <v>44841</v>
+      </c>
+      <c r="B49" s="26">
+        <v>1431</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" s="66" t="s">
+        <v>138</v>
+      </c>
+      <c r="F49" s="18">
+        <v>2</v>
+      </c>
+      <c r="G49" s="27">
+        <v>-10.68</v>
+      </c>
+      <c r="H49" s="28">
+        <f t="shared" si="12"/>
+        <v>-21.36</v>
+      </c>
+      <c r="M49">
+        <v>3636</v>
+      </c>
+      <c r="N49">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -8527,11 +8672,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE4BC4F-EB6D-4F7C-A4AB-32C246F0D899}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J29" activeCellId="1" sqref="I24:J25 J29"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8626,7 +8771,7 @@
       </c>
       <c r="N2" s="42">
         <f>SUM(H:H)</f>
-        <v>17.88</v>
+        <v>7.1999999999999993</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -9071,11 +9216,11 @@
         <v>-9.8800000000000008</v>
       </c>
       <c r="H16" s="28">
-        <f t="shared" ref="H16:H25" si="6">G16*F16</f>
+        <f t="shared" ref="H16:H26" si="6">G16*F16</f>
         <v>-9.8800000000000008</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="25">
         <v>44838</v>
       </c>
@@ -9106,7 +9251,7 @@
         <v>-7.11</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="25">
         <v>44838</v>
       </c>
@@ -9130,7 +9275,7 @@
         <v>-8.73</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="25">
         <v>44839</v>
       </c>
@@ -9164,7 +9309,7 @@
         <v>-8.91</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="25">
         <v>44839</v>
       </c>
@@ -9198,7 +9343,7 @@
         <v>-9.2099999999999991</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="25">
         <v>44839</v>
       </c>
@@ -9222,7 +9367,7 @@
         <v>-9.58</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="25">
         <v>44840</v>
       </c>
@@ -9256,7 +9401,7 @@
         <v>-7.7099999999999991</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="25">
         <v>44840</v>
       </c>
@@ -9290,7 +9435,7 @@
         <v>-7.41</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="25">
         <v>44841</v>
       </c>
@@ -9321,7 +9466,7 @@
         <v>-11.91</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="25">
         <v>44841</v>
       </c>
@@ -9350,6 +9495,36 @@
       <c r="J25" s="42">
         <f t="shared" si="10"/>
         <v>-10.41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="25">
+        <v>44841</v>
+      </c>
+      <c r="B26" s="26">
+        <v>1431</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="66" t="s">
+        <v>138</v>
+      </c>
+      <c r="F26" s="18">
+        <v>1</v>
+      </c>
+      <c r="G26" s="27">
+        <v>-10.68</v>
+      </c>
+      <c r="H26" s="28">
+        <f t="shared" si="6"/>
+        <v>-10.68</v>
+      </c>
+      <c r="M26">
+        <v>3636</v>
+      </c>
+      <c r="N26">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -9360,11 +9535,11 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5E4B5F-C3CE-4821-8081-9385439A4F7E}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9447,7 +9622,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="28">
-        <f t="shared" ref="H2:H25" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H26" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="29">
@@ -9459,7 +9634,7 @@
       </c>
       <c r="N2" s="42">
         <f>SUM(H:H)</f>
-        <v>10.429999999999996</v>
+        <v>-0.25000000000000355</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -9904,7 +10079,7 @@
         <v>-9.8800000000000008</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="25">
         <v>44838</v>
       </c>
@@ -9935,7 +10110,7 @@
         <v>-7.11</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="25">
         <v>44838</v>
       </c>
@@ -9959,7 +10134,7 @@
         <v>-8.73</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="25">
         <v>44839</v>
       </c>
@@ -9993,7 +10168,7 @@
         <v>-8.91</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="25">
         <v>44839</v>
       </c>
@@ -10027,7 +10202,7 @@
         <v>-9.2099999999999991</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="25">
         <v>44839</v>
       </c>
@@ -10051,7 +10226,7 @@
         <v>-9.58</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="25">
         <v>44840</v>
       </c>
@@ -10085,7 +10260,7 @@
         <v>-7.7099999999999991</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="25">
         <v>44840</v>
       </c>
@@ -10119,7 +10294,7 @@
         <v>-7.41</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="25">
         <v>44841</v>
       </c>
@@ -10150,7 +10325,7 @@
         <v>-11.91</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="25">
         <v>44841</v>
       </c>
@@ -10179,6 +10354,36 @@
       <c r="J25" s="42">
         <f t="shared" si="9"/>
         <v>-10.41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="25">
+        <v>44841</v>
+      </c>
+      <c r="B26" s="26">
+        <v>1431</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="66" t="s">
+        <v>138</v>
+      </c>
+      <c r="F26" s="18">
+        <v>1</v>
+      </c>
+      <c r="G26" s="27">
+        <v>-10.68</v>
+      </c>
+      <c r="H26" s="28">
+        <f t="shared" si="0"/>
+        <v>-10.68</v>
+      </c>
+      <c r="M26">
+        <v>3636</v>
+      </c>
+      <c r="N26">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Market Open Oct 10 2022
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA26D18-6BA8-456A-9F08-DF2FF518E871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62DDDAE-17F7-4DAE-A023-1CA58B9F3996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32445" yWindow="4995" windowWidth="20505" windowHeight="14460" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="142">
   <si>
     <t>Updated</t>
   </si>
@@ -455,6 +455,15 @@
   </si>
   <si>
     <t>Oct07 3645/3620 Bull Put @ -10.65</t>
+  </si>
+  <si>
+    <t>Oct10 3590/3565 Bull Put @ -2.2</t>
+  </si>
+  <si>
+    <t>Oct10 3600/3575 Bull Put @ -3</t>
+  </si>
+  <si>
+    <t>Oct10 3685/3710 Bear Call @ -2.9</t>
   </si>
 </sst>
 </file>
@@ -5551,7 +5560,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5575,7 +5584,7 @@
         <v>44844</v>
       </c>
       <c r="C2" s="67">
-        <v>925</v>
+        <v>951</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -5636,14 +5645,14 @@
         <v>116</v>
       </c>
       <c r="C8" s="11">
-        <v>3706.74</v>
+        <v>3640</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F8" s="74">
         <f>MROUND(MAX(F10:F11),5)</f>
-        <v>3750</v>
+        <v>3685</v>
       </c>
       <c r="G8" s="75"/>
       <c r="H8" s="13" t="s">
@@ -5651,16 +5660,14 @@
       </c>
       <c r="I8" s="72">
         <f>MROUND(MIN(I10:I11),5)</f>
-        <v>3655</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="11">
-        <v>3639.66</v>
-      </c>
+      <c r="C9" s="11"/>
       <c r="E9" s="2"/>
       <c r="F9" s="13"/>
       <c r="G9" s="76"/>
@@ -5672,14 +5679,14 @@
         <v>1</v>
       </c>
       <c r="C10" s="12">
-        <v>0.27200000000000002</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>101</v>
       </c>
       <c r="F10" s="74">
         <f>C8+C13</f>
-        <v>3749.7383192575867</v>
+        <v>3684.7079053412258</v>
       </c>
       <c r="G10" s="75"/>
       <c r="H10" s="13" t="s">
@@ -5687,7 +5694,7 @@
       </c>
       <c r="I10" s="72">
         <f>C8-C13</f>
-        <v>3663.7416807424129</v>
+        <v>3595.2920946587742</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5696,7 +5703,7 @@
       </c>
       <c r="F11" s="77">
         <f>C14+C13</f>
-        <v>3743.1648744190929</v>
+        <v>3678.383623169399</v>
       </c>
       <c r="G11" s="78"/>
       <c r="H11" s="79" t="s">
@@ -5704,7 +5711,7 @@
       </c>
       <c r="I11" s="73">
         <f>C14-C13</f>
-        <v>3657.1682359039191</v>
+        <v>3588.9678124869474</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -5719,7 +5726,7 @@
       </c>
       <c r="C13" s="3">
         <f>$C$8*C$10*SQRT((11/24)/252)</f>
-        <v>42.998319257586935</v>
+        <v>44.707905341225725</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5728,7 +5735,7 @@
       </c>
       <c r="C14" s="5">
         <f>C23*(1-F24)+C24*F24</f>
-        <v>3700.166555161506</v>
+        <v>3633.6757178281732</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5744,7 +5751,7 @@
       </c>
       <c r="C17" s="3">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)*C$10*SQRT((24/24)/252)</f>
-        <v>62.363351880418641</v>
+        <v>66.03178434397266</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -5753,7 +5760,7 @@
       </c>
       <c r="C18" s="3">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)+C17</f>
-        <v>3702.0233518804184</v>
+        <v>3705.6917843439724</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5762,7 +5769,7 @@
       </c>
       <c r="C19" s="5">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)-C17</f>
-        <v>3577.2966481195813</v>
+        <v>3573.6282156560274</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -5789,7 +5796,7 @@
       </c>
       <c r="C23" s="85">
         <f>$C$8+C22*F22</f>
-        <v>3702.3529029009765</v>
+        <v>3635.6129029009767</v>
       </c>
       <c r="E23" s="84" t="s">
         <v>113</v>
@@ -5807,7 +5814,7 @@
       </c>
       <c r="C24" s="85">
         <f>_xlfn.FORECAST.LINEAR(G24+F23, C6:C8, G22:G24)</f>
-        <v>3686.7361333333329</v>
+        <v>3621.7758666666664</v>
       </c>
       <c r="E24" s="84" t="s">
         <v>111</v>
@@ -6167,7 +6174,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="30" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="8.140625" style="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.140625" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.85546875" style="71" bestFit="1" customWidth="1"/>
@@ -6187,19 +6194,19 @@
       </c>
       <c r="B1" s="87">
         <f>Indicator!$C$8</f>
-        <v>3706.74</v>
+        <v>3640</v>
       </c>
       <c r="C1" s="87">
         <f>Indicator!$C$9</f>
-        <v>3639.66</v>
+        <v>0</v>
       </c>
       <c r="D1" s="87">
         <f>Indicator!$C$14</f>
-        <v>3700.166555161506</v>
+        <v>3633.6757178281732</v>
       </c>
       <c r="E1" s="88">
         <f>Indicator!$C$10</f>
-        <v>0.27200000000000002</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="F1" s="71">
         <f>IF(ABS(D1-C1)&gt;=SQRT((7/24)/252)*E1*B1,       1, 0)</f>
@@ -6207,11 +6214,11 @@
       </c>
       <c r="G1" s="89">
         <f>SUMIF(Trades!A:A,Tracker!A1,Trades!H:H)</f>
-        <v>0</v>
+        <v>10.95</v>
       </c>
       <c r="H1" s="90">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A1,  Trades!C:C, "STO")</f>
-        <v>0</v>
+        <v>10.95</v>
       </c>
       <c r="I1" s="91"/>
       <c r="J1" s="92"/>
@@ -7030,16 +7037,16 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="26" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.28515625" style="13" customWidth="1"/>
@@ -8069,7 +8076,7 @@
         <v>4.87</v>
       </c>
       <c r="H31" s="28">
-        <f t="shared" ref="H31:H49" si="12">G31*F31</f>
+        <f t="shared" ref="H31:H52" si="12">G31*F31</f>
         <v>9.74</v>
       </c>
       <c r="I31" s="29">
@@ -8661,6 +8668,108 @@
       </c>
       <c r="N49">
         <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="25">
+        <v>44844</v>
+      </c>
+      <c r="B50" s="26">
+        <v>941</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="66" t="s">
+        <v>141</v>
+      </c>
+      <c r="E50" s="64">
+        <v>0.15</v>
+      </c>
+      <c r="F50" s="18">
+        <v>2</v>
+      </c>
+      <c r="G50" s="27">
+        <v>2.88</v>
+      </c>
+      <c r="H50" s="28">
+        <f t="shared" si="12"/>
+        <v>5.76</v>
+      </c>
+      <c r="I50" s="29">
+        <v>3</v>
+      </c>
+      <c r="J50" s="42">
+        <f t="shared" ref="J50:J52" si="19">-I50*G50</f>
+        <v>-8.64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="25">
+        <v>44844</v>
+      </c>
+      <c r="B51" s="26">
+        <v>942</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="66" t="s">
+        <v>140</v>
+      </c>
+      <c r="E51" s="64">
+        <v>-0.15</v>
+      </c>
+      <c r="F51" s="18">
+        <v>1</v>
+      </c>
+      <c r="G51" s="27">
+        <v>3.02</v>
+      </c>
+      <c r="H51" s="28">
+        <f t="shared" si="12"/>
+        <v>3.02</v>
+      </c>
+      <c r="I51" s="29">
+        <v>3</v>
+      </c>
+      <c r="J51" s="42">
+        <f t="shared" si="19"/>
+        <v>-9.06</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="25">
+        <v>44844</v>
+      </c>
+      <c r="B52" s="26">
+        <v>943</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="66" t="s">
+        <v>139</v>
+      </c>
+      <c r="E52" s="64">
+        <v>-0.11</v>
+      </c>
+      <c r="F52" s="18">
+        <v>1</v>
+      </c>
+      <c r="G52" s="27">
+        <v>2.17</v>
+      </c>
+      <c r="H52" s="28">
+        <f t="shared" si="12"/>
+        <v>2.17</v>
+      </c>
+      <c r="I52" s="29">
+        <v>3</v>
+      </c>
+      <c r="J52" s="42">
+        <f t="shared" si="19"/>
+        <v>-6.51</v>
       </c>
     </row>
   </sheetData>
@@ -8672,16 +8781,16 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE4BC4F-EB6D-4F7C-A4AB-32C246F0D899}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="A29:J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="26" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.42578125" style="13" bestFit="1" customWidth="1"/>
@@ -8771,7 +8880,7 @@
       </c>
       <c r="N2" s="42">
         <f>SUM(H:H)</f>
-        <v>7.1999999999999993</v>
+        <v>13.099999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -9216,7 +9325,7 @@
         <v>-9.8800000000000008</v>
       </c>
       <c r="H16" s="28">
-        <f t="shared" ref="H16:H26" si="6">G16*F16</f>
+        <f t="shared" ref="H16:H29" si="6">G16*F16</f>
         <v>-9.8800000000000008</v>
       </c>
     </row>
@@ -9526,6 +9635,77 @@
       <c r="N26">
         <v>9</v>
       </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="25">
+        <v>44844</v>
+      </c>
+      <c r="B27" s="26">
+        <v>941</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="66" t="s">
+        <v>141</v>
+      </c>
+      <c r="E27" s="64">
+        <v>0.15</v>
+      </c>
+      <c r="F27" s="18">
+        <v>1</v>
+      </c>
+      <c r="G27" s="27">
+        <v>2.88</v>
+      </c>
+      <c r="H27" s="28">
+        <f t="shared" si="6"/>
+        <v>2.88</v>
+      </c>
+      <c r="I27" s="29">
+        <v>3</v>
+      </c>
+      <c r="J27" s="42">
+        <f t="shared" ref="J27:J29" si="11">-I27*G27</f>
+        <v>-8.64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="25">
+        <v>44844</v>
+      </c>
+      <c r="B28" s="26">
+        <v>942</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="66" t="s">
+        <v>140</v>
+      </c>
+      <c r="E28" s="64">
+        <v>-0.15</v>
+      </c>
+      <c r="F28" s="18">
+        <v>1</v>
+      </c>
+      <c r="G28" s="27">
+        <v>3.02</v>
+      </c>
+      <c r="H28" s="28">
+        <f t="shared" si="6"/>
+        <v>3.02</v>
+      </c>
+      <c r="I28" s="29">
+        <v>3</v>
+      </c>
+      <c r="J28" s="42">
+        <f t="shared" si="11"/>
+        <v>-9.06</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D29" s="66"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9535,16 +9715,16 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5E4B5F-C3CE-4821-8081-9385439A4F7E}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="26" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.42578125" style="13" bestFit="1" customWidth="1"/>
@@ -9622,7 +9802,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="28">
-        <f t="shared" ref="H2:H26" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H28" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="29">
@@ -9634,7 +9814,7 @@
       </c>
       <c r="N2" s="42">
         <f>SUM(H:H)</f>
-        <v>-0.25000000000000355</v>
+        <v>4.7999999999999963</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -10384,6 +10564,74 @@
       </c>
       <c r="N26">
         <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="25">
+        <v>44844</v>
+      </c>
+      <c r="B27" s="26">
+        <v>941</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="66" t="s">
+        <v>141</v>
+      </c>
+      <c r="E27" s="64">
+        <v>0.15</v>
+      </c>
+      <c r="F27" s="18">
+        <v>1</v>
+      </c>
+      <c r="G27" s="27">
+        <v>2.88</v>
+      </c>
+      <c r="H27" s="28">
+        <f t="shared" si="0"/>
+        <v>2.88</v>
+      </c>
+      <c r="I27" s="29">
+        <v>3</v>
+      </c>
+      <c r="J27" s="42">
+        <f t="shared" ref="J27:J28" si="10">-I27*G27</f>
+        <v>-8.64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="25">
+        <v>44844</v>
+      </c>
+      <c r="B28" s="26">
+        <v>943</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="66" t="s">
+        <v>139</v>
+      </c>
+      <c r="E28" s="64">
+        <v>-0.11</v>
+      </c>
+      <c r="F28" s="18">
+        <v>1</v>
+      </c>
+      <c r="G28" s="27">
+        <v>2.17</v>
+      </c>
+      <c r="H28" s="28">
+        <f t="shared" si="0"/>
+        <v>2.17</v>
+      </c>
+      <c r="I28" s="29">
+        <v>3</v>
+      </c>
+      <c r="J28" s="42">
+        <f t="shared" si="10"/>
+        <v>-6.51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Market Close Oct 10 2022
</commit_message>
<xml_diff>
--- a/0DTE Experiment.xlsx
+++ b/0DTE Experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62DDDAE-17F7-4DAE-A023-1CA58B9F3996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5D88AC-1D57-405F-BE5E-4F5BB99ACA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32445" yWindow="4995" windowWidth="20505" windowHeight="14460" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
+    <workbookView xWindow="29595" yWindow="4890" windowWidth="20505" windowHeight="14460" xr2:uid="{70494AAA-D256-49B2-A3DF-05E6F986F6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="144">
   <si>
     <t>Updated</t>
   </si>
@@ -464,6 +464,12 @@
   </si>
   <si>
     <t>Oct10 3685/3710 Bear Call @ -2.9</t>
+  </si>
+  <si>
+    <t>Oct10 3600/3575 Bull Put @ -9.15</t>
+  </si>
+  <si>
+    <t>Oct10 3590/3565 Bull Put @ -6.8</t>
   </si>
 </sst>
 </file>
@@ -1004,6 +1010,9 @@
                 <c:pt idx="13">
                   <c:v>44841</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>44844</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1054,6 +1063,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>-1139.0000000000009</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1645.0000000000009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1165,6 +1177,9 @@
                       <c:pt idx="13">
                         <c:v>44841</c:v>
                       </c:pt>
+                      <c:pt idx="14">
+                        <c:v>44844</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1221,6 +1236,9 @@
                       </c:pt>
                       <c:pt idx="13">
                         <c:v>-6.4799999999999986</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>-5.0600000000000005</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1320,6 +1338,9 @@
                       <c:pt idx="13">
                         <c:v>44841</c:v>
                       </c:pt>
+                      <c:pt idx="14">
+                        <c:v>44844</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1376,6 +1397,9 @@
                       </c:pt>
                       <c:pt idx="13">
                         <c:v>14.88</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>10.95</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1475,6 +1499,9 @@
                       <c:pt idx="13">
                         <c:v>44841</c:v>
                       </c:pt>
+                      <c:pt idx="14">
+                        <c:v>44844</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -1531,6 +1558,9 @@
                       </c:pt>
                       <c:pt idx="13">
                         <c:v>-0.43548387096774183</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>-0.46210045662100463</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1845,6 +1875,9 @@
                 <c:pt idx="13">
                   <c:v>44841</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>44844</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -1896,6 +1929,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>14.88</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.95</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2006,6 +2042,9 @@
                       <c:pt idx="13">
                         <c:v>44841</c:v>
                       </c:pt>
+                      <c:pt idx="14">
+                        <c:v>44844</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2062,6 +2101,9 @@
                       </c:pt>
                       <c:pt idx="13">
                         <c:v>-0.43548387096774183</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>-0.46210045662100463</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2158,6 +2200,9 @@
                       <c:pt idx="13">
                         <c:v>44841</c:v>
                       </c:pt>
+                      <c:pt idx="14">
+                        <c:v>44844</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2214,6 +2259,9 @@
                       </c:pt>
                       <c:pt idx="13">
                         <c:v>-1139.0000000000009</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>-1645.0000000000009</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2296,6 +2344,9 @@
                 <c:pt idx="13">
                   <c:v>44841</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>44844</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -2347,6 +2398,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>-6.4799999999999986</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-5.0600000000000005</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2753,6 +2807,9 @@
                 <c:pt idx="13">
                   <c:v>44841</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>44844</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -2804,6 +2861,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>-0.43548387096774183</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.46210045662100463</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2900,6 +2960,9 @@
                       <c:pt idx="13">
                         <c:v>44841</c:v>
                       </c:pt>
+                      <c:pt idx="14">
+                        <c:v>44844</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -2956,6 +3019,9 @@
                       </c:pt>
                       <c:pt idx="13">
                         <c:v>14.88</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>10.95</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3052,6 +3118,9 @@
                       <c:pt idx="13">
                         <c:v>44841</c:v>
                       </c:pt>
+                      <c:pt idx="14">
+                        <c:v>44844</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -3108,6 +3177,9 @@
                       </c:pt>
                       <c:pt idx="13">
                         <c:v>-1139.0000000000009</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>-1645.0000000000009</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3211,6 +3283,9 @@
                       <c:pt idx="13">
                         <c:v>44841</c:v>
                       </c:pt>
+                      <c:pt idx="14">
+                        <c:v>44844</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -3267,6 +3342,9 @@
                       </c:pt>
                       <c:pt idx="13">
                         <c:v>-6.4799999999999986</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>-5.0600000000000005</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -5560,7 +5638,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5619,7 +5697,7 @@
       </c>
       <c r="C6" s="96">
         <f>INDEX(Tracker!B:B,COUNTA(Tracker!B:B)+0)</f>
-        <v>3771.97</v>
+        <v>3706.74</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5628,7 +5706,7 @@
       </c>
       <c r="C7" s="97">
         <f>INDEX(Tracker!B:B,COUNTA(Tracker!B:B)+1)</f>
-        <v>3706.74</v>
+        <v>3647.51</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>104</v>
@@ -5645,14 +5723,14 @@
         <v>116</v>
       </c>
       <c r="C8" s="11">
-        <v>3640</v>
+        <v>3647.51</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F8" s="74">
         <f>MROUND(MAX(F10:F11),5)</f>
-        <v>3685</v>
+        <v>3690</v>
       </c>
       <c r="G8" s="75"/>
       <c r="H8" s="13" t="s">
@@ -5660,14 +5738,16 @@
       </c>
       <c r="I8" s="72">
         <f>MROUND(MIN(I10:I11),5)</f>
-        <v>3590</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="11">
+        <v>3612.39</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="13"/>
       <c r="G9" s="76"/>
@@ -5686,7 +5766,7 @@
       </c>
       <c r="F10" s="74">
         <f>C8+C13</f>
-        <v>3684.7079053412258</v>
+        <v>3692.310146101971</v>
       </c>
       <c r="G10" s="75"/>
       <c r="H10" s="13" t="s">
@@ -5694,7 +5774,7 @@
       </c>
       <c r="I10" s="72">
         <f>C8-C13</f>
-        <v>3595.2920946587742</v>
+        <v>3602.7098538980295</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5703,7 +5783,7 @@
       </c>
       <c r="F11" s="77">
         <f>C14+C13</f>
-        <v>3678.383623169399</v>
+        <v>3685.7155756554926</v>
       </c>
       <c r="G11" s="78"/>
       <c r="H11" s="79" t="s">
@@ -5711,7 +5791,7 @@
       </c>
       <c r="I11" s="73">
         <f>C14-C13</f>
-        <v>3588.9678124869474</v>
+        <v>3596.115283451551</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -5726,7 +5806,7 @@
       </c>
       <c r="C13" s="3">
         <f>$C$8*C$10*SQRT((11/24)/252)</f>
-        <v>44.707905341225725</v>
+        <v>44.800146101970952</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5735,7 +5815,7 @@
       </c>
       <c r="C14" s="5">
         <f>C23*(1-F24)+C24*F24</f>
-        <v>3633.6757178281732</v>
+        <v>3640.9154295535218</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5751,7 +5831,7 @@
       </c>
       <c r="C17" s="3">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)*C$10*SQRT((24/24)/252)</f>
-        <v>66.03178434397266</v>
+        <v>65.537043967382502</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -5760,7 +5840,7 @@
       </c>
       <c r="C18" s="3">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)+C17</f>
-        <v>3705.6917843439724</v>
+        <v>3677.9270439673824</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5769,7 +5849,7 @@
       </c>
       <c r="C19" s="5">
         <f>INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1)-C17</f>
-        <v>3573.6282156560274</v>
+        <v>3546.8529560326174</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -5778,7 +5858,7 @@
       </c>
       <c r="C22" s="85">
         <f>SLOPE(INDEX(Tracker!C:C,COUNTA(Tracker!C:C)-23):INDEX(Tracker!C:C,COUNTA(Tracker!C:C)+1),  INDEX(Tracker!A:A,COUNTA(Tracker!A:A)-23):INDEX(Tracker!A:A,COUNTA(Tracker!A:A)+1))</f>
-        <v>-11.248966920572517</v>
+        <v>-12.079991392801247</v>
       </c>
       <c r="E22" s="84" t="s">
         <v>112</v>
@@ -5796,7 +5876,7 @@
       </c>
       <c r="C23" s="85">
         <f>$C$8+C22*F22</f>
-        <v>3635.6129029009767</v>
+        <v>3642.7988033568076</v>
       </c>
       <c r="E23" s="84" t="s">
         <v>113</v>
@@ -5814,7 +5894,7 @@
       </c>
       <c r="C24" s="85">
         <f>_xlfn.FORECAST.LINEAR(G24+F23, C6:C8, G22:G24)</f>
-        <v>3621.7758666666664</v>
+        <v>3629.3461333333339</v>
       </c>
       <c r="E24" s="84" t="s">
         <v>111</v>
@@ -5832,7 +5912,7 @@
       </c>
       <c r="C26" s="85">
         <f>SUM(INDEX(Tracker!C:F,COUNTA(Tracker!C:C)-2,4):INDEX(Tracker!C:F,COUNTA(Tracker!C:C)+1,4))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26" s="83" t="s">
         <v>98</v>
@@ -5962,14 +6042,14 @@
       </c>
       <c r="F3" s="47">
         <f>COUNTA(Tracker!J:J)-1</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="49" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="41">
         <f>C7/F3</f>
-        <v>-81.357142857142918</v>
+        <v>-109.66666666666673</v>
       </c>
       <c r="J3" s="17" t="s">
         <v>55</v>
@@ -6000,7 +6080,7 @@
       </c>
       <c r="G4" s="50">
         <f>F4/F3</f>
-        <v>0.5</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="H4" s="41">
         <f>(SUMIF(Tracker!G:G, "&gt;0", Tracker!G:G)-SUMIF(Tracker!G1,"&gt;0", Tracker!G1))/F4*100</f>
@@ -6030,15 +6110,15 @@
       </c>
       <c r="F5" s="47">
         <f>COUNTIF(Tracker!I:I, "&lt;0")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G5" s="50">
         <f>F5/F3</f>
-        <v>0.5</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="H5" s="41">
         <f>IFERROR((SUMIF(Tracker!G:G, "&lt;0", Tracker!G:G)-SUMIF(Tracker!G1,"&lt;0", Tracker!G1))/F5*100, 0)</f>
-        <v>-1203.4285714285716</v>
+        <v>-1116.2500000000002</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>57</v>
@@ -6063,14 +6143,14 @@
       </c>
       <c r="C7" s="41">
         <f>INDEX(Tracker!J:J, COUNTA(Tracker!J:J)+18)</f>
-        <v>-1139.0000000000009</v>
+        <v>-1645.0000000000009</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="45">
         <f>C7/C4</f>
-        <v>-4.8096310856718213E-2</v>
+        <v>-6.9463065284724707E-2</v>
       </c>
       <c r="G7" s="45"/>
       <c r="J7" s="17" t="s">
@@ -6089,14 +6169,14 @@
       </c>
       <c r="C8" s="41">
         <f>INDEX(Tracker!K:K, COUNTA(Tracker!K:K)+18)</f>
-        <v>19276</v>
+        <v>20371</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="45">
         <f>(1+F7)^(365/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>-0.57545265885784314</v>
+        <v>-0.71387193078190858</v>
       </c>
       <c r="G8" s="45"/>
       <c r="J8" s="17" t="s">
@@ -6117,14 +6197,14 @@
       </c>
       <c r="C9" s="45">
         <f>C7/C8</f>
-        <v>-5.9089022618800627E-2</v>
+        <v>-8.0752049482106958E-2</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>46</v>
       </c>
       <c r="F9" s="45">
         <f>(1+F7)^((44927-C3)/(Indicator!B2-Dashboard!C3+1))-1</f>
-        <v>-0.21475747532648704</v>
+        <v>-0.2975008070594819</v>
       </c>
       <c r="G9" s="45"/>
       <c r="J9" s="17" t="s">
@@ -6165,11 +6245,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C82D01-CC02-4066-B9D6-9DFF5A0A89C9}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L33" sqref="L33"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6194,15 +6274,15 @@
       </c>
       <c r="B1" s="87">
         <f>Indicator!$C$8</f>
-        <v>3640</v>
+        <v>3647.51</v>
       </c>
       <c r="C1" s="87">
         <f>Indicator!$C$9</f>
-        <v>0</v>
+        <v>3612.39</v>
       </c>
       <c r="D1" s="87">
         <f>Indicator!$C$14</f>
-        <v>3633.6757178281732</v>
+        <v>3640.9154295535218</v>
       </c>
       <c r="E1" s="88">
         <f>Indicator!$C$10</f>
@@ -6210,11 +6290,11 @@
       </c>
       <c r="F1" s="71">
         <f>IF(ABS(D1-C1)&gt;=SQRT((7/24)/252)*E1*B1,       1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1" s="89">
         <f>SUMIF(Trades!A:A,Tracker!A1,Trades!H:H)</f>
-        <v>10.95</v>
+        <v>-5.0600000000000005</v>
       </c>
       <c r="H1" s="90">
         <f>SUMIFS(Trades!H:H,  Trades!A:A,Tracker!A1,  Trades!C:C, "STO")</f>
@@ -7025,6 +7105,44 @@
         <v>19276</v>
       </c>
     </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="30">
+        <v>44844</v>
+      </c>
+      <c r="B34" s="21">
+        <v>3647.51</v>
+      </c>
+      <c r="C34" s="21">
+        <v>3612.39</v>
+      </c>
+      <c r="D34" s="21">
+        <v>3632.2222075403761</v>
+      </c>
+      <c r="E34" s="20">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="F34" s="71">
+        <v>0</v>
+      </c>
+      <c r="G34" s="13">
+        <v>-5.0600000000000005</v>
+      </c>
+      <c r="H34" s="31">
+        <v>10.95</v>
+      </c>
+      <c r="I34" s="16">
+        <f t="shared" ref="I34" si="26">G34/H34</f>
+        <v>-0.46210045662100463</v>
+      </c>
+      <c r="J34" s="35">
+        <f t="shared" ref="J34" si="27">J33+G34*100</f>
+        <v>-1645.0000000000009</v>
+      </c>
+      <c r="K34" s="68">
+        <f t="shared" ref="K34" si="28">H34*100+K33</f>
+        <v>20371</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:C19">
     <sortCondition ref="A6:A19"/>
@@ -7037,11 +7155,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64AAA6-779C-4846-96DE-7528F04CBAF7}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8772,6 +8890,66 @@
         <v>-6.51</v>
       </c>
     </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="25">
+        <v>44844</v>
+      </c>
+      <c r="B53" s="26">
+        <v>1251</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53" s="66" t="s">
+        <v>142</v>
+      </c>
+      <c r="F53" s="18">
+        <v>1</v>
+      </c>
+      <c r="G53" s="27">
+        <v>-9.18</v>
+      </c>
+      <c r="H53" s="28">
+        <f t="shared" ref="H53:H54" si="20">G53*F53</f>
+        <v>-9.18</v>
+      </c>
+      <c r="M53">
+        <v>3598</v>
+      </c>
+      <c r="N53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="25">
+        <v>44844</v>
+      </c>
+      <c r="B54" s="26">
+        <v>1253</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D54" s="66" t="s">
+        <v>143</v>
+      </c>
+      <c r="F54" s="18">
+        <v>1</v>
+      </c>
+      <c r="G54" s="27">
+        <v>-6.83</v>
+      </c>
+      <c r="H54" s="28">
+        <f t="shared" si="20"/>
+        <v>-6.83</v>
+      </c>
+      <c r="M54">
+        <v>3956</v>
+      </c>
+      <c r="N54">
+        <v>-6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8785,7 +8963,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J29" sqref="A29:J30"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8880,7 +9058,7 @@
       </c>
       <c r="N2" s="42">
         <f>SUM(H:H)</f>
-        <v>13.099999999999998</v>
+        <v>3.9199999999999982</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -9666,7 +9844,7 @@
         <v>3</v>
       </c>
       <c r="J27" s="42">
-        <f t="shared" ref="J27:J29" si="11">-I27*G27</f>
+        <f t="shared" ref="J27:J28" si="11">-I27*G27</f>
         <v>-8.64</v>
       </c>
     </row>
@@ -9705,7 +9883,28 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D29" s="66"/>
+      <c r="A29" s="25">
+        <v>44844</v>
+      </c>
+      <c r="B29" s="26">
+        <v>1251</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="66" t="s">
+        <v>142</v>
+      </c>
+      <c r="F29" s="18">
+        <v>1</v>
+      </c>
+      <c r="G29" s="27">
+        <v>-9.18</v>
+      </c>
+      <c r="H29" s="28">
+        <f t="shared" si="6"/>
+        <v>-9.18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9715,11 +9914,11 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5E4B5F-C3CE-4821-8081-9385439A4F7E}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9802,7 +10001,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="H2" s="28">
-        <f t="shared" ref="H2:H28" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H29" si="0">G2*F2</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="I2" s="29">
@@ -9814,7 +10013,7 @@
       </c>
       <c r="N2" s="42">
         <f>SUM(H:H)</f>
-        <v>4.7999999999999963</v>
+        <v>-2.0300000000000038</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -10632,6 +10831,30 @@
       <c r="J28" s="42">
         <f t="shared" si="10"/>
         <v>-6.51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="25">
+        <v>44844</v>
+      </c>
+      <c r="B29" s="26">
+        <v>1253</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="66" t="s">
+        <v>143</v>
+      </c>
+      <c r="F29" s="18">
+        <v>1</v>
+      </c>
+      <c r="G29" s="27">
+        <v>-6.83</v>
+      </c>
+      <c r="H29" s="28">
+        <f t="shared" si="0"/>
+        <v>-6.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>